<commit_message>
Added some more components to the BOM, Still need to figure out HIROSE Connectors, would like to use 2 pin instead of 3 pin. Took forever to figure out the antenna connector that was used
</commit_message>
<xml_diff>
--- a/RADSAT-SK Timer/RADSAT-SK Timer.xlsx
+++ b/RADSAT-SK Timer/RADSAT-SK Timer.xlsx
@@ -5,22 +5,33 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\riley\USST\RADSAT-SK\power-and-electrical\RADSAT-SK Timer\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\USST\power-and-electrical\RADSAT-SK Timer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73799B21-8251-49BC-A8C9-89745B7448F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25DE6DC8-3A8B-43BD-AD4C-80055808F616}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-3000" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RADSAT-SK Timer" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="157">
   <si>
     <t>Source:</t>
   </si>
@@ -64,9 +75,6 @@
     <t>Description</t>
   </si>
   <si>
-    <t>datasheet</t>
-  </si>
-  <si>
     <t>Vendor</t>
   </si>
   <si>
@@ -211,9 +219,6 @@
     <t>Connector_Molex:Molex_PicoBlade_53047-0710_1x07_P1.25mm_Vertical</t>
   </si>
   <si>
-    <t>Generic connector, single row, 01x07,</t>
-  </si>
-  <si>
     <t xml:space="preserve">J202, </t>
   </si>
   <si>
@@ -304,9 +309,6 @@
     <t>Package_TO_SOT_THT:TO-92L_Inline_Wide</t>
   </si>
   <si>
-    <t>P-JFET transistor, drain/gate/source</t>
-  </si>
-  <si>
     <t xml:space="preserve">R101, R103, R107, R113, R114, R117, R118, R124, R126, R203, </t>
   </si>
   <si>
@@ -425,6 +427,81 @@
   </si>
   <si>
     <t>digikey</t>
+  </si>
+  <si>
+    <t>Product URL</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/molex/0510470700/4693261</t>
+  </si>
+  <si>
+    <t>Price2</t>
+  </si>
+  <si>
+    <t>Related Components</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/onsemi/J176-D74Z/4213841</t>
+  </si>
+  <si>
+    <t>https://www.onsemi.com/pdf/datasheet/j175-d.pdf</t>
+  </si>
+  <si>
+    <t>Datasheet</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/infineon-technologies/irlml2060trpbf/2271899</t>
+  </si>
+  <si>
+    <t>P Channel JFET *product shortage on SMD components</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/texas-instruments/CD4052BPWRG3/2596791</t>
+  </si>
+  <si>
+    <t>https://www.analog.com/media/en/technical-documentation/data-sheets/3440fd.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/analog-devices-inc/LTC3440EMS-PBF/890929?s=N4IgTCBcDaIDIBUDCBmALGgDAUQLIGUAFAIQDEQBdAXyA</t>
+  </si>
+  <si>
+    <t>Total Component Cost:</t>
+  </si>
+  <si>
+    <t>Price total</t>
+  </si>
+  <si>
+    <t>https://www.ti.com/general/docs/suppproductinfo.tsp?distId=10&amp;gotoUrl=https%3A%2F%2Fwww.ti.com%2Flit%2Fgpn%2Flm397</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/texas-instruments/LM397MF/3701445</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/molex/0530470710/242858</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Molex Picoblade 53047 Header and accompanying Picoblade 51047 Connector</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/molex/0500588000/634442</t>
+  </si>
+  <si>
+    <t>crimps?</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/hirose-electric-co-ltd/DF13-2P-1-25DSA-76/9170620</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/Hirose-Connector/DF13-5P-125DSA?qs=Ux3WWAnHpjDJWf8XCjmDFw%3D%3D</t>
+  </si>
+  <si>
+    <t>Mouser</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/datasheet/2/185/DF13_Catalog_D31687_en-2486995.pdf</t>
+  </si>
+  <si>
+    <t>no vertical through hole?</t>
   </si>
 </sst>
 </file>
@@ -432,9 +509,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -573,6 +650,18 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -918,17 +1007,19 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="43"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="42" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="42" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="43" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="44">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -976,7 +1067,10 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
+    <dxf>
+      <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -994,18 +1088,24 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A7:I42" totalsRowShown="0">
-  <autoFilter ref="A7:I42" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Ref" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A7:M42" totalsRowShown="0">
+  <autoFilter ref="A7:M42" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <tableColumns count="13">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Ref" dataDxfId="1"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Qnty"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Value"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Cmp name"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Footprint"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Description"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="datasheet"/>
+    <tableColumn id="12" xr3:uid="{AC2AB4E9-9984-41C3-88C4-EF1E70A1C977}" name="Datasheet"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Product URL"/>
     <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Vendor"/>
     <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Price" dataCellStyle="Currency"/>
+    <tableColumn id="10" xr3:uid="{7C21AC37-B81A-4891-A949-B8777B84C389}" name="Related Components"/>
+    <tableColumn id="11" xr3:uid="{73FB3C5D-D954-4E05-BC68-91835A2C1577}" name="Price2" dataCellStyle="Currency"/>
+    <tableColumn id="13" xr3:uid="{37B8C3F1-4773-42D9-BB38-8CAD10942CF3}" name="Price total" dataDxfId="0">
+      <calculatedColumnFormula>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1308,10 +1408,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I42"/>
+  <dimension ref="A1:O42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F4" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="H1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="P24" sqref="P24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1321,12 +1422,15 @@
     <col min="3" max="4" width="22" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="67.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="107.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="87" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="107.28515625" customWidth="1"/>
+    <col min="8" max="8" width="87" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.7109375" customWidth="1"/>
+    <col min="11" max="11" width="25" customWidth="1"/>
+    <col min="12" max="12" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1334,15 +1438,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -1350,7 +1454,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
@@ -1358,7 +1462,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
@@ -1366,7 +1470,16 @@
         <v>116</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="B6" s="6">
+        <f>SUM(M8:M42)</f>
+        <v>31.773</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
@@ -1386,470 +1499,627 @@
         <v>13</v>
       </c>
       <c r="G7" t="s">
+        <v>138</v>
+      </c>
+      <c r="H7" t="s">
+        <v>132</v>
+      </c>
+      <c r="I7" t="s">
         <v>14</v>
       </c>
-      <c r="H7" t="s">
+      <c r="J7" t="s">
         <v>15</v>
       </c>
-      <c r="I7" t="s">
+      <c r="K7" t="s">
+        <v>135</v>
+      </c>
+      <c r="L7" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="M7" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
         <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>17</v>
       </c>
       <c r="B8">
         <v>2</v>
       </c>
       <c r="C8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" t="s">
         <v>18</v>
       </c>
-      <c r="D8" t="s">
-        <v>18</v>
-      </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>19</v>
       </c>
-      <c r="F8" t="s">
+      <c r="J8" s="4"/>
+      <c r="M8" s="6">
+        <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
         <v>20</v>
-      </c>
-      <c r="I8" s="4"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>21</v>
       </c>
       <c r="B9">
         <v>6</v>
       </c>
       <c r="C9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" t="s">
         <v>22</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>23</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>24</v>
       </c>
-      <c r="F9" t="s">
+      <c r="J9" s="4"/>
+      <c r="M9" s="6">
+        <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
         <v>25</v>
-      </c>
-      <c r="I9" s="4"/>
-    </row>
-    <row r="10" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>26</v>
       </c>
       <c r="B10">
         <v>8</v>
       </c>
       <c r="C10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" t="s">
         <v>27</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>28</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>29</v>
       </c>
-      <c r="F10" t="s">
+      <c r="J10" s="4"/>
+      <c r="M10" s="6">
+        <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
         <v>30</v>
-      </c>
-      <c r="I10" s="4"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>31</v>
       </c>
       <c r="B11">
         <v>1</v>
       </c>
       <c r="C11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" t="s">
+        <v>27</v>
+      </c>
+      <c r="E11" t="s">
+        <v>28</v>
+      </c>
+      <c r="F11" t="s">
+        <v>29</v>
+      </c>
+      <c r="J11" s="4"/>
+      <c r="M11" s="6">
+        <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
         <v>32</v>
-      </c>
-      <c r="D11" t="s">
-        <v>28</v>
-      </c>
-      <c r="E11" t="s">
-        <v>29</v>
-      </c>
-      <c r="F11" t="s">
-        <v>30</v>
-      </c>
-      <c r="I11" s="4"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>33</v>
       </c>
       <c r="B12">
         <v>1</v>
       </c>
       <c r="C12" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" t="s">
+        <v>27</v>
+      </c>
+      <c r="E12" t="s">
+        <v>28</v>
+      </c>
+      <c r="F12" t="s">
+        <v>29</v>
+      </c>
+      <c r="J12" s="4"/>
+      <c r="M12" s="6">
+        <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
         <v>34</v>
-      </c>
-      <c r="D12" t="s">
-        <v>28</v>
-      </c>
-      <c r="E12" t="s">
-        <v>29</v>
-      </c>
-      <c r="F12" t="s">
-        <v>30</v>
-      </c>
-      <c r="I12" s="4"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>35</v>
       </c>
       <c r="B13">
         <v>1</v>
       </c>
       <c r="C13" t="s">
+        <v>35</v>
+      </c>
+      <c r="D13" t="s">
+        <v>27</v>
+      </c>
+      <c r="E13" t="s">
+        <v>28</v>
+      </c>
+      <c r="F13" t="s">
+        <v>29</v>
+      </c>
+      <c r="J13" s="4"/>
+      <c r="M13" s="6">
+        <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
         <v>36</v>
-      </c>
-      <c r="D13" t="s">
-        <v>28</v>
-      </c>
-      <c r="E13" t="s">
-        <v>29</v>
-      </c>
-      <c r="F13" t="s">
-        <v>30</v>
-      </c>
-      <c r="I13" s="4"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>37</v>
       </c>
       <c r="B14">
         <v>1</v>
       </c>
       <c r="C14" t="s">
+        <v>37</v>
+      </c>
+      <c r="D14" t="s">
+        <v>27</v>
+      </c>
+      <c r="E14" t="s">
+        <v>28</v>
+      </c>
+      <c r="F14" t="s">
+        <v>29</v>
+      </c>
+      <c r="J14" s="4"/>
+      <c r="M14" s="6">
+        <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
         <v>38</v>
-      </c>
-      <c r="D14" t="s">
-        <v>28</v>
-      </c>
-      <c r="E14" t="s">
-        <v>29</v>
-      </c>
-      <c r="F14" t="s">
-        <v>30</v>
-      </c>
-      <c r="I14" s="4"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>39</v>
       </c>
       <c r="B15">
         <v>1</v>
       </c>
       <c r="C15" t="s">
+        <v>39</v>
+      </c>
+      <c r="D15" t="s">
+        <v>39</v>
+      </c>
+      <c r="E15" t="s">
         <v>40</v>
       </c>
-      <c r="D15" t="s">
-        <v>40</v>
-      </c>
-      <c r="E15" t="s">
+      <c r="F15" t="s">
         <v>41</v>
       </c>
-      <c r="F15" t="s">
+      <c r="J15" s="4"/>
+      <c r="M15" s="6">
+        <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
         <v>42</v>
-      </c>
-      <c r="I15" s="4"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>43</v>
       </c>
       <c r="B16">
         <v>1</v>
       </c>
       <c r="C16" t="s">
+        <v>43</v>
+      </c>
+      <c r="D16" t="s">
+        <v>43</v>
+      </c>
+      <c r="E16" t="s">
         <v>44</v>
       </c>
-      <c r="D16" t="s">
-        <v>44</v>
-      </c>
-      <c r="E16" t="s">
+      <c r="F16" t="s">
         <v>45</v>
       </c>
-      <c r="F16" t="s">
+      <c r="J16" s="4"/>
+      <c r="M16" s="6">
+        <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
         <v>46</v>
-      </c>
-      <c r="I16" s="4"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>47</v>
       </c>
       <c r="B17">
         <v>1</v>
       </c>
       <c r="C17" t="s">
+        <v>47</v>
+      </c>
+      <c r="D17" t="s">
         <v>48</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
         <v>49</v>
       </c>
-      <c r="E17" t="s">
+      <c r="F17" t="s">
         <v>50</v>
       </c>
-      <c r="F17" t="s">
+      <c r="G17" t="s">
         <v>51</v>
       </c>
-      <c r="G17" t="s">
+      <c r="J17" s="4"/>
+      <c r="M17" s="6">
+        <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
         <v>52</v>
-      </c>
-      <c r="I17" s="4"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
-        <v>53</v>
       </c>
       <c r="B18">
         <v>3</v>
       </c>
       <c r="C18" t="s">
+        <v>53</v>
+      </c>
+      <c r="D18" t="s">
+        <v>53</v>
+      </c>
+      <c r="E18" t="s">
+        <v>44</v>
+      </c>
+      <c r="F18" t="s">
         <v>54</v>
       </c>
-      <c r="D18" t="s">
-        <v>54</v>
-      </c>
-      <c r="E18" t="s">
-        <v>45</v>
-      </c>
-      <c r="F18" t="s">
+      <c r="J18" s="4"/>
+      <c r="M18" s="6">
+        <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
         <v>55</v>
-      </c>
-      <c r="I18" s="4"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
-        <v>56</v>
       </c>
       <c r="B19">
         <v>2</v>
       </c>
       <c r="C19" t="s">
+        <v>56</v>
+      </c>
+      <c r="D19" t="s">
+        <v>56</v>
+      </c>
+      <c r="E19" t="s">
         <v>57</v>
       </c>
-      <c r="D19" t="s">
-        <v>57</v>
-      </c>
-      <c r="E19" t="s">
+      <c r="F19" t="s">
         <v>58</v>
       </c>
-      <c r="F19" t="s">
+      <c r="J19" s="4"/>
+      <c r="M19" s="6">
+        <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
+        <v>0</v>
+      </c>
+      <c r="O19" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
         <v>59</v>
-      </c>
-      <c r="I19" s="4"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
-        <v>60</v>
       </c>
       <c r="B20">
         <v>1</v>
       </c>
       <c r="C20" t="s">
+        <v>60</v>
+      </c>
+      <c r="D20" t="s">
+        <v>60</v>
+      </c>
+      <c r="E20" t="s">
         <v>61</v>
       </c>
-      <c r="D20" t="s">
-        <v>61</v>
-      </c>
-      <c r="E20" t="s">
+      <c r="F20" t="s">
+        <v>149</v>
+      </c>
+      <c r="H20" t="s">
+        <v>148</v>
+      </c>
+      <c r="I20" t="s">
+        <v>131</v>
+      </c>
+      <c r="J20" s="4">
+        <v>0.61</v>
+      </c>
+      <c r="K20" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="L20" s="4">
+        <v>0.52</v>
+      </c>
+      <c r="M20" s="6">
+        <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
+        <v>1.1299999999999999</v>
+      </c>
+      <c r="O20" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
         <v>62</v>
-      </c>
-      <c r="F20" t="s">
-        <v>63</v>
-      </c>
-      <c r="I20" s="4"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
-        <v>64</v>
       </c>
       <c r="B21">
         <v>1</v>
       </c>
       <c r="C21" t="s">
+        <v>63</v>
+      </c>
+      <c r="D21" t="s">
+        <v>63</v>
+      </c>
+      <c r="E21" t="s">
+        <v>64</v>
+      </c>
+      <c r="F21" t="s">
         <v>65</v>
       </c>
-      <c r="D21" t="s">
-        <v>65</v>
-      </c>
-      <c r="E21" t="s">
+      <c r="G21" t="s">
+        <v>155</v>
+      </c>
+      <c r="H21" t="s">
+        <v>153</v>
+      </c>
+      <c r="I21" t="s">
+        <v>154</v>
+      </c>
+      <c r="J21" s="4">
+        <v>0.59299999999999997</v>
+      </c>
+      <c r="M21" s="6">
+        <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
+        <v>0.59299999999999997</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
         <v>66</v>
-      </c>
-      <c r="F21" t="s">
-        <v>67</v>
-      </c>
-      <c r="I21" s="4"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
-        <v>68</v>
       </c>
       <c r="B22">
         <v>1</v>
       </c>
       <c r="C22" t="s">
+        <v>67</v>
+      </c>
+      <c r="D22" t="s">
+        <v>67</v>
+      </c>
+      <c r="E22" t="s">
+        <v>68</v>
+      </c>
+      <c r="F22" t="s">
         <v>69</v>
       </c>
-      <c r="D22" t="s">
-        <v>69</v>
-      </c>
-      <c r="E22" t="s">
+      <c r="J22" s="4"/>
+      <c r="M22" s="6">
+        <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
+        <v>0</v>
+      </c>
+      <c r="O22" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
         <v>70</v>
-      </c>
-      <c r="F22" t="s">
-        <v>71</v>
-      </c>
-      <c r="I22" s="4"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
-        <v>72</v>
       </c>
       <c r="B23">
         <v>3</v>
       </c>
       <c r="C23" t="s">
+        <v>71</v>
+      </c>
+      <c r="D23" t="s">
+        <v>71</v>
+      </c>
+      <c r="E23" t="s">
+        <v>72</v>
+      </c>
+      <c r="F23" t="s">
         <v>73</v>
       </c>
-      <c r="D23" t="s">
-        <v>73</v>
-      </c>
-      <c r="E23" t="s">
+      <c r="H23" t="s">
+        <v>152</v>
+      </c>
+      <c r="I23" t="s">
+        <v>131</v>
+      </c>
+      <c r="J23" s="4">
+        <v>0.66</v>
+      </c>
+      <c r="M23" s="6">
+        <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
+        <v>1.98</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
         <v>74</v>
-      </c>
-      <c r="F23" t="s">
-        <v>75</v>
-      </c>
-      <c r="I23" s="4"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
-        <v>76</v>
       </c>
       <c r="B24">
         <v>1</v>
       </c>
       <c r="C24" t="s">
+        <v>75</v>
+      </c>
+      <c r="D24" t="s">
+        <v>75</v>
+      </c>
+      <c r="E24" t="s">
+        <v>76</v>
+      </c>
+      <c r="H24" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="D24" t="s">
-        <v>77</v>
-      </c>
-      <c r="E24" t="s">
+      <c r="I24" t="s">
+        <v>131</v>
+      </c>
+      <c r="J24" s="4">
+        <v>1.76</v>
+      </c>
+      <c r="M24" s="6">
+        <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
+        <v>1.76</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
         <v>78</v>
-      </c>
-      <c r="G24" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="H24" t="s">
-        <v>134</v>
-      </c>
-      <c r="I24" s="4">
-        <v>1.76</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
-        <v>80</v>
       </c>
       <c r="B25">
         <v>1</v>
       </c>
       <c r="C25" t="s">
+        <v>79</v>
+      </c>
+      <c r="D25" t="s">
+        <v>80</v>
+      </c>
+      <c r="E25" t="s">
         <v>81</v>
       </c>
-      <c r="D25" t="s">
+      <c r="F25" t="s">
         <v>82</v>
       </c>
-      <c r="E25" t="s">
+      <c r="J25" s="4"/>
+      <c r="M25" s="6">
+        <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
         <v>83</v>
-      </c>
-      <c r="F25" t="s">
-        <v>84</v>
-      </c>
-      <c r="I25" s="4"/>
-    </row>
-    <row r="26" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
-        <v>85</v>
       </c>
       <c r="B26">
         <v>11</v>
       </c>
       <c r="C26" t="s">
+        <v>84</v>
+      </c>
+      <c r="D26" t="s">
+        <v>84</v>
+      </c>
+      <c r="E26" t="s">
+        <v>85</v>
+      </c>
+      <c r="F26" t="s">
         <v>86</v>
       </c>
-      <c r="D26" t="s">
-        <v>86</v>
-      </c>
-      <c r="E26" t="s">
+      <c r="G26" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="F26" t="s">
+      <c r="H26" t="s">
+        <v>139</v>
+      </c>
+      <c r="I26" t="s">
+        <v>131</v>
+      </c>
+      <c r="J26" s="4">
+        <v>0.63</v>
+      </c>
+      <c r="M26" s="6">
+        <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
+        <v>6.93</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
         <v>88</v>
-      </c>
-      <c r="G26" t="s">
-        <v>89</v>
-      </c>
-      <c r="I26" s="4"/>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
-        <v>90</v>
       </c>
       <c r="B27">
         <v>4</v>
       </c>
       <c r="C27" t="s">
+        <v>89</v>
+      </c>
+      <c r="D27" t="s">
+        <v>90</v>
+      </c>
+      <c r="E27" t="s">
         <v>91</v>
       </c>
-      <c r="D27" t="s">
+      <c r="F27" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="H27" t="s">
+        <v>136</v>
+      </c>
+      <c r="I27" t="s">
+        <v>131</v>
+      </c>
+      <c r="J27" s="4">
+        <v>0.77</v>
+      </c>
+      <c r="M27" s="6">
+        <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
+        <v>3.08</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
         <v>92</v>
-      </c>
-      <c r="E27" t="s">
-        <v>93</v>
-      </c>
-      <c r="F27" t="s">
-        <v>94</v>
-      </c>
-      <c r="I27" s="4"/>
-    </row>
-    <row r="28" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
-        <v>95</v>
       </c>
       <c r="B28">
         <v>10</v>
       </c>
       <c r="C28" t="s">
+        <v>93</v>
+      </c>
+      <c r="D28" t="s">
+        <v>94</v>
+      </c>
+      <c r="E28" t="s">
+        <v>95</v>
+      </c>
+      <c r="F28" t="s">
         <v>96</v>
       </c>
-      <c r="D28" t="s">
+      <c r="J28" s="4"/>
+      <c r="M28" s="6">
+        <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
         <v>97</v>
-      </c>
-      <c r="E28" t="s">
-        <v>98</v>
-      </c>
-      <c r="F28" t="s">
-        <v>99</v>
-      </c>
-      <c r="I28" s="4"/>
-    </row>
-    <row r="29" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
-        <v>100</v>
       </c>
       <c r="B29">
         <v>12</v>
@@ -1858,293 +2128,383 @@
         <v>100</v>
       </c>
       <c r="D29" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="E29" t="s">
+        <v>95</v>
+      </c>
+      <c r="F29" t="s">
+        <v>96</v>
+      </c>
+      <c r="J29" s="4"/>
+      <c r="M29" s="6">
+        <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
         <v>98</v>
-      </c>
-      <c r="F29" t="s">
-        <v>99</v>
-      </c>
-      <c r="I29" s="4"/>
-    </row>
-    <row r="30" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
-        <v>101</v>
       </c>
       <c r="B30">
         <v>16</v>
       </c>
       <c r="C30" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="D30" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="E30" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="F30" t="s">
-        <v>99</v>
-      </c>
-      <c r="I30" s="4"/>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+      <c r="J30" s="4"/>
+      <c r="M30" s="6">
+        <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B31">
         <v>3</v>
       </c>
       <c r="C31" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="D31" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="E31" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="F31" t="s">
-        <v>99</v>
-      </c>
-      <c r="I31" s="4"/>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+      <c r="J31" s="4"/>
+      <c r="M31" s="6">
+        <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B32">
         <v>3</v>
       </c>
       <c r="C32" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="D32" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="E32" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="F32" t="s">
-        <v>99</v>
-      </c>
-      <c r="I32" s="4"/>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+      <c r="J32" s="4"/>
+      <c r="M32" s="6">
+        <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B33">
         <v>1</v>
       </c>
       <c r="C33" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="D33" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="E33" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="F33" t="s">
-        <v>99</v>
-      </c>
-      <c r="I33" s="4"/>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+      <c r="J33" s="4"/>
+      <c r="M33" s="6">
+        <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B34">
         <v>1</v>
       </c>
       <c r="C34" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="D34" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="E34" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="F34" t="s">
-        <v>99</v>
-      </c>
-      <c r="I34" s="4"/>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+      <c r="J34" s="4"/>
+      <c r="M34" s="6">
+        <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B35">
         <v>1</v>
       </c>
       <c r="C35" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="D35" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="E35" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="F35" t="s">
-        <v>99</v>
-      </c>
-      <c r="I35" s="4"/>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+      <c r="J35" s="4"/>
+      <c r="M35" s="6">
+        <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B36">
         <v>1</v>
       </c>
       <c r="C36" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="D36" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="E36" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="F36" t="s">
-        <v>99</v>
-      </c>
-      <c r="I36" s="4"/>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+      <c r="J36" s="4"/>
+      <c r="M36" s="6">
+        <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B37">
         <v>1</v>
       </c>
       <c r="C37" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D37" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="E37" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="F37" t="s">
-        <v>99</v>
-      </c>
-      <c r="I37" s="4"/>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+      <c r="J37" s="4"/>
+      <c r="M37" s="6">
+        <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B38">
         <v>1</v>
       </c>
       <c r="C38" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="D38" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="E38" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="F38" t="s">
-        <v>99</v>
-      </c>
-      <c r="I38" s="4"/>
-    </row>
-    <row r="39" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+      <c r="J38" s="4"/>
+      <c r="M38" s="6">
+        <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B39">
         <v>6</v>
       </c>
       <c r="C39" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="D39" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="E39" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F39" t="s">
-        <v>121</v>
-      </c>
-      <c r="I39" s="4"/>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+      <c r="J39" s="4"/>
+      <c r="M39" s="6">
+        <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B40">
         <v>3</v>
       </c>
       <c r="C40" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="D40" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="E40" t="s">
-        <v>124</v>
-      </c>
-      <c r="I40" s="4"/>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+        <v>121</v>
+      </c>
+      <c r="G40" t="s">
+        <v>146</v>
+      </c>
+      <c r="H40" t="s">
+        <v>147</v>
+      </c>
+      <c r="I40" t="s">
+        <v>131</v>
+      </c>
+      <c r="J40" s="4">
+        <v>1.96</v>
+      </c>
+      <c r="M40" s="6">
+        <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
+        <v>5.88</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B41">
         <v>1</v>
       </c>
       <c r="C41" t="s">
+        <v>123</v>
+      </c>
+      <c r="D41" t="s">
+        <v>123</v>
+      </c>
+      <c r="E41" t="s">
+        <v>124</v>
+      </c>
+      <c r="F41" t="s">
+        <v>125</v>
+      </c>
+      <c r="G41" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="D41" t="s">
-        <v>126</v>
-      </c>
-      <c r="E41" t="s">
+      <c r="H41" t="s">
+        <v>141</v>
+      </c>
+      <c r="I41" t="s">
+        <v>131</v>
+      </c>
+      <c r="J41" s="4">
+        <v>0.81</v>
+      </c>
+      <c r="M41" s="6">
+        <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
+        <v>0.81</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
         <v>127</v>
-      </c>
-      <c r="F41" t="s">
-        <v>128</v>
-      </c>
-      <c r="G41" t="s">
-        <v>129</v>
-      </c>
-      <c r="I41" s="4"/>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A42" s="2" t="s">
-        <v>130</v>
       </c>
       <c r="B42">
         <v>1</v>
       </c>
       <c r="C42" t="s">
+        <v>128</v>
+      </c>
+      <c r="D42" t="s">
+        <v>128</v>
+      </c>
+      <c r="E42" t="s">
+        <v>129</v>
+      </c>
+      <c r="G42" t="s">
+        <v>142</v>
+      </c>
+      <c r="H42" t="s">
+        <v>143</v>
+      </c>
+      <c r="I42" t="s">
         <v>131</v>
       </c>
-      <c r="D42" t="s">
-        <v>131</v>
-      </c>
-      <c r="E42" t="s">
-        <v>132</v>
-      </c>
-      <c r="I42" s="4"/>
+      <c r="J42" s="4">
+        <v>9.61</v>
+      </c>
+      <c r="M42" s="6">
+        <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
+        <v>9.61</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="19" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="G24" r:id="rId1" xr:uid="{DD8AD352-FB06-4715-B587-8B7434FCD99F}"/>
+    <hyperlink ref="H24" r:id="rId1" xr:uid="{DD8AD352-FB06-4715-B587-8B7434FCD99F}"/>
+    <hyperlink ref="G26" r:id="rId2" xr:uid="{5EFE7EEC-7A33-4705-B297-C4BD3E05DA2C}"/>
+    <hyperlink ref="G41" r:id="rId3" xr:uid="{71FE485A-AA2E-4950-BE10-E132C884D307}"/>
+    <hyperlink ref="K20" r:id="rId4" xr:uid="{DB18BABB-D85D-4D81-84B1-06B4803F7A71}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId5"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
More components to the BOM and fixed footprints on the schematic to mathc chosen parts
</commit_message>
<xml_diff>
--- a/RADSAT-SK Timer/RADSAT-SK Timer.xlsx
+++ b/RADSAT-SK Timer/RADSAT-SK Timer.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\USST\power-and-electrical\RADSAT-SK Timer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25DE6DC8-3A8B-43BD-AD4C-80055808F616}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4662F800-20E8-414A-B847-5AE9725A4C5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-3000" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="170">
   <si>
     <t>Source:</t>
   </si>
@@ -72,9 +72,6 @@
     <t>Footprint</t>
   </si>
   <si>
-    <t>Description</t>
-  </si>
-  <si>
     <t>Vendor</t>
   </si>
   <si>
@@ -174,27 +171,9 @@
     <t xml:space="preserve">D203, </t>
   </si>
   <si>
-    <t>MBRM1020T3</t>
-  </si>
-  <si>
-    <t>MBR1020VL</t>
-  </si>
-  <si>
-    <t>Diode_SMD:D_SOD-123F</t>
-  </si>
-  <si>
-    <t>20V, 1A, 340 mV, Schottky Diode Rectifier, SOD-123F</t>
-  </si>
-  <si>
-    <t>https://www.onsemi.com/pub/Collateral/MBR1020VL-D.PDF</t>
-  </si>
-  <si>
     <t xml:space="preserve">D204, D205, D206, </t>
   </si>
   <si>
-    <t>D</t>
-  </si>
-  <si>
     <t>Diode</t>
   </si>
   <si>
@@ -207,9 +186,6 @@
     <t>Connector_PinSocket_2.54mm:PinSocket_2x26_P2.54mm_Vertical</t>
   </si>
   <si>
-    <t xml:space="preserve">Generic connector, double row, 02x26, odd/even pin numbering scheme (row 1 odd numbers, row 2 even numbers),  </t>
-  </si>
-  <si>
     <t xml:space="preserve">J201, </t>
   </si>
   <si>
@@ -243,18 +219,12 @@
     <t xml:space="preserve">Generic connector, single row, 01x03, </t>
   </si>
   <si>
-    <t xml:space="preserve">J204, J205, J206, </t>
-  </si>
-  <si>
     <t>Conn_01x02</t>
   </si>
   <si>
     <t>Connector_Hirose:Hirose_DF13-02P-1.25DSA_1x02_P1.25mm_Vertical</t>
   </si>
   <si>
-    <t>Generic connector, single row, 01x02,</t>
-  </si>
-  <si>
     <t xml:space="preserve">J210, </t>
   </si>
   <si>
@@ -279,9 +249,6 @@
     <t>Inductor_SMD:L_0805_2012Metric</t>
   </si>
   <si>
-    <t>Inductor</t>
-  </si>
-  <si>
     <t xml:space="preserve">Q101, Q102, Q103, Q104, Q105, Q106, Q107, Q108, Q109, Q201, Q202, </t>
   </si>
   <si>
@@ -381,9 +348,6 @@
     <t>200k</t>
   </si>
   <si>
-    <t xml:space="preserve">SW201, SW202, SW203, SW204, SW205, SW206, </t>
-  </si>
-  <si>
     <t>SW_Push</t>
   </si>
   <si>
@@ -502,6 +466,81 @@
   </si>
   <si>
     <t>no vertical through hole?</t>
+  </si>
+  <si>
+    <t>https://www.onsemi.com/pdf/datasheet/mbrm120l-d.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/onsemi/MBRM120LT3G/1748989</t>
+  </si>
+  <si>
+    <t>MBRM120LT3G</t>
+  </si>
+  <si>
+    <t>D_Schottky</t>
+  </si>
+  <si>
+    <t>Diode_SMD:D_Powermite_AK</t>
+  </si>
+  <si>
+    <t>https://www.mccsemi.com/pdf/Products/SM5817PL-SM5819PL(SOD-123FL).PDF</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/micro-commercial-co/SM5817PL-TP/1793251</t>
+  </si>
+  <si>
+    <t>SM5817PL-TP</t>
+  </si>
+  <si>
+    <t>USB Connector</t>
+  </si>
+  <si>
+    <t>https://products.sumida.com/products/pdf/CDRH4D28.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/sumida-america-components-inc/CDRH4D28NP-100NC/1059478</t>
+  </si>
+  <si>
+    <t>DIGIKEY</t>
+  </si>
+  <si>
+    <t>DIODE SCHOTTKY 20V 1A POWERMITE | from boost circuit</t>
+  </si>
+  <si>
+    <t>FIXED IND 10UH 1A 128.3 MOHM SMD  |  from boost circuit</t>
+  </si>
+  <si>
+    <t>Description/Notes</t>
+  </si>
+  <si>
+    <t>CSKB</t>
+  </si>
+  <si>
+    <t>https://www.hirose.com/product/document?clcode=CL0536-0109-0-76&amp;productname=DF13-10P-1.25DSA(76)&amp;series=DF13&amp;documenttype=Catalog&amp;lang=en&amp;documentid=D31687_en</t>
+  </si>
+  <si>
+    <t xml:space="preserve">J204, J205, J206, SW201, SW202, SW203, SW204, SW205, SW206, </t>
+  </si>
+  <si>
+    <t>22 µF ±20% 6.3V Ceramic Capacitor X5R 1210 (3225 Metric)</t>
+  </si>
+  <si>
+    <t>https://ds.yuden.co.jp/TYCOMPAS/ut/detail?pn=JMK325BJ226MY-T%20%20&amp;u=M</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/taiyo-yuden/JMK325BJ226MY-T/930737?s=N4IgjCBcoLQExVAYygFwE4FcCmAaEA9lANogCsIAugL74wTQgqQBmAhgDYDOehJ5ADgDsVarRAJIpADqoABHDhyArQDE5ARrgAGAKRyAbADoAzADU5AYWzo2AWwCWSK2wAObJA9QF0cgBpkAEpyYHBg2nIAFCaKZHIAstgYTgCUokA</t>
+  </si>
+  <si>
+    <t>Capacitor_SMD:C_1210_3225Metric</t>
+  </si>
+  <si>
+    <t>https://www.yuden.co.jp/productdata/catalog/mlcc06_e.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/taiyo-yuden/JMK212BJ106MG-T/1169928?s=N4IgTCBcDaICoEECSBNA8gAhQVQCIFEA5DAKQFkBpMARjACETqAGANjIHEQBdAXyA</t>
+  </si>
+  <si>
+    <t>10 µF ±20% 6.3V Ceramic Capacitor X5R 0805 (2012 Metric)</t>
   </si>
 </sst>
 </file>
@@ -1088,15 +1127,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A7:M42" totalsRowShown="0">
-  <autoFilter ref="A7:M42" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A7:M41" totalsRowShown="0">
+  <autoFilter ref="A7:M41" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Ref" dataDxfId="1"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Qnty"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Value"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Cmp name"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Footprint"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Description"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Description/Notes"/>
     <tableColumn id="12" xr3:uid="{AC2AB4E9-9984-41C3-88C4-EF1E70A1C977}" name="Datasheet"/>
     <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Product URL"/>
     <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Vendor"/>
@@ -1408,18 +1447,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O42"/>
+  <dimension ref="A1:O41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="H1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="P24" sqref="P24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="40.85546875" style="2" customWidth="1"/>
     <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="22" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.140625" customWidth="1"/>
+    <col min="4" max="4" width="22" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="67.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="107.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="107.28515625" customWidth="1"/>
@@ -1443,7 +1483,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>130</v>
+        <v>118</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -1472,11 +1512,11 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>144</v>
+        <v>132</v>
       </c>
       <c r="B6" s="6">
-        <f>SUM(M8:M42)</f>
-        <v>31.773</v>
+        <f>SUM(M8:M41)</f>
+        <v>40.675999999999995</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -1496,48 +1536,48 @@
         <v>12</v>
       </c>
       <c r="F7" t="s">
+        <v>159</v>
+      </c>
+      <c r="G7" t="s">
+        <v>126</v>
+      </c>
+      <c r="H7" t="s">
+        <v>120</v>
+      </c>
+      <c r="I7" t="s">
         <v>13</v>
       </c>
-      <c r="G7" t="s">
-        <v>138</v>
-      </c>
-      <c r="H7" t="s">
-        <v>132</v>
-      </c>
-      <c r="I7" t="s">
+      <c r="J7" t="s">
         <v>14</v>
       </c>
-      <c r="J7" t="s">
-        <v>15</v>
-      </c>
       <c r="K7" t="s">
-        <v>135</v>
+        <v>123</v>
       </c>
       <c r="L7" s="4" t="s">
-        <v>134</v>
+        <v>122</v>
       </c>
       <c r="M7" t="s">
-        <v>145</v>
+        <v>133</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B8">
         <v>2</v>
       </c>
       <c r="C8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" t="s">
         <v>17</v>
       </c>
-      <c r="D8" t="s">
-        <v>17</v>
-      </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>18</v>
-      </c>
-      <c r="F8" t="s">
-        <v>19</v>
       </c>
       <c r="J8" s="4"/>
       <c r="M8" s="6">
@@ -1547,22 +1587,22 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B9">
         <v>6</v>
       </c>
       <c r="C9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" t="s">
         <v>21</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>22</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>23</v>
-      </c>
-      <c r="F9" t="s">
-        <v>24</v>
       </c>
       <c r="J9" s="4"/>
       <c r="M9" s="6">
@@ -1572,22 +1612,22 @@
     </row>
     <row r="10" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B10">
         <v>8</v>
       </c>
       <c r="C10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" t="s">
         <v>26</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>27</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>28</v>
-      </c>
-      <c r="F10" t="s">
-        <v>29</v>
       </c>
       <c r="J10" s="4"/>
       <c r="M10" s="6">
@@ -1597,47 +1637,58 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B11">
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D11" t="s">
+        <v>26</v>
+      </c>
+      <c r="E11" t="s">
         <v>27</v>
       </c>
-      <c r="E11" t="s">
-        <v>28</v>
-      </c>
-      <c r="F11" t="s">
-        <v>29</v>
-      </c>
-      <c r="J11" s="4"/>
+      <c r="F11" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="G11" t="s">
+        <v>167</v>
+      </c>
+      <c r="H11" t="s">
+        <v>168</v>
+      </c>
+      <c r="I11" t="s">
+        <v>119</v>
+      </c>
+      <c r="J11" s="4">
+        <v>0.41</v>
+      </c>
       <c r="M11" s="6">
         <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
-        <v>0</v>
+        <v>0.41</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B12">
         <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D12" t="s">
+        <v>26</v>
+      </c>
+      <c r="E12" t="s">
         <v>27</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
         <v>28</v>
-      </c>
-      <c r="F12" t="s">
-        <v>29</v>
       </c>
       <c r="J12" s="4"/>
       <c r="M12" s="6">
@@ -1647,22 +1698,22 @@
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B13">
         <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D13" t="s">
+        <v>26</v>
+      </c>
+      <c r="E13" t="s">
         <v>27</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
         <v>28</v>
-      </c>
-      <c r="F13" t="s">
-        <v>29</v>
       </c>
       <c r="J13" s="4"/>
       <c r="M13" s="6">
@@ -1672,47 +1723,58 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B14">
         <v>1</v>
       </c>
       <c r="C14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E14" t="s">
-        <v>28</v>
-      </c>
-      <c r="F14" t="s">
-        <v>29</v>
-      </c>
-      <c r="J14" s="4"/>
+        <v>166</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="G14" t="s">
+        <v>164</v>
+      </c>
+      <c r="H14" t="s">
+        <v>165</v>
+      </c>
+      <c r="I14" t="s">
+        <v>119</v>
+      </c>
+      <c r="J14" s="4">
+        <v>1.0900000000000001</v>
+      </c>
       <c r="M14" s="6">
         <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
-        <v>0</v>
+        <v>1.0900000000000001</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B15">
         <v>1</v>
       </c>
       <c r="C15" t="s">
+        <v>38</v>
+      </c>
+      <c r="D15" t="s">
+        <v>38</v>
+      </c>
+      <c r="E15" t="s">
         <v>39</v>
       </c>
-      <c r="D15" t="s">
-        <v>39</v>
-      </c>
-      <c r="E15" t="s">
+      <c r="F15" t="s">
         <v>40</v>
-      </c>
-      <c r="F15" t="s">
-        <v>41</v>
       </c>
       <c r="J15" s="4"/>
       <c r="M15" s="6">
@@ -1722,22 +1784,22 @@
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B16">
         <v>1</v>
       </c>
       <c r="C16" t="s">
+        <v>42</v>
+      </c>
+      <c r="D16" t="s">
+        <v>42</v>
+      </c>
+      <c r="E16" t="s">
         <v>43</v>
       </c>
-      <c r="D16" t="s">
-        <v>43</v>
-      </c>
-      <c r="E16" t="s">
+      <c r="F16" t="s">
         <v>44</v>
-      </c>
-      <c r="F16" t="s">
-        <v>45</v>
       </c>
       <c r="J16" s="4"/>
       <c r="M16" s="6">
@@ -1747,75 +1809,94 @@
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B17">
         <v>1</v>
       </c>
       <c r="C17" t="s">
-        <v>47</v>
+        <v>147</v>
       </c>
       <c r="D17" t="s">
-        <v>48</v>
+        <v>148</v>
       </c>
       <c r="E17" t="s">
-        <v>49</v>
+        <v>149</v>
       </c>
       <c r="F17" t="s">
-        <v>50</v>
-      </c>
-      <c r="G17" t="s">
-        <v>51</v>
-      </c>
-      <c r="J17" s="4"/>
+        <v>157</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="H17" t="s">
+        <v>146</v>
+      </c>
+      <c r="I17" t="s">
+        <v>119</v>
+      </c>
+      <c r="J17" s="4">
+        <v>0.76</v>
+      </c>
       <c r="M17" s="6">
         <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0.76</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="B18">
         <v>3</v>
       </c>
-      <c r="C18" t="s">
-        <v>53</v>
+      <c r="C18" s="2" t="s">
+        <v>152</v>
       </c>
       <c r="D18" t="s">
-        <v>53</v>
+        <v>148</v>
       </c>
       <c r="E18" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F18" t="s">
-        <v>54</v>
-      </c>
-      <c r="J18" s="4"/>
+        <v>47</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="H18" t="s">
+        <v>151</v>
+      </c>
+      <c r="I18" t="s">
+        <v>119</v>
+      </c>
+      <c r="J18" s="4">
+        <v>0.65</v>
+      </c>
       <c r="M18" s="6">
         <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
-        <v>0</v>
+        <v>1.9500000000000002</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="B19">
         <v>2</v>
       </c>
       <c r="C19" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="D19" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="E19" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="F19" t="s">
-        <v>58</v>
+        <v>160</v>
       </c>
       <c r="J19" s="4"/>
       <c r="M19" s="6">
@@ -1823,39 +1904,39 @@
         <v>0</v>
       </c>
       <c r="O19" t="s">
-        <v>151</v>
+        <v>139</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="B20">
         <v>1</v>
       </c>
       <c r="C20" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="D20" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="E20" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="F20" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="H20" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="I20" t="s">
-        <v>131</v>
+        <v>119</v>
       </c>
       <c r="J20" s="4">
         <v>0.61</v>
       </c>
       <c r="K20" s="3" t="s">
-        <v>133</v>
+        <v>121</v>
       </c>
       <c r="L20" s="4">
         <v>0.52</v>
@@ -1865,36 +1946,36 @@
         <v>1.1299999999999999</v>
       </c>
       <c r="O20" t="s">
-        <v>150</v>
+        <v>138</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="B21">
         <v>1</v>
       </c>
       <c r="C21" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="D21" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="E21" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="F21" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="G21" t="s">
-        <v>155</v>
+        <v>143</v>
       </c>
       <c r="H21" t="s">
-        <v>153</v>
+        <v>141</v>
       </c>
       <c r="I21" t="s">
-        <v>154</v>
+        <v>142</v>
       </c>
       <c r="J21" s="4">
         <v>0.59299999999999997</v>
@@ -1906,22 +1987,22 @@
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="B22">
         <v>1</v>
       </c>
       <c r="C22" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="D22" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="E22" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="F22" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="J22" s="4"/>
       <c r="M22" s="6">
@@ -1929,187 +2010,193 @@
         <v>0</v>
       </c>
       <c r="O22" t="s">
-        <v>156</v>
+        <v>144</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="B23">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C23" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="D23" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="E23" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="F23" t="s">
-        <v>73</v>
-      </c>
-      <c r="H23" t="s">
-        <v>152</v>
+        <v>153</v>
+      </c>
+      <c r="H23" s="3" t="s">
+        <v>67</v>
       </c>
       <c r="I23" t="s">
-        <v>131</v>
+        <v>119</v>
       </c>
       <c r="J23" s="4">
-        <v>0.66</v>
+        <v>1.76</v>
       </c>
       <c r="M23" s="6">
         <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
-        <v>1.98</v>
+        <v>1.76</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="B24">
         <v>1</v>
       </c>
       <c r="C24" t="s">
+        <v>69</v>
+      </c>
+      <c r="D24" t="s">
+        <v>70</v>
+      </c>
+      <c r="E24" t="s">
+        <v>71</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="G24" t="s">
+        <v>154</v>
+      </c>
+      <c r="H24" t="s">
+        <v>155</v>
+      </c>
+      <c r="I24" t="s">
+        <v>156</v>
+      </c>
+      <c r="J24" s="4">
+        <v>1.48</v>
+      </c>
+      <c r="M24" s="6">
+        <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
+        <v>1.48</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B25">
+        <v>11</v>
+      </c>
+      <c r="C25" t="s">
+        <v>73</v>
+      </c>
+      <c r="D25" t="s">
+        <v>73</v>
+      </c>
+      <c r="E25" t="s">
+        <v>74</v>
+      </c>
+      <c r="F25" t="s">
         <v>75</v>
       </c>
-      <c r="D24" t="s">
-        <v>75</v>
-      </c>
-      <c r="E24" t="s">
+      <c r="G25" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="H24" s="3" t="s">
+      <c r="H25" t="s">
+        <v>127</v>
+      </c>
+      <c r="I25" t="s">
+        <v>119</v>
+      </c>
+      <c r="J25" s="4">
+        <v>0.63</v>
+      </c>
+      <c r="M25" s="6">
+        <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
+        <v>6.93</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="I24" t="s">
-        <v>131</v>
-      </c>
-      <c r="J24" s="4">
-        <v>1.76</v>
-      </c>
-      <c r="M24" s="6">
-        <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
-        <v>1.76</v>
-      </c>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
+      <c r="B26">
+        <v>4</v>
+      </c>
+      <c r="C26" t="s">
         <v>78</v>
       </c>
-      <c r="B25">
-        <v>1</v>
-      </c>
-      <c r="C25" t="s">
+      <c r="D26" t="s">
         <v>79</v>
       </c>
-      <c r="D25" t="s">
+      <c r="E26" t="s">
         <v>80</v>
       </c>
-      <c r="E25" t="s">
+      <c r="F26" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="H26" t="s">
+        <v>124</v>
+      </c>
+      <c r="I26" t="s">
+        <v>119</v>
+      </c>
+      <c r="J26" s="4">
+        <v>0.77</v>
+      </c>
+      <c r="M26" s="6">
+        <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
+        <v>3.08</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="F25" t="s">
+      <c r="B27">
+        <v>10</v>
+      </c>
+      <c r="C27" t="s">
         <v>82</v>
       </c>
-      <c r="J25" s="4"/>
-      <c r="M25" s="6">
+      <c r="D27" t="s">
+        <v>83</v>
+      </c>
+      <c r="E27" t="s">
+        <v>84</v>
+      </c>
+      <c r="F27" t="s">
+        <v>85</v>
+      </c>
+      <c r="J27" s="4"/>
+      <c r="M27" s="6">
         <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
         <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="B26">
-        <v>11</v>
-      </c>
-      <c r="C26" t="s">
-        <v>84</v>
-      </c>
-      <c r="D26" t="s">
-        <v>84</v>
-      </c>
-      <c r="E26" t="s">
-        <v>85</v>
-      </c>
-      <c r="F26" t="s">
-        <v>86</v>
-      </c>
-      <c r="G26" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="H26" t="s">
-        <v>139</v>
-      </c>
-      <c r="I26" t="s">
-        <v>131</v>
-      </c>
-      <c r="J26" s="4">
-        <v>0.63</v>
-      </c>
-      <c r="M26" s="6">
-        <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
-        <v>6.93</v>
-      </c>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="B27">
-        <v>4</v>
-      </c>
-      <c r="C27" t="s">
-        <v>89</v>
-      </c>
-      <c r="D27" t="s">
-        <v>90</v>
-      </c>
-      <c r="E27" t="s">
-        <v>91</v>
-      </c>
-      <c r="F27" s="5" t="s">
-        <v>140</v>
-      </c>
-      <c r="G27" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="H27" t="s">
-        <v>136</v>
-      </c>
-      <c r="I27" t="s">
-        <v>131</v>
-      </c>
-      <c r="J27" s="4">
-        <v>0.77</v>
-      </c>
-      <c r="M27" s="6">
-        <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
-        <v>3.08</v>
       </c>
     </row>
     <row r="28" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="B28">
-        <v>10</v>
-      </c>
-      <c r="C28" t="s">
-        <v>93</v>
+        <v>12</v>
+      </c>
+      <c r="C28">
+        <v>100</v>
       </c>
       <c r="D28" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="E28" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="F28" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="J28" s="4"/>
       <c r="M28" s="6">
@@ -2117,24 +2204,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="B29">
-        <v>12</v>
-      </c>
-      <c r="C29">
-        <v>100</v>
+        <v>16</v>
+      </c>
+      <c r="C29" t="s">
+        <v>88</v>
       </c>
       <c r="D29" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="E29" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="F29" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="J29" s="4"/>
       <c r="M29" s="6">
@@ -2142,24 +2229,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="B30">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="C30" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="D30" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="E30" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="F30" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="J30" s="4"/>
       <c r="M30" s="6">
@@ -2169,22 +2256,22 @@
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="B31">
         <v>3</v>
       </c>
       <c r="C31" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="D31" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="E31" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="F31" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="J31" s="4"/>
       <c r="M31" s="6">
@@ -2194,22 +2281,22 @@
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="B32">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C32" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="D32" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="E32" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="F32" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="J32" s="4"/>
       <c r="M32" s="6">
@@ -2219,22 +2306,22 @@
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="B33">
         <v>1</v>
       </c>
       <c r="C33" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="D33" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="E33" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="F33" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="J33" s="4"/>
       <c r="M33" s="6">
@@ -2244,22 +2331,22 @@
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="B34">
         <v>1</v>
       </c>
       <c r="C34" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="D34" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="E34" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="F34" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="J34" s="4"/>
       <c r="M34" s="6">
@@ -2269,22 +2356,22 @@
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="B35">
         <v>1</v>
       </c>
       <c r="C35" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="D35" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="E35" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="F35" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="J35" s="4"/>
       <c r="M35" s="6">
@@ -2294,22 +2381,22 @@
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="B36">
         <v>1</v>
       </c>
       <c r="C36" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="D36" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="E36" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="F36" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="J36" s="4"/>
       <c r="M36" s="6">
@@ -2319,22 +2406,22 @@
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="B37">
         <v>1</v>
       </c>
       <c r="C37" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="D37" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="E37" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="F37" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="J37" s="4"/>
       <c r="M37" s="6">
@@ -2342,154 +2429,140 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>114</v>
+        <v>162</v>
       </c>
       <c r="B38">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C38" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="D38" t="s">
-        <v>94</v>
+        <v>62</v>
       </c>
       <c r="E38" t="s">
-        <v>95</v>
+        <v>63</v>
       </c>
       <c r="F38" t="s">
-        <v>96</v>
-      </c>
-      <c r="J38" s="4"/>
+        <v>106</v>
+      </c>
+      <c r="G38" t="s">
+        <v>161</v>
+      </c>
+      <c r="H38" t="s">
+        <v>140</v>
+      </c>
+      <c r="I38" t="s">
+        <v>119</v>
+      </c>
+      <c r="J38" s="4">
+        <v>0.57699999999999996</v>
+      </c>
       <c r="M38" s="6">
         <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+        <v>5.1929999999999996</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="B39">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C39" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="D39" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="E39" t="s">
-        <v>72</v>
-      </c>
-      <c r="F39" t="s">
-        <v>118</v>
-      </c>
-      <c r="J39" s="4"/>
+        <v>109</v>
+      </c>
+      <c r="G39" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="H39" t="s">
+        <v>135</v>
+      </c>
+      <c r="I39" t="s">
+        <v>119</v>
+      </c>
+      <c r="J39" s="4">
+        <v>1.96</v>
+      </c>
       <c r="M39" s="6">
         <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
-        <v>0</v>
+        <v>5.88</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B40">
+        <v>1</v>
+      </c>
+      <c r="C40" t="s">
+        <v>111</v>
+      </c>
+      <c r="D40" t="s">
+        <v>111</v>
+      </c>
+      <c r="E40" t="s">
+        <v>112</v>
+      </c>
+      <c r="F40" t="s">
+        <v>113</v>
+      </c>
+      <c r="G40" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="H40" t="s">
+        <v>129</v>
+      </c>
+      <c r="I40" t="s">
         <v>119</v>
       </c>
-      <c r="B40">
-        <v>3</v>
-      </c>
-      <c r="C40" t="s">
-        <v>120</v>
-      </c>
-      <c r="D40" t="s">
-        <v>120</v>
-      </c>
-      <c r="E40" t="s">
-        <v>121</v>
-      </c>
-      <c r="G40" t="s">
-        <v>146</v>
-      </c>
-      <c r="H40" t="s">
-        <v>147</v>
-      </c>
-      <c r="I40" t="s">
-        <v>131</v>
-      </c>
       <c r="J40" s="4">
-        <v>1.96</v>
+        <v>0.81</v>
       </c>
       <c r="M40" s="6">
         <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
-        <v>5.88</v>
+        <v>0.81</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="B41">
         <v>1</v>
       </c>
       <c r="C41" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="D41" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="E41" t="s">
-        <v>124</v>
-      </c>
-      <c r="F41" t="s">
-        <v>125</v>
-      </c>
-      <c r="G41" s="3" t="s">
-        <v>126</v>
+        <v>117</v>
+      </c>
+      <c r="G41" t="s">
+        <v>130</v>
       </c>
       <c r="H41" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
       <c r="I41" t="s">
-        <v>131</v>
+        <v>119</v>
       </c>
       <c r="J41" s="4">
-        <v>0.81</v>
+        <v>9.61</v>
       </c>
       <c r="M41" s="6">
-        <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
-        <v>0.81</v>
-      </c>
-    </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A42" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="B42">
-        <v>1</v>
-      </c>
-      <c r="C42" t="s">
-        <v>128</v>
-      </c>
-      <c r="D42" t="s">
-        <v>128</v>
-      </c>
-      <c r="E42" t="s">
-        <v>129</v>
-      </c>
-      <c r="G42" t="s">
-        <v>142</v>
-      </c>
-      <c r="H42" t="s">
-        <v>143</v>
-      </c>
-      <c r="I42" t="s">
-        <v>131</v>
-      </c>
-      <c r="J42" s="4">
-        <v>9.61</v>
-      </c>
-      <c r="M42" s="6">
         <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
         <v>9.61</v>
       </c>
@@ -2497,14 +2570,18 @@
   </sheetData>
   <phoneticPr fontId="19" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="H24" r:id="rId1" xr:uid="{DD8AD352-FB06-4715-B587-8B7434FCD99F}"/>
-    <hyperlink ref="G26" r:id="rId2" xr:uid="{5EFE7EEC-7A33-4705-B297-C4BD3E05DA2C}"/>
-    <hyperlink ref="G41" r:id="rId3" xr:uid="{71FE485A-AA2E-4950-BE10-E132C884D307}"/>
+    <hyperlink ref="H23" r:id="rId1" xr:uid="{DD8AD352-FB06-4715-B587-8B7434FCD99F}"/>
+    <hyperlink ref="G25" r:id="rId2" xr:uid="{5EFE7EEC-7A33-4705-B297-C4BD3E05DA2C}"/>
+    <hyperlink ref="G40" r:id="rId3" xr:uid="{71FE485A-AA2E-4950-BE10-E132C884D307}"/>
     <hyperlink ref="K20" r:id="rId4" xr:uid="{DB18BABB-D85D-4D81-84B1-06B4803F7A71}"/>
+    <hyperlink ref="G17" r:id="rId5" xr:uid="{6E03D079-3A0C-4BF5-810D-97558264CB66}"/>
+    <hyperlink ref="G18" r:id="rId6" xr:uid="{7C702CAB-8E1E-429C-9A90-1E47838C9BF7}"/>
+    <hyperlink ref="G39" r:id="rId7" xr:uid="{ACFE634D-160F-4B71-8DB2-7FFC85727160}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId8"/>
   <tableParts count="1">
-    <tablePart r:id="rId5"/>
+    <tablePart r:id="rId9"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
This commit contains more ccomponent sourcing, mainly a diode array for the inhibitor logic diodes, handsoldering footprints have been chosen for some of the sourced components, see BOM, this should help us save time and frustration in handsoldering the testboard, SW connectors were reorganized to make better connections and now both side panels must be closed to connect the battery
</commit_message>
<xml_diff>
--- a/RADSAT-SK Timer/RADSAT-SK Timer.xlsx
+++ b/RADSAT-SK Timer/RADSAT-SK Timer.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\USST\power-and-electrical\RADSAT-SK Timer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4662F800-20E8-414A-B847-5AE9725A4C5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01E67C85-A19D-4B89-9F0D-C3DA7D52D1D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-3000" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="172">
   <si>
     <t>Source:</t>
   </si>
@@ -150,9 +150,6 @@
     <t>LED</t>
   </si>
   <si>
-    <t>LED_SMD:LED_0805_2012Metric</t>
-  </si>
-  <si>
     <t>Light emitting diode</t>
   </si>
   <si>
@@ -171,12 +168,6 @@
     <t xml:space="preserve">D203, </t>
   </si>
   <si>
-    <t xml:space="preserve">D204, D205, D206, </t>
-  </si>
-  <si>
-    <t>Diode</t>
-  </si>
-  <si>
     <t xml:space="preserve">J101, J103, </t>
   </si>
   <si>
@@ -246,18 +237,12 @@
     <t>L</t>
   </si>
   <si>
-    <t>Inductor_SMD:L_0805_2012Metric</t>
-  </si>
-  <si>
     <t xml:space="preserve">Q101, Q102, Q103, Q104, Q105, Q106, Q107, Q108, Q109, Q201, Q202, </t>
   </si>
   <si>
     <t>IRLML2060</t>
   </si>
   <si>
-    <t>Package_TO_SOT_SMD:SOT-23</t>
-  </si>
-  <si>
     <t>1.2A Id, 60V Vds, 480mOhm Rds, N-Channel HEXFET Power MOSFET, SOT-23</t>
   </si>
   <si>
@@ -360,9 +345,6 @@
     <t>LM397MF</t>
   </si>
   <si>
-    <t>Package_TO_SOT_SMD:TSOT-23-5</t>
-  </si>
-  <si>
     <t xml:space="preserve">U104, </t>
   </si>
   <si>
@@ -483,15 +465,6 @@
     <t>Diode_SMD:D_Powermite_AK</t>
   </si>
   <si>
-    <t>https://www.mccsemi.com/pdf/Products/SM5817PL-SM5819PL(SOD-123FL).PDF</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ca/en/products/detail/micro-commercial-co/SM5817PL-TP/1793251</t>
-  </si>
-  <si>
-    <t>SM5817PL-TP</t>
-  </si>
-  <si>
     <t>USB Connector</t>
   </si>
   <si>
@@ -541,6 +514,39 @@
   </si>
   <si>
     <t>10 µF ±20% 6.3V Ceramic Capacitor X5R 0805 (2012 Metric)</t>
+  </si>
+  <si>
+    <t>D204</t>
+  </si>
+  <si>
+    <t>BAT54CDW</t>
+  </si>
+  <si>
+    <t>Package_TO_SOT_SMD:SOT-363_SC-70-6_Handsoldering</t>
+  </si>
+  <si>
+    <t>Diode Array 2 Pair Common Cathode Schottky 30 V 200mA (DC) Surface Mount 6-TSSOP, SC-88, SOT-363</t>
+  </si>
+  <si>
+    <t>https://www.panjit.com.tw/upload/datasheet/BAT54TW_SERIES.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/panjit-international-inc/BAT54CDW-R1-00001/14660464</t>
+  </si>
+  <si>
+    <t>LED_SMD:LED_0603_1608Metric_Pad1.05x0.95mm_HandSolder</t>
+  </si>
+  <si>
+    <t>Package_TO_SOT_SMD:SOT-23_Handsoldering</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>Package_TO_SOT_SMD:TSOT-23-5_HandSoldering</t>
+  </si>
+  <si>
+    <t>**NONSTANDARD NEED TO CREATE***</t>
   </si>
 </sst>
 </file>
@@ -1049,7 +1055,7 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1059,6 +1065,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="42" applyFont="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="43" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="44">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1127,8 +1134,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A7:M41" totalsRowShown="0">
-  <autoFilter ref="A7:M41" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A7:M42" totalsRowShown="0">
+  <autoFilter ref="A7:M42" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Ref" dataDxfId="1"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Qnty"/>
@@ -1447,11 +1454,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O41"/>
+  <dimension ref="A1:O42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="F5" sqref="F5"/>
+      <selection pane="topRight" activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1483,7 +1490,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -1512,11 +1519,11 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="B6" s="6">
-        <f>SUM(M8:M41)</f>
-        <v>40.675999999999995</v>
+        <f>SUM(M8:M42)</f>
+        <v>39.275999999999996</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -1536,13 +1543,13 @@
         <v>12</v>
       </c>
       <c r="F7" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="G7" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="H7" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="I7" t="s">
         <v>13</v>
@@ -1551,13 +1558,13 @@
         <v>14</v>
       </c>
       <c r="K7" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="L7" s="4" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="M7" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
@@ -1652,16 +1659,16 @@
         <v>27</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="G11" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="H11" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="I11" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="J11" s="4">
         <v>0.41</v>
@@ -1735,19 +1742,19 @@
         <v>26</v>
       </c>
       <c r="E14" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="G14" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="H14" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="I14" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="J14" s="4">
         <v>1.0900000000000001</v>
@@ -1771,10 +1778,10 @@
         <v>38</v>
       </c>
       <c r="E15" t="s">
+        <v>167</v>
+      </c>
+      <c r="F15" t="s">
         <v>39</v>
-      </c>
-      <c r="F15" t="s">
-        <v>40</v>
       </c>
       <c r="J15" s="4"/>
       <c r="M15" s="6">
@@ -1784,22 +1791,22 @@
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B16">
         <v>1</v>
       </c>
       <c r="C16" t="s">
+        <v>41</v>
+      </c>
+      <c r="D16" t="s">
+        <v>41</v>
+      </c>
+      <c r="E16" t="s">
         <v>42</v>
       </c>
-      <c r="D16" t="s">
-        <v>42</v>
-      </c>
-      <c r="E16" t="s">
+      <c r="F16" t="s">
         <v>43</v>
-      </c>
-      <c r="F16" t="s">
-        <v>44</v>
       </c>
       <c r="J16" s="4"/>
       <c r="M16" s="6">
@@ -1809,31 +1816,31 @@
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B17">
         <v>1</v>
       </c>
       <c r="C17" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="D17" t="s">
+        <v>142</v>
+      </c>
+      <c r="E17" t="s">
+        <v>143</v>
+      </c>
+      <c r="F17" t="s">
         <v>148</v>
       </c>
-      <c r="E17" t="s">
-        <v>149</v>
-      </c>
-      <c r="F17" t="s">
-        <v>157</v>
-      </c>
       <c r="G17" s="3" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="H17" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="I17" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="J17" s="4">
         <v>0.76</v>
@@ -1845,58 +1852,58 @@
     </row>
     <row r="18" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>46</v>
+        <v>161</v>
       </c>
       <c r="B18">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>152</v>
+        <v>162</v>
       </c>
       <c r="D18" t="s">
-        <v>148</v>
+        <v>162</v>
       </c>
       <c r="E18" t="s">
-        <v>43</v>
+        <v>163</v>
       </c>
       <c r="F18" t="s">
-        <v>47</v>
+        <v>164</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>150</v>
+        <v>165</v>
       </c>
       <c r="H18" t="s">
-        <v>151</v>
+        <v>166</v>
       </c>
       <c r="I18" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="J18" s="4">
-        <v>0.65</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="M18" s="6">
         <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
-        <v>1.9500000000000002</v>
+        <v>0.55000000000000004</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B19">
         <v>2</v>
       </c>
       <c r="C19" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D19" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E19" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="F19" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="J19" s="4"/>
       <c r="M19" s="6">
@@ -1904,39 +1911,39 @@
         <v>0</v>
       </c>
       <c r="O19" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B20">
         <v>1</v>
       </c>
       <c r="C20" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D20" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E20" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="F20" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="H20" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="I20" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="J20" s="4">
         <v>0.61</v>
       </c>
       <c r="K20" s="3" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="L20" s="4">
         <v>0.52</v>
@@ -1946,36 +1953,36 @@
         <v>1.1299999999999999</v>
       </c>
       <c r="O20" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B21">
         <v>1</v>
       </c>
       <c r="C21" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D21" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E21" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="F21" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="G21" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="H21" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="I21" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="J21" s="4">
         <v>0.59299999999999997</v>
@@ -1987,22 +1994,22 @@
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B22">
         <v>1</v>
       </c>
       <c r="C22" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D22" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="E22" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="F22" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="J22" s="4"/>
       <c r="M22" s="6">
@@ -2010,33 +2017,33 @@
         <v>0</v>
       </c>
       <c r="O22" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B23">
         <v>1</v>
       </c>
       <c r="C23" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D23" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E23" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="F23" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="I23" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="J23" s="4">
         <v>1.76</v>
@@ -2048,31 +2055,31 @@
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B24">
         <v>1</v>
       </c>
       <c r="C24" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D24" t="s">
-        <v>70</v>
-      </c>
-      <c r="E24" t="s">
-        <v>71</v>
+        <v>67</v>
+      </c>
+      <c r="E24" s="7" t="s">
+        <v>171</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="G24" t="s">
-        <v>154</v>
-      </c>
-      <c r="H24" t="s">
-        <v>155</v>
+        <v>145</v>
+      </c>
+      <c r="H24" s="3" t="s">
+        <v>146</v>
       </c>
       <c r="I24" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="J24" s="4">
         <v>1.48</v>
@@ -2084,31 +2091,31 @@
     </row>
     <row r="25" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B25">
         <v>11</v>
       </c>
       <c r="C25" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="D25" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="E25" t="s">
-        <v>74</v>
+        <v>168</v>
       </c>
       <c r="F25" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="H25" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="I25" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="J25" s="4">
         <v>0.63</v>
@@ -2120,31 +2127,31 @@
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B26">
         <v>4</v>
       </c>
       <c r="C26" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="D26" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="E26" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="H26" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="I26" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="J26" s="4">
         <v>0.77</v>
@@ -2156,22 +2163,22 @@
     </row>
     <row r="27" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="B27">
         <v>10</v>
       </c>
       <c r="C27" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="D27" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="E27" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="F27" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="J27" s="4"/>
       <c r="M27" s="6">
@@ -2181,7 +2188,7 @@
     </row>
     <row r="28" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="B28">
         <v>12</v>
@@ -2190,13 +2197,13 @@
         <v>100</v>
       </c>
       <c r="D28" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="E28" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="F28" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="J28" s="4"/>
       <c r="M28" s="6">
@@ -2206,22 +2213,22 @@
     </row>
     <row r="29" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B29">
         <v>16</v>
       </c>
       <c r="C29" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="D29" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="E29" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="F29" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="J29" s="4"/>
       <c r="M29" s="6">
@@ -2231,22 +2238,22 @@
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="B30">
         <v>3</v>
       </c>
       <c r="C30" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="D30" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="E30" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="F30" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="J30" s="4"/>
       <c r="M30" s="6">
@@ -2256,22 +2263,22 @@
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="B31">
         <v>3</v>
       </c>
       <c r="C31" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="D31" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="E31" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="F31" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="J31" s="4"/>
       <c r="M31" s="6">
@@ -2281,22 +2288,22 @@
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="B32">
         <v>1</v>
       </c>
       <c r="C32" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="D32" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="E32" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="F32" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="J32" s="4"/>
       <c r="M32" s="6">
@@ -2306,22 +2313,22 @@
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="B33">
         <v>1</v>
       </c>
       <c r="C33" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="D33" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="E33" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="F33" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="J33" s="4"/>
       <c r="M33" s="6">
@@ -2331,22 +2338,22 @@
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="B34">
         <v>1</v>
       </c>
       <c r="C34" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="D34" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="E34" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="F34" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="J34" s="4"/>
       <c r="M34" s="6">
@@ -2356,22 +2363,22 @@
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="B35">
         <v>1</v>
       </c>
       <c r="C35" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="D35" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="E35" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="F35" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="J35" s="4"/>
       <c r="M35" s="6">
@@ -2381,22 +2388,22 @@
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="B36">
         <v>1</v>
       </c>
       <c r="C36" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="D36" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="E36" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="F36" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="J36" s="4"/>
       <c r="M36" s="6">
@@ -2406,22 +2413,22 @@
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="B37">
         <v>1</v>
       </c>
       <c r="C37" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="D37" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="E37" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="F37" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="J37" s="4"/>
       <c r="M37" s="6">
@@ -2431,31 +2438,31 @@
     </row>
     <row r="38" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="B38">
         <v>9</v>
       </c>
       <c r="C38" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="D38" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="E38" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="F38" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="G38" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="H38" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="I38" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="J38" s="4">
         <v>0.57699999999999996</v>
@@ -2467,28 +2474,28 @@
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="B39">
         <v>3</v>
       </c>
       <c r="C39" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="D39" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="E39" t="s">
-        <v>109</v>
+        <v>170</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="H39" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="I39" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="J39" s="4">
         <v>1.96</v>
@@ -2500,31 +2507,31 @@
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="B40">
         <v>1</v>
       </c>
       <c r="C40" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="D40" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="E40" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="F40" t="s">
+        <v>107</v>
+      </c>
+      <c r="G40" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="H40" t="s">
+        <v>123</v>
+      </c>
+      <c r="I40" t="s">
         <v>113</v>
-      </c>
-      <c r="G40" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="H40" t="s">
-        <v>129</v>
-      </c>
-      <c r="I40" t="s">
-        <v>119</v>
       </c>
       <c r="J40" s="4">
         <v>0.81</v>
@@ -2536,28 +2543,28 @@
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="B41">
         <v>1</v>
       </c>
       <c r="C41" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="D41" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="E41" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="G41" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="H41" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="I41" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="J41" s="4">
         <v>9.61</v>
@@ -2565,6 +2572,16 @@
       <c r="M41" s="6">
         <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
         <v>9.61</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E42" t="s">
+        <v>169</v>
+      </c>
+      <c r="J42" s="4"/>
+      <c r="M42" s="6">
+        <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2577,11 +2594,12 @@
     <hyperlink ref="G17" r:id="rId5" xr:uid="{6E03D079-3A0C-4BF5-810D-97558264CB66}"/>
     <hyperlink ref="G18" r:id="rId6" xr:uid="{7C702CAB-8E1E-429C-9A90-1E47838C9BF7}"/>
     <hyperlink ref="G39" r:id="rId7" xr:uid="{ACFE634D-160F-4B71-8DB2-7FFC85727160}"/>
+    <hyperlink ref="H24" r:id="rId8" xr:uid="{7C8D1661-4DCD-43AD-B870-FF77BABDB784}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId8"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId9"/>
   <tableParts count="1">
-    <tablePart r:id="rId9"/>
+    <tablePart r:id="rId10"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
actually did the other relays for the inhibits, played around with layout stuff
</commit_message>
<xml_diff>
--- a/RADSAT-SK Timer/RADSAT-SK Timer.xlsx
+++ b/RADSAT-SK Timer/RADSAT-SK Timer.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\USST\power-and-electrical\RADSAT-SK Timer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01E67C85-A19D-4B89-9F0D-C3DA7D52D1D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A28E265C-CDC4-4F18-8D80-529C66E8E711}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-3000" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="345" yWindow="735" windowWidth="16200" windowHeight="8265" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RADSAT-SK Timer" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="165">
   <si>
     <t>Source:</t>
   </si>
@@ -237,9 +237,6 @@
     <t>L</t>
   </si>
   <si>
-    <t xml:space="preserve">Q101, Q102, Q103, Q104, Q105, Q106, Q107, Q108, Q109, Q201, Q202, </t>
-  </si>
-  <si>
     <t>IRLML2060</t>
   </si>
   <si>
@@ -249,18 +246,6 @@
     <t>https://www.infineon.com/dgdl/irlml2060pbf.pdf?fileId=5546d462533600a401535664b7fb25ee</t>
   </si>
   <si>
-    <t xml:space="preserve">Q203, Q204, Q205, Q206, </t>
-  </si>
-  <si>
-    <t>PJFET</t>
-  </si>
-  <si>
-    <t>Q_PJFET_DGS</t>
-  </si>
-  <si>
-    <t>Package_TO_SOT_THT:TO-92L_Inline_Wide</t>
-  </si>
-  <si>
     <t xml:space="preserve">R101, R103, R107, R113, R114, R117, R118, R124, R126, R203, </t>
   </si>
   <si>
@@ -387,21 +372,12 @@
     <t>Related Components</t>
   </si>
   <si>
-    <t>https://www.digikey.ca/en/products/detail/onsemi/J176-D74Z/4213841</t>
-  </si>
-  <si>
-    <t>https://www.onsemi.com/pdf/datasheet/j175-d.pdf</t>
-  </si>
-  <si>
     <t>Datasheet</t>
   </si>
   <si>
     <t>https://www.digikey.ca/en/products/detail/infineon-technologies/irlml2060trpbf/2271899</t>
   </si>
   <si>
-    <t>P Channel JFET *product shortage on SMD components</t>
-  </si>
-  <si>
     <t>https://www.digikey.ca/en/products/detail/texas-instruments/CD4052BPWRG3/2596791</t>
   </si>
   <si>
@@ -547,6 +523,9 @@
   </si>
   <si>
     <t>**NONSTANDARD NEED TO CREATE***</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q101, Q102, Q103, Q104, Q105, Q106, Q107, Q108, Q109, Q201, Q202, Q203, Q204, Q205, Q206, </t>
   </si>
 </sst>
 </file>
@@ -556,7 +535,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -701,12 +680,6 @@
     </font>
     <font>
       <sz val="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1055,7 +1028,7 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1063,7 +1036,6 @@
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="43"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="42" applyFont="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="43" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
@@ -1134,8 +1106,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A7:M42" totalsRowShown="0">
-  <autoFilter ref="A7:M42" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A7:M41" totalsRowShown="0">
+  <autoFilter ref="A7:M41" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Ref" dataDxfId="1"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Qnty"/>
@@ -1454,11 +1426,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O42"/>
+  <dimension ref="A1:O41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E29" sqref="E29"/>
+      <selection pane="topRight" activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1490,7 +1462,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -1519,11 +1491,11 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="B6" s="6">
-        <f>SUM(M8:M42)</f>
-        <v>39.275999999999996</v>
+        <v>118</v>
+      </c>
+      <c r="B6" s="5">
+        <f>SUM(M8:M41)</f>
+        <v>38.715999999999994</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -1543,13 +1515,13 @@
         <v>12</v>
       </c>
       <c r="F7" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="G7" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="H7" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="I7" t="s">
         <v>13</v>
@@ -1558,13 +1530,13 @@
         <v>14</v>
       </c>
       <c r="K7" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="L7" s="4" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="M7" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
@@ -1587,7 +1559,7 @@
         <v>18</v>
       </c>
       <c r="J8" s="4"/>
-      <c r="M8" s="6">
+      <c r="M8" s="5">
         <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
         <v>0</v>
       </c>
@@ -1612,7 +1584,7 @@
         <v>23</v>
       </c>
       <c r="J9" s="4"/>
-      <c r="M9" s="6">
+      <c r="M9" s="5">
         <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
         <v>0</v>
       </c>
@@ -1637,7 +1609,7 @@
         <v>28</v>
       </c>
       <c r="J10" s="4"/>
-      <c r="M10" s="6">
+      <c r="M10" s="5">
         <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
         <v>0</v>
       </c>
@@ -1659,21 +1631,21 @@
         <v>27</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="G11" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="H11" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="I11" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="J11" s="4">
         <v>0.41</v>
       </c>
-      <c r="M11" s="6">
+      <c r="M11" s="5">
         <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
         <v>0.41</v>
       </c>
@@ -1698,7 +1670,7 @@
         <v>28</v>
       </c>
       <c r="J12" s="4"/>
-      <c r="M12" s="6">
+      <c r="M12" s="5">
         <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
         <v>0</v>
       </c>
@@ -1723,7 +1695,7 @@
         <v>28</v>
       </c>
       <c r="J13" s="4"/>
-      <c r="M13" s="6">
+      <c r="M13" s="5">
         <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
         <v>0</v>
       </c>
@@ -1742,24 +1714,24 @@
         <v>26</v>
       </c>
       <c r="E14" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="G14" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="H14" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="I14" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="J14" s="4">
         <v>1.0900000000000001</v>
       </c>
-      <c r="M14" s="6">
+      <c r="M14" s="5">
         <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
         <v>1.0900000000000001</v>
       </c>
@@ -1778,13 +1750,13 @@
         <v>38</v>
       </c>
       <c r="E15" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="F15" t="s">
         <v>39</v>
       </c>
       <c r="J15" s="4"/>
-      <c r="M15" s="6">
+      <c r="M15" s="5">
         <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
         <v>0</v>
       </c>
@@ -1809,7 +1781,7 @@
         <v>43</v>
       </c>
       <c r="J16" s="4"/>
-      <c r="M16" s="6">
+      <c r="M16" s="5">
         <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
         <v>0</v>
       </c>
@@ -1822,66 +1794,66 @@
         <v>1</v>
       </c>
       <c r="C17" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="D17" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="E17" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="F17" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="H17" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="I17" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="J17" s="4">
         <v>0.76</v>
       </c>
-      <c r="M17" s="6">
+      <c r="M17" s="5">
         <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
         <v>0.76</v>
       </c>
     </row>
     <row r="18" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="B18">
         <v>1</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="D18" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="E18" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="F18" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="H18" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="I18" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="J18" s="4">
         <v>0.55000000000000004</v>
       </c>
-      <c r="M18" s="6">
+      <c r="M18" s="5">
         <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
         <v>0.55000000000000004</v>
       </c>
@@ -1903,15 +1875,15 @@
         <v>47</v>
       </c>
       <c r="F19" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="J19" s="4"/>
-      <c r="M19" s="6">
+      <c r="M19" s="5">
         <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
         <v>0</v>
       </c>
       <c r="O19" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
@@ -1931,29 +1903,29 @@
         <v>50</v>
       </c>
       <c r="F20" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="H20" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="I20" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="J20" s="4">
         <v>0.61</v>
       </c>
       <c r="K20" s="3" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="L20" s="4">
         <v>0.52</v>
       </c>
-      <c r="M20" s="6">
+      <c r="M20" s="5">
         <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
         <v>1.1299999999999999</v>
       </c>
       <c r="O20" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
@@ -1976,18 +1948,18 @@
         <v>54</v>
       </c>
       <c r="G21" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="H21" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="I21" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="J21" s="4">
         <v>0.59299999999999997</v>
       </c>
-      <c r="M21" s="6">
+      <c r="M21" s="5">
         <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
         <v>0.59299999999999997</v>
       </c>
@@ -2012,12 +1984,12 @@
         <v>58</v>
       </c>
       <c r="J22" s="4"/>
-      <c r="M22" s="6">
+      <c r="M22" s="5">
         <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
         <v>0</v>
       </c>
       <c r="O22" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
@@ -2037,18 +2009,18 @@
         <v>63</v>
       </c>
       <c r="F23" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="H23" s="3" t="s">
         <v>64</v>
       </c>
       <c r="I23" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="J23" s="4">
         <v>1.76</v>
       </c>
-      <c r="M23" s="6">
+      <c r="M23" s="5">
         <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
         <v>1.76</v>
       </c>
@@ -2066,99 +2038,88 @@
       <c r="D24" t="s">
         <v>67</v>
       </c>
-      <c r="E24" s="7" t="s">
-        <v>171</v>
+      <c r="E24" s="6" t="s">
+        <v>163</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="G24" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="I24" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="J24" s="4">
         <v>1.48</v>
       </c>
-      <c r="M24" s="6">
+      <c r="M24" s="5">
         <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
         <v>1.48</v>
       </c>
     </row>
-    <row r="25" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="B25">
+        <v>15</v>
+      </c>
+      <c r="C25" t="s">
         <v>68</v>
       </c>
-      <c r="B25">
-        <v>11</v>
-      </c>
-      <c r="C25" t="s">
+      <c r="D25" t="s">
+        <v>68</v>
+      </c>
+      <c r="E25" t="s">
+        <v>160</v>
+      </c>
+      <c r="F25" t="s">
         <v>69</v>
       </c>
-      <c r="D25" t="s">
-        <v>69</v>
-      </c>
-      <c r="E25" t="s">
-        <v>168</v>
-      </c>
-      <c r="F25" t="s">
+      <c r="G25" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="G25" s="3" t="s">
-        <v>71</v>
-      </c>
       <c r="H25" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="I25" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="J25" s="4">
         <v>0.63</v>
       </c>
-      <c r="M25" s="6">
-        <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
-        <v>6.93</v>
-      </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M25" s="5">
+        <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
+        <v>9.4499999999999993</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B26">
+        <v>10</v>
+      </c>
+      <c r="C26" t="s">
         <v>72</v>
       </c>
-      <c r="B26">
-        <v>4</v>
-      </c>
-      <c r="C26" t="s">
+      <c r="D26" t="s">
         <v>73</v>
       </c>
-      <c r="D26" t="s">
+      <c r="E26" t="s">
         <v>74</v>
       </c>
-      <c r="E26" t="s">
+      <c r="F26" t="s">
         <v>75</v>
       </c>
-      <c r="F26" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="G26" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="H26" t="s">
-        <v>118</v>
-      </c>
-      <c r="I26" t="s">
-        <v>113</v>
-      </c>
-      <c r="J26" s="4">
-        <v>0.77</v>
-      </c>
-      <c r="M26" s="6">
-        <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
-        <v>3.08</v>
+      <c r="J26" s="4"/>
+      <c r="M26" s="5">
+        <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:15" ht="30" x14ac:dyDescent="0.25">
@@ -2166,343 +2127,354 @@
         <v>76</v>
       </c>
       <c r="B27">
-        <v>10</v>
-      </c>
-      <c r="C27" t="s">
+        <v>12</v>
+      </c>
+      <c r="C27">
+        <v>100</v>
+      </c>
+      <c r="D27" t="s">
+        <v>73</v>
+      </c>
+      <c r="E27" t="s">
+        <v>74</v>
+      </c>
+      <c r="F27" t="s">
+        <v>75</v>
+      </c>
+      <c r="J27" s="4"/>
+      <c r="M27" s="5">
+        <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="D27" t="s">
+      <c r="B28">
+        <v>16</v>
+      </c>
+      <c r="C28" t="s">
         <v>78</v>
       </c>
-      <c r="E27" t="s">
+      <c r="D28" t="s">
+        <v>73</v>
+      </c>
+      <c r="E28" t="s">
+        <v>74</v>
+      </c>
+      <c r="F28" t="s">
+        <v>75</v>
+      </c>
+      <c r="J28" s="4"/>
+      <c r="M28" s="5">
+        <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="F27" t="s">
+      <c r="B29">
+        <v>3</v>
+      </c>
+      <c r="C29" t="s">
         <v>80</v>
       </c>
-      <c r="J27" s="4"/>
-      <c r="M27" s="6">
-        <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="B28">
-        <v>12</v>
-      </c>
-      <c r="C28">
-        <v>100</v>
-      </c>
-      <c r="D28" t="s">
-        <v>78</v>
-      </c>
-      <c r="E28" t="s">
-        <v>79</v>
-      </c>
-      <c r="F28" t="s">
-        <v>80</v>
-      </c>
-      <c r="J28" s="4"/>
-      <c r="M28" s="6">
-        <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:15" ht="45" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="B29">
-        <v>16</v>
-      </c>
-      <c r="C29" t="s">
-        <v>83</v>
-      </c>
       <c r="D29" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="E29" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="F29" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="J29" s="4"/>
-      <c r="M29" s="6">
+      <c r="M29" s="5">
         <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
         <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B30">
         <v>3</v>
       </c>
       <c r="C30" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D30" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="E30" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="F30" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="J30" s="4"/>
-      <c r="M30" s="6">
+      <c r="M30" s="5">
         <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
         <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B31">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C31" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D31" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="E31" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="F31" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="J31" s="4"/>
-      <c r="M31" s="6">
+      <c r="M31" s="5">
         <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
         <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B32">
         <v>1</v>
       </c>
       <c r="C32" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="D32" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="E32" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="F32" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="J32" s="4"/>
-      <c r="M32" s="6">
+      <c r="M32" s="5">
         <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
         <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B33">
         <v>1</v>
       </c>
       <c r="C33" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D33" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="E33" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="F33" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="J33" s="4"/>
-      <c r="M33" s="6">
+      <c r="M33" s="5">
         <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
         <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B34">
         <v>1</v>
       </c>
       <c r="C34" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D34" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="E34" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="F34" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="J34" s="4"/>
-      <c r="M34" s="6">
+      <c r="M34" s="5">
         <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
         <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B35">
         <v>1</v>
       </c>
       <c r="C35" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D35" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="E35" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="F35" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="J35" s="4"/>
-      <c r="M35" s="6">
+      <c r="M35" s="5">
         <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
         <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B36">
         <v>1</v>
       </c>
       <c r="C36" t="s">
+        <v>94</v>
+      </c>
+      <c r="D36" t="s">
+        <v>73</v>
+      </c>
+      <c r="E36" t="s">
+        <v>74</v>
+      </c>
+      <c r="F36" t="s">
+        <v>75</v>
+      </c>
+      <c r="J36" s="4"/>
+      <c r="M36" s="5">
+        <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="B37">
+        <v>9</v>
+      </c>
+      <c r="C37" t="s">
+        <v>95</v>
+      </c>
+      <c r="D37" t="s">
+        <v>59</v>
+      </c>
+      <c r="E37" t="s">
+        <v>60</v>
+      </c>
+      <c r="F37" t="s">
+        <v>96</v>
+      </c>
+      <c r="G37" t="s">
+        <v>144</v>
+      </c>
+      <c r="H37" t="s">
+        <v>126</v>
+      </c>
+      <c r="I37" t="s">
+        <v>108</v>
+      </c>
+      <c r="J37" s="4">
+        <v>0.57699999999999996</v>
+      </c>
+      <c r="M37" s="5">
+        <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
+        <v>5.1929999999999996</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="D36" t="s">
-        <v>78</v>
-      </c>
-      <c r="E36" t="s">
-        <v>79</v>
-      </c>
-      <c r="F36" t="s">
-        <v>80</v>
-      </c>
-      <c r="J36" s="4"/>
-      <c r="M36" s="6">
-        <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A37" s="2" t="s">
+      <c r="B38">
+        <v>3</v>
+      </c>
+      <c r="C38" t="s">
         <v>98</v>
       </c>
-      <c r="B37">
-        <v>1</v>
-      </c>
-      <c r="C37" t="s">
-        <v>99</v>
-      </c>
-      <c r="D37" t="s">
-        <v>78</v>
-      </c>
-      <c r="E37" t="s">
-        <v>79</v>
-      </c>
-      <c r="F37" t="s">
-        <v>80</v>
-      </c>
-      <c r="J37" s="4"/>
-      <c r="M37" s="6">
-        <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A38" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="B38">
-        <v>9</v>
-      </c>
-      <c r="C38" t="s">
-        <v>100</v>
-      </c>
       <c r="D38" t="s">
-        <v>59</v>
+        <v>98</v>
       </c>
       <c r="E38" t="s">
-        <v>60</v>
-      </c>
-      <c r="F38" t="s">
-        <v>101</v>
-      </c>
-      <c r="G38" t="s">
-        <v>152</v>
+        <v>162</v>
+      </c>
+      <c r="G38" s="3" t="s">
+        <v>120</v>
       </c>
       <c r="H38" t="s">
-        <v>134</v>
+        <v>121</v>
       </c>
       <c r="I38" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="J38" s="4">
-        <v>0.57699999999999996</v>
-      </c>
-      <c r="M38" s="6">
-        <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
-        <v>5.1929999999999996</v>
+        <v>1.96</v>
+      </c>
+      <c r="M38" s="5">
+        <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
+        <v>5.88</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B39">
+        <v>1</v>
+      </c>
+      <c r="C39" t="s">
+        <v>100</v>
+      </c>
+      <c r="D39" t="s">
+        <v>100</v>
+      </c>
+      <c r="E39" t="s">
+        <v>101</v>
+      </c>
+      <c r="F39" t="s">
         <v>102</v>
       </c>
-      <c r="B39">
-        <v>3</v>
-      </c>
-      <c r="C39" t="s">
+      <c r="G39" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="D39" t="s">
-        <v>103</v>
-      </c>
-      <c r="E39" t="s">
-        <v>170</v>
-      </c>
-      <c r="G39" s="3" t="s">
-        <v>128</v>
-      </c>
       <c r="H39" t="s">
-        <v>129</v>
+        <v>115</v>
       </c>
       <c r="I39" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="J39" s="4">
-        <v>1.96</v>
-      </c>
-      <c r="M39" s="6">
-        <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
-        <v>5.88</v>
+        <v>0.81</v>
+      </c>
+      <c r="M39" s="5">
+        <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
+        <v>0.81</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
@@ -2521,65 +2493,29 @@
       <c r="E40" t="s">
         <v>106</v>
       </c>
-      <c r="F40" t="s">
-        <v>107</v>
-      </c>
-      <c r="G40" s="3" t="s">
+      <c r="G40" t="s">
+        <v>116</v>
+      </c>
+      <c r="H40" t="s">
+        <v>117</v>
+      </c>
+      <c r="I40" t="s">
         <v>108</v>
       </c>
-      <c r="H40" t="s">
-        <v>123</v>
-      </c>
-      <c r="I40" t="s">
-        <v>113</v>
-      </c>
       <c r="J40" s="4">
-        <v>0.81</v>
-      </c>
-      <c r="M40" s="6">
-        <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
-        <v>0.81</v>
+        <v>9.61</v>
+      </c>
+      <c r="M40" s="5">
+        <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
+        <v>9.61</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A41" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="B41">
-        <v>1</v>
-      </c>
-      <c r="C41" t="s">
-        <v>110</v>
-      </c>
-      <c r="D41" t="s">
-        <v>110</v>
-      </c>
       <c r="E41" t="s">
-        <v>111</v>
-      </c>
-      <c r="G41" t="s">
-        <v>124</v>
-      </c>
-      <c r="H41" t="s">
-        <v>125</v>
-      </c>
-      <c r="I41" t="s">
-        <v>113</v>
-      </c>
-      <c r="J41" s="4">
-        <v>9.61</v>
-      </c>
-      <c r="M41" s="6">
-        <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
-        <v>9.61</v>
-      </c>
-    </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="E42" t="s">
-        <v>169</v>
-      </c>
-      <c r="J42" s="4"/>
-      <c r="M42" s="6">
+        <v>161</v>
+      </c>
+      <c r="J41" s="4"/>
+      <c r="M41" s="5">
         <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
         <v>0</v>
       </c>
@@ -2589,11 +2525,11 @@
   <hyperlinks>
     <hyperlink ref="H23" r:id="rId1" xr:uid="{DD8AD352-FB06-4715-B587-8B7434FCD99F}"/>
     <hyperlink ref="G25" r:id="rId2" xr:uid="{5EFE7EEC-7A33-4705-B297-C4BD3E05DA2C}"/>
-    <hyperlink ref="G40" r:id="rId3" xr:uid="{71FE485A-AA2E-4950-BE10-E132C884D307}"/>
+    <hyperlink ref="G39" r:id="rId3" xr:uid="{71FE485A-AA2E-4950-BE10-E132C884D307}"/>
     <hyperlink ref="K20" r:id="rId4" xr:uid="{DB18BABB-D85D-4D81-84B1-06B4803F7A71}"/>
     <hyperlink ref="G17" r:id="rId5" xr:uid="{6E03D079-3A0C-4BF5-810D-97558264CB66}"/>
     <hyperlink ref="G18" r:id="rId6" xr:uid="{7C702CAB-8E1E-429C-9A90-1E47838C9BF7}"/>
-    <hyperlink ref="G39" r:id="rId7" xr:uid="{ACFE634D-160F-4B71-8DB2-7FFC85727160}"/>
+    <hyperlink ref="G38" r:id="rId7" xr:uid="{ACFE634D-160F-4B71-8DB2-7FFC85727160}"/>
     <hyperlink ref="H24" r:id="rId8" xr:uid="{7C8D1661-4DCD-43AD-B870-FF77BABDB784}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Adjusted the BOM to refelct previosu changes, made the 3d Model of the layout look good, swapped the antenna and the usb charger to other sides of the boards
</commit_message>
<xml_diff>
--- a/RADSAT-SK Timer/RADSAT-SK Timer.xlsx
+++ b/RADSAT-SK Timer/RADSAT-SK Timer.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\USST\power-and-electrical\RADSAT-SK Timer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A28E265C-CDC4-4F18-8D80-529C66E8E711}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44A376D5-2556-4214-9FFA-81CF2C196FAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="345" yWindow="735" windowWidth="16200" windowHeight="8265" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RADSAT-SK Timer" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="170">
   <si>
     <t>Source:</t>
   </si>
@@ -162,9 +162,6 @@
     <t>Diode_SMD:D_0805_2012Metric</t>
   </si>
   <si>
-    <t>Zener diode</t>
-  </si>
-  <si>
     <t xml:space="preserve">D203, </t>
   </si>
   <si>
@@ -261,12 +258,6 @@
     <t>Resistor</t>
   </si>
   <si>
-    <t xml:space="preserve">R102, R111, R115, R116, R133, R134, R202, R204, R209, R210, R211, R212, </t>
-  </si>
-  <si>
-    <t xml:space="preserve">R104, R108, R109, R110, R112, R119, R120, R127, R128, R129, R130, R131, R132, R135, R136, R138, </t>
-  </si>
-  <si>
     <t>1k</t>
   </si>
   <si>
@@ -321,9 +312,6 @@
     <t>SW_Push</t>
   </si>
   <si>
-    <t>Push button switch, generic, two pins</t>
-  </si>
-  <si>
     <t xml:space="preserve">U101, U102, U103, </t>
   </si>
   <si>
@@ -516,16 +504,43 @@
     <t>Package_TO_SOT_SMD:SOT-23_Handsoldering</t>
   </si>
   <si>
-    <t>e</t>
-  </si>
-  <si>
     <t>Package_TO_SOT_SMD:TSOT-23-5_HandSoldering</t>
   </si>
   <si>
     <t>**NONSTANDARD NEED TO CREATE***</t>
   </si>
   <si>
-    <t xml:space="preserve">Q101, Q102, Q103, Q104, Q105, Q106, Q107, Q108, Q109, Q201, Q202, Q203, Q204, Q205, Q206, </t>
+    <t>Connecotrs  for wires to 331XS4-T honeywell switch</t>
+  </si>
+  <si>
+    <t>U230,U240,U250,U260</t>
+  </si>
+  <si>
+    <t>CPC1117N</t>
+  </si>
+  <si>
+    <t>Package_SO:SOP-4_3.8x4.1mm_P2.54mm</t>
+  </si>
+  <si>
+    <t>https://www.ixysic.com/home/pdfs.nsf/www/CPC1106N.pdf/$file/CPC1106N.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/ixys-integrated-circuits-division/CPC1106NTR/3077493</t>
+  </si>
+  <si>
+    <t>Solid State SPST-NC (1 Form B) 4-SOP (0.150", 3.81mm)</t>
+  </si>
+  <si>
+    <t>R104, R108, R109, R110, R112, R119, R120, R127, R128, R129, R130, R131, R132, R135, R136, R138, R210,R212,R214,R216</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R102, R111, R115, R116, R133, R134, R202, R204, R209, R211, R213, R215, </t>
+  </si>
+  <si>
+    <t>Q101, Q102, Q103, Q104, Q105, Q106, Q107, Q108, Q109, Q201, Q202, Q203, Q204, Q205, Q206</t>
+  </si>
+  <si>
+    <t>5V Zener diode</t>
   </si>
 </sst>
 </file>
@@ -1428,9 +1443,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1447,6 +1462,7 @@
     <col min="10" max="10" width="7.7109375" customWidth="1"/>
     <col min="11" max="11" width="25" customWidth="1"/>
     <col min="12" max="12" width="9.140625" style="4"/>
+    <col min="13" max="13" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
@@ -1462,7 +1478,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -1491,11 +1507,11 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B6" s="5">
         <f>SUM(M8:M41)</f>
-        <v>38.715999999999994</v>
+        <v>45.555999999999997</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -1515,13 +1531,13 @@
         <v>12</v>
       </c>
       <c r="F7" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="G7" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="H7" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="I7" t="s">
         <v>13</v>
@@ -1530,13 +1546,13 @@
         <v>14</v>
       </c>
       <c r="K7" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="L7" s="4" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="M7" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
@@ -1631,16 +1647,16 @@
         <v>27</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="G11" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="H11" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="I11" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="J11" s="4">
         <v>0.41</v>
@@ -1714,19 +1730,19 @@
         <v>26</v>
       </c>
       <c r="E14" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="G14" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="H14" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="I14" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="J14" s="4">
         <v>1.0900000000000001</v>
@@ -1750,7 +1766,7 @@
         <v>38</v>
       </c>
       <c r="E15" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="F15" t="s">
         <v>39</v>
@@ -1778,7 +1794,7 @@
         <v>42</v>
       </c>
       <c r="F16" t="s">
-        <v>43</v>
+        <v>169</v>
       </c>
       <c r="J16" s="4"/>
       <c r="M16" s="5">
@@ -1788,31 +1804,31 @@
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B17">
         <v>1</v>
       </c>
       <c r="C17" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="D17" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="E17" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="F17" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="H17" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="I17" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="J17" s="4">
         <v>0.76</v>
@@ -1824,31 +1840,31 @@
     </row>
     <row r="18" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="B18">
         <v>1</v>
       </c>
       <c r="C18" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="D18" t="s">
+        <v>150</v>
+      </c>
+      <c r="E18" t="s">
+        <v>151</v>
+      </c>
+      <c r="F18" t="s">
+        <v>152</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="H18" t="s">
         <v>154</v>
       </c>
-      <c r="D18" t="s">
-        <v>154</v>
-      </c>
-      <c r="E18" t="s">
-        <v>155</v>
-      </c>
-      <c r="F18" t="s">
-        <v>156</v>
-      </c>
-      <c r="G18" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="H18" t="s">
-        <v>158</v>
-      </c>
       <c r="I18" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="J18" s="4">
         <v>0.55000000000000004</v>
@@ -1860,22 +1876,22 @@
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B19">
         <v>2</v>
       </c>
       <c r="C19" t="s">
+        <v>45</v>
+      </c>
+      <c r="D19" t="s">
+        <v>45</v>
+      </c>
+      <c r="E19" t="s">
         <v>46</v>
       </c>
-      <c r="D19" t="s">
-        <v>46</v>
-      </c>
-      <c r="E19" t="s">
-        <v>47</v>
-      </c>
       <c r="F19" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="J19" s="4"/>
       <c r="M19" s="5">
@@ -1883,39 +1899,39 @@
         <v>0</v>
       </c>
       <c r="O19" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B20">
         <v>1</v>
       </c>
       <c r="C20" t="s">
+        <v>48</v>
+      </c>
+      <c r="D20" t="s">
+        <v>48</v>
+      </c>
+      <c r="E20" t="s">
         <v>49</v>
       </c>
-      <c r="D20" t="s">
-        <v>49</v>
-      </c>
-      <c r="E20" t="s">
-        <v>50</v>
-      </c>
       <c r="F20" t="s">
-        <v>123</v>
-      </c>
-      <c r="H20" t="s">
-        <v>122</v>
+        <v>119</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>118</v>
       </c>
       <c r="I20" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="J20" s="4">
         <v>0.61</v>
       </c>
       <c r="K20" s="3" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="L20" s="4">
         <v>0.52</v>
@@ -1924,37 +1940,37 @@
         <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
         <v>1.1299999999999999</v>
       </c>
-      <c r="O20" t="s">
-        <v>124</v>
+      <c r="O20" s="3" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B21">
         <v>1</v>
       </c>
       <c r="C21" t="s">
+        <v>51</v>
+      </c>
+      <c r="D21" t="s">
+        <v>51</v>
+      </c>
+      <c r="E21" t="s">
         <v>52</v>
       </c>
-      <c r="D21" t="s">
-        <v>52</v>
-      </c>
-      <c r="E21" t="s">
+      <c r="F21" t="s">
         <v>53</v>
       </c>
-      <c r="F21" t="s">
-        <v>54</v>
-      </c>
       <c r="G21" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="H21" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="I21" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="J21" s="4">
         <v>0.59299999999999997</v>
@@ -1966,22 +1982,22 @@
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B22">
         <v>1</v>
       </c>
       <c r="C22" t="s">
+        <v>55</v>
+      </c>
+      <c r="D22" t="s">
+        <v>55</v>
+      </c>
+      <c r="E22" t="s">
         <v>56</v>
       </c>
-      <c r="D22" t="s">
-        <v>56</v>
-      </c>
-      <c r="E22" t="s">
+      <c r="F22" t="s">
         <v>57</v>
-      </c>
-      <c r="F22" t="s">
-        <v>58</v>
       </c>
       <c r="J22" s="4"/>
       <c r="M22" s="5">
@@ -1989,33 +2005,33 @@
         <v>0</v>
       </c>
       <c r="O22" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B23">
         <v>1</v>
       </c>
       <c r="C23" t="s">
+        <v>61</v>
+      </c>
+      <c r="D23" t="s">
+        <v>61</v>
+      </c>
+      <c r="E23" t="s">
         <v>62</v>
       </c>
-      <c r="D23" t="s">
-        <v>62</v>
-      </c>
-      <c r="E23" t="s">
+      <c r="F23" t="s">
+        <v>132</v>
+      </c>
+      <c r="H23" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="F23" t="s">
-        <v>136</v>
-      </c>
-      <c r="H23" s="3" t="s">
-        <v>64</v>
-      </c>
       <c r="I23" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="J23" s="4">
         <v>1.76</v>
@@ -2027,31 +2043,31 @@
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B24">
         <v>1</v>
       </c>
       <c r="C24" t="s">
+        <v>65</v>
+      </c>
+      <c r="D24" t="s">
         <v>66</v>
       </c>
-      <c r="D24" t="s">
-        <v>67</v>
-      </c>
       <c r="E24" s="6" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="G24" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="I24" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="J24" s="4">
         <v>1.48</v>
@@ -2063,31 +2079,31 @@
     </row>
     <row r="25" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="B25">
         <v>15</v>
       </c>
       <c r="C25" t="s">
+        <v>67</v>
+      </c>
+      <c r="D25" t="s">
+        <v>67</v>
+      </c>
+      <c r="E25" t="s">
+        <v>156</v>
+      </c>
+      <c r="F25" t="s">
         <v>68</v>
       </c>
-      <c r="D25" t="s">
-        <v>68</v>
-      </c>
-      <c r="E25" t="s">
-        <v>160</v>
-      </c>
-      <c r="F25" t="s">
+      <c r="G25" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="G25" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="H25" t="s">
-        <v>114</v>
+      <c r="H25" s="3" t="s">
+        <v>110</v>
       </c>
       <c r="I25" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="J25" s="4">
         <v>0.63</v>
@@ -2099,22 +2115,22 @@
     </row>
     <row r="26" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B26">
         <v>10</v>
       </c>
       <c r="C26" t="s">
+        <v>71</v>
+      </c>
+      <c r="D26" t="s">
         <v>72</v>
       </c>
-      <c r="D26" t="s">
+      <c r="E26" t="s">
         <v>73</v>
       </c>
-      <c r="E26" t="s">
+      <c r="F26" t="s">
         <v>74</v>
-      </c>
-      <c r="F26" t="s">
-        <v>75</v>
       </c>
       <c r="J26" s="4"/>
       <c r="M26" s="5">
@@ -2124,7 +2140,7 @@
     </row>
     <row r="27" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>76</v>
+        <v>167</v>
       </c>
       <c r="B27">
         <v>12</v>
@@ -2133,13 +2149,13 @@
         <v>100</v>
       </c>
       <c r="D27" t="s">
+        <v>72</v>
+      </c>
+      <c r="E27" t="s">
         <v>73</v>
       </c>
-      <c r="E27" t="s">
+      <c r="F27" t="s">
         <v>74</v>
-      </c>
-      <c r="F27" t="s">
-        <v>75</v>
       </c>
       <c r="J27" s="4"/>
       <c r="M27" s="5">
@@ -2149,22 +2165,22 @@
     </row>
     <row r="28" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>77</v>
+        <v>166</v>
       </c>
       <c r="B28">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C28" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D28" t="s">
+        <v>72</v>
+      </c>
+      <c r="E28" t="s">
         <v>73</v>
       </c>
-      <c r="E28" t="s">
+      <c r="F28" t="s">
         <v>74</v>
-      </c>
-      <c r="F28" t="s">
-        <v>75</v>
       </c>
       <c r="J28" s="4"/>
       <c r="M28" s="5">
@@ -2174,22 +2190,22 @@
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B29">
         <v>3</v>
       </c>
       <c r="C29" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D29" t="s">
+        <v>72</v>
+      </c>
+      <c r="E29" t="s">
         <v>73</v>
       </c>
-      <c r="E29" t="s">
+      <c r="F29" t="s">
         <v>74</v>
-      </c>
-      <c r="F29" t="s">
-        <v>75</v>
       </c>
       <c r="J29" s="4"/>
       <c r="M29" s="5">
@@ -2199,22 +2215,22 @@
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B30">
         <v>3</v>
       </c>
       <c r="C30" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D30" t="s">
+        <v>72</v>
+      </c>
+      <c r="E30" t="s">
         <v>73</v>
       </c>
-      <c r="E30" t="s">
+      <c r="F30" t="s">
         <v>74</v>
-      </c>
-      <c r="F30" t="s">
-        <v>75</v>
       </c>
       <c r="J30" s="4"/>
       <c r="M30" s="5">
@@ -2224,22 +2240,22 @@
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B31">
         <v>1</v>
       </c>
       <c r="C31" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D31" t="s">
+        <v>72</v>
+      </c>
+      <c r="E31" t="s">
         <v>73</v>
       </c>
-      <c r="E31" t="s">
+      <c r="F31" t="s">
         <v>74</v>
-      </c>
-      <c r="F31" t="s">
-        <v>75</v>
       </c>
       <c r="J31" s="4"/>
       <c r="M31" s="5">
@@ -2249,22 +2265,22 @@
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B32">
         <v>1</v>
       </c>
       <c r="C32" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D32" t="s">
+        <v>72</v>
+      </c>
+      <c r="E32" t="s">
         <v>73</v>
       </c>
-      <c r="E32" t="s">
+      <c r="F32" t="s">
         <v>74</v>
-      </c>
-      <c r="F32" t="s">
-        <v>75</v>
       </c>
       <c r="J32" s="4"/>
       <c r="M32" s="5">
@@ -2274,22 +2290,22 @@
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B33">
         <v>1</v>
       </c>
       <c r="C33" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D33" t="s">
+        <v>72</v>
+      </c>
+      <c r="E33" t="s">
         <v>73</v>
       </c>
-      <c r="E33" t="s">
+      <c r="F33" t="s">
         <v>74</v>
-      </c>
-      <c r="F33" t="s">
-        <v>75</v>
       </c>
       <c r="J33" s="4"/>
       <c r="M33" s="5">
@@ -2299,22 +2315,22 @@
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B34">
         <v>1</v>
       </c>
       <c r="C34" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D34" t="s">
+        <v>72</v>
+      </c>
+      <c r="E34" t="s">
         <v>73</v>
       </c>
-      <c r="E34" t="s">
+      <c r="F34" t="s">
         <v>74</v>
-      </c>
-      <c r="F34" t="s">
-        <v>75</v>
       </c>
       <c r="J34" s="4"/>
       <c r="M34" s="5">
@@ -2324,22 +2340,22 @@
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B35">
         <v>1</v>
       </c>
       <c r="C35" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D35" t="s">
+        <v>72</v>
+      </c>
+      <c r="E35" t="s">
         <v>73</v>
       </c>
-      <c r="E35" t="s">
+      <c r="F35" t="s">
         <v>74</v>
-      </c>
-      <c r="F35" t="s">
-        <v>75</v>
       </c>
       <c r="J35" s="4"/>
       <c r="M35" s="5">
@@ -2349,22 +2365,22 @@
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B36">
         <v>1</v>
       </c>
       <c r="C36" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D36" t="s">
+        <v>72</v>
+      </c>
+      <c r="E36" t="s">
         <v>73</v>
       </c>
-      <c r="E36" t="s">
+      <c r="F36" t="s">
         <v>74</v>
-      </c>
-      <c r="F36" t="s">
-        <v>75</v>
       </c>
       <c r="J36" s="4"/>
       <c r="M36" s="5">
@@ -2374,31 +2390,31 @@
     </row>
     <row r="37" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="B37">
         <v>9</v>
       </c>
       <c r="C37" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D37" t="s">
+        <v>58</v>
+      </c>
+      <c r="E37" t="s">
         <v>59</v>
       </c>
-      <c r="E37" t="s">
-        <v>60</v>
-      </c>
       <c r="F37" t="s">
-        <v>96</v>
+        <v>159</v>
       </c>
       <c r="G37" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="H37" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="I37" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="J37" s="4">
         <v>0.57699999999999996</v>
@@ -2410,28 +2426,28 @@
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B38">
         <v>3</v>
       </c>
       <c r="C38" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="D38" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="E38" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="H38" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="I38" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="J38" s="4">
         <v>1.96</v>
@@ -2443,31 +2459,31 @@
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="B39">
         <v>1</v>
       </c>
       <c r="C39" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="D39" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="E39" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="F39" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="H39" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="I39" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="J39" s="4">
         <v>0.81</v>
@@ -2479,28 +2495,28 @@
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B40">
         <v>1</v>
       </c>
       <c r="C40" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="D40" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="E40" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="G40" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="H40" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="I40" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="J40" s="4">
         <v>9.61</v>
@@ -2511,13 +2527,39 @@
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="B41">
+        <v>4</v>
+      </c>
+      <c r="C41" t="s">
+        <v>161</v>
+      </c>
+      <c r="D41" t="s">
+        <v>161</v>
+      </c>
       <c r="E41" t="s">
-        <v>161</v>
-      </c>
-      <c r="J41" s="4"/>
+        <v>162</v>
+      </c>
+      <c r="F41" t="s">
+        <v>165</v>
+      </c>
+      <c r="G41" t="s">
+        <v>163</v>
+      </c>
+      <c r="H41" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="I41" t="s">
+        <v>104</v>
+      </c>
+      <c r="J41" s="4">
+        <v>1.71</v>
+      </c>
       <c r="M41" s="5">
         <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
-        <v>0</v>
+        <v>6.84</v>
       </c>
     </row>
   </sheetData>
@@ -2531,11 +2573,15 @@
     <hyperlink ref="G18" r:id="rId6" xr:uid="{7C702CAB-8E1E-429C-9A90-1E47838C9BF7}"/>
     <hyperlink ref="G38" r:id="rId7" xr:uid="{ACFE634D-160F-4B71-8DB2-7FFC85727160}"/>
     <hyperlink ref="H24" r:id="rId8" xr:uid="{7C8D1661-4DCD-43AD-B870-FF77BABDB784}"/>
+    <hyperlink ref="H20" r:id="rId9" xr:uid="{257864EB-78CF-4B88-864D-5BF4D3EC4937}"/>
+    <hyperlink ref="O20" r:id="rId10" xr:uid="{438620CA-1198-495F-B2D1-DE18D03FD0CF}"/>
+    <hyperlink ref="H25" r:id="rId11" xr:uid="{50608FB6-E114-4108-91A8-FC7B919453D0}"/>
+    <hyperlink ref="H41" r:id="rId12" xr:uid="{8161F553-B981-424E-8CA4-DA1BB9415ECC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId9"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId13"/>
   <tableParts count="1">
-    <tablePart r:id="rId10"/>
+    <tablePart r:id="rId14"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Sourced coin cell battery and tantalum caps, still need to footprint coin cell holders
</commit_message>
<xml_diff>
--- a/RADSAT-SK Timer/RADSAT-SK Timer.xlsx
+++ b/RADSAT-SK Timer/RADSAT-SK Timer.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\USST\power-and-electrical\RADSAT-SK Timer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44A376D5-2556-4214-9FFA-81CF2C196FAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7475BC52-36B6-4081-992B-D67B2E143347}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-3000" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RADSAT-SK Timer" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="176">
   <si>
     <t>Source:</t>
   </si>
@@ -99,12 +99,6 @@
     <t>CP</t>
   </si>
   <si>
-    <t>Capacitor_Tantalum_SMD:CP_EIA-7343-31_Kemet-D</t>
-  </si>
-  <si>
-    <t>Polarized capacitor</t>
-  </si>
-  <si>
     <t xml:space="preserve">C103, C104, C109, C110, C111, C112, C113, C114, </t>
   </si>
   <si>
@@ -150,9 +144,6 @@
     <t>LED</t>
   </si>
   <si>
-    <t>Light emitting diode</t>
-  </si>
-  <si>
     <t xml:space="preserve">D201, </t>
   </si>
   <si>
@@ -541,6 +532,33 @@
   </si>
   <si>
     <t>5V Zener diode</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/stackpole-electronics-inc/RNCP0805FTD100R/2240209</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/kyocera-avx/F931A337KNC/4005190</t>
+  </si>
+  <si>
+    <t>330 µF Molded Tantalum Capacitors 10 V 2917 (7343 Metric) 500mOhm @ 100kHz</t>
+  </si>
+  <si>
+    <t>Capacitor_Tantalum_SMD:CP_EIA-7343-30_AVX-N_Pad2.25x2.55mm_HandSolder</t>
+  </si>
+  <si>
+    <t>Green 571nm LED Indication - Discrete 2V 0603 (1608 Metric)</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/lite-on-inc/LTST-C190KGKT/386815</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/Panasonic-Industrial-Devices/CR-2025-F2N?qs=FNor9lU6pf%2F%2FKr9xpq%252B%252BCQ%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/keystone-electronics/1061/303558</t>
+  </si>
+  <si>
+    <t>didkey/mouser</t>
   </si>
 </sst>
 </file>
@@ -1443,9 +1461,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="H1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="R10" sqref="R10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1478,7 +1496,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -1507,11 +1525,11 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B6" s="5">
         <f>SUM(M8:M41)</f>
-        <v>45.555999999999997</v>
+        <v>78.73</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -1531,13 +1549,13 @@
         <v>12</v>
       </c>
       <c r="F7" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="G7" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="H7" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="I7" t="s">
         <v>13</v>
@@ -1546,13 +1564,13 @@
         <v>14</v>
       </c>
       <c r="K7" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="L7" s="4" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="M7" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
@@ -1574,10 +1592,24 @@
       <c r="F8" t="s">
         <v>18</v>
       </c>
-      <c r="J8" s="4"/>
+      <c r="H8" t="s">
+        <v>174</v>
+      </c>
+      <c r="I8" t="s">
+        <v>175</v>
+      </c>
+      <c r="J8" s="4">
+        <v>4.09</v>
+      </c>
+      <c r="K8" t="s">
+        <v>173</v>
+      </c>
+      <c r="L8" s="4">
+        <v>1.61</v>
+      </c>
       <c r="M8" s="5">
         <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
-        <v>0</v>
+        <v>11.4</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
@@ -1594,35 +1626,43 @@
         <v>21</v>
       </c>
       <c r="E9" t="s">
-        <v>22</v>
+        <v>170</v>
       </c>
       <c r="F9" t="s">
-        <v>23</v>
-      </c>
-      <c r="J9" s="4"/>
+        <v>169</v>
+      </c>
+      <c r="H9" t="s">
+        <v>168</v>
+      </c>
+      <c r="I9" t="s">
+        <v>101</v>
+      </c>
+      <c r="J9" s="4">
+        <v>3.36</v>
+      </c>
       <c r="M9" s="5">
         <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
-        <v>0</v>
+        <v>20.16</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B10">
         <v>8</v>
       </c>
       <c r="C10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10" t="s">
         <v>25</v>
       </c>
-      <c r="D10" t="s">
+      <c r="F10" t="s">
         <v>26</v>
-      </c>
-      <c r="E10" t="s">
-        <v>27</v>
-      </c>
-      <c r="F10" t="s">
-        <v>28</v>
       </c>
       <c r="J10" s="4"/>
       <c r="M10" s="5">
@@ -1632,31 +1672,31 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B11">
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D11" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E11" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="G11" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="H11" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="I11" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="J11" s="4">
         <v>0.41</v>
@@ -1668,22 +1708,22 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B12">
         <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D12" t="s">
+        <v>24</v>
+      </c>
+      <c r="E12" t="s">
+        <v>25</v>
+      </c>
+      <c r="F12" t="s">
         <v>26</v>
-      </c>
-      <c r="E12" t="s">
-        <v>27</v>
-      </c>
-      <c r="F12" t="s">
-        <v>28</v>
       </c>
       <c r="J12" s="4"/>
       <c r="M12" s="5">
@@ -1693,22 +1733,22 @@
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B13">
         <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D13" t="s">
+        <v>24</v>
+      </c>
+      <c r="E13" t="s">
+        <v>25</v>
+      </c>
+      <c r="F13" t="s">
         <v>26</v>
-      </c>
-      <c r="E13" t="s">
-        <v>27</v>
-      </c>
-      <c r="F13" t="s">
-        <v>28</v>
       </c>
       <c r="J13" s="4"/>
       <c r="M13" s="5">
@@ -1718,31 +1758,31 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B14">
         <v>1</v>
       </c>
       <c r="C14" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D14" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E14" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="G14" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="H14" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="I14" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="J14" s="4">
         <v>1.0900000000000001</v>
@@ -1754,47 +1794,55 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B15">
         <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D15" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E15" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="F15" t="s">
-        <v>39</v>
-      </c>
-      <c r="J15" s="4"/>
+        <v>171</v>
+      </c>
+      <c r="H15" t="s">
+        <v>172</v>
+      </c>
+      <c r="I15" t="s">
+        <v>101</v>
+      </c>
+      <c r="J15" s="4">
+        <v>0.33</v>
+      </c>
       <c r="M15" s="5">
         <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
-        <v>0</v>
+        <v>0.33</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B16">
         <v>1</v>
       </c>
       <c r="C16" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D16" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E16" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F16" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="J16" s="4"/>
       <c r="M16" s="5">
@@ -1804,31 +1852,31 @@
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B17">
         <v>1</v>
       </c>
       <c r="C17" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="D17" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="E17" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="F17" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="H17" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="I17" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="J17" s="4">
         <v>0.76</v>
@@ -1840,31 +1888,31 @@
     </row>
     <row r="18" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B18">
         <v>1</v>
       </c>
       <c r="C18" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="D18" t="s">
+        <v>147</v>
+      </c>
+      <c r="E18" t="s">
+        <v>148</v>
+      </c>
+      <c r="F18" t="s">
+        <v>149</v>
+      </c>
+      <c r="G18" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="D18" t="s">
-        <v>150</v>
-      </c>
-      <c r="E18" t="s">
+      <c r="H18" t="s">
         <v>151</v>
       </c>
-      <c r="F18" t="s">
-        <v>152</v>
-      </c>
-      <c r="G18" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="H18" t="s">
-        <v>154</v>
-      </c>
       <c r="I18" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="J18" s="4">
         <v>0.55000000000000004</v>
@@ -1876,22 +1924,22 @@
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B19">
         <v>2</v>
       </c>
       <c r="C19" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D19" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E19" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="F19" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="J19" s="4"/>
       <c r="M19" s="5">
@@ -1899,39 +1947,39 @@
         <v>0</v>
       </c>
       <c r="O19" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B20">
         <v>1</v>
       </c>
       <c r="C20" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D20" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E20" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="F20" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="I20" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="J20" s="4">
         <v>0.61</v>
       </c>
       <c r="K20" s="3" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="L20" s="4">
         <v>0.52</v>
@@ -1941,36 +1989,36 @@
         <v>1.1299999999999999</v>
       </c>
       <c r="O20" s="3" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B21">
         <v>1</v>
       </c>
       <c r="C21" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D21" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E21" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="F21" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="G21" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="H21" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="I21" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="J21" s="4">
         <v>0.59299999999999997</v>
@@ -1982,22 +2030,22 @@
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B22">
         <v>1</v>
       </c>
       <c r="C22" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D22" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E22" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="F22" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="J22" s="4"/>
       <c r="M22" s="5">
@@ -2005,33 +2053,33 @@
         <v>0</v>
       </c>
       <c r="O22" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B23">
         <v>1</v>
       </c>
       <c r="C23" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D23" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E23" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="F23" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="I23" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="J23" s="4">
         <v>1.76</v>
@@ -2043,31 +2091,31 @@
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B24">
         <v>1</v>
       </c>
       <c r="C24" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D24" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="G24" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="I24" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="J24" s="4">
         <v>1.48</v>
@@ -2079,31 +2127,31 @@
     </row>
     <row r="25" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B25">
         <v>15</v>
       </c>
       <c r="C25" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D25" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E25" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="F25" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="I25" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="J25" s="4">
         <v>0.63</v>
@@ -2115,22 +2163,22 @@
     </row>
     <row r="26" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B26">
         <v>10</v>
       </c>
       <c r="C26" t="s">
+        <v>68</v>
+      </c>
+      <c r="D26" t="s">
+        <v>69</v>
+      </c>
+      <c r="E26" t="s">
+        <v>70</v>
+      </c>
+      <c r="F26" t="s">
         <v>71</v>
-      </c>
-      <c r="D26" t="s">
-        <v>72</v>
-      </c>
-      <c r="E26" t="s">
-        <v>73</v>
-      </c>
-      <c r="F26" t="s">
-        <v>74</v>
       </c>
       <c r="J26" s="4"/>
       <c r="M26" s="5">
@@ -2140,7 +2188,7 @@
     </row>
     <row r="27" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B27">
         <v>12</v>
@@ -2149,38 +2197,46 @@
         <v>100</v>
       </c>
       <c r="D27" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E27" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="F27" t="s">
-        <v>74</v>
-      </c>
-      <c r="J27" s="4"/>
+        <v>71</v>
+      </c>
+      <c r="H27" t="s">
+        <v>167</v>
+      </c>
+      <c r="I27" t="s">
+        <v>101</v>
+      </c>
+      <c r="J27" s="4">
+        <v>0.107</v>
+      </c>
       <c r="M27" s="5">
         <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
-        <v>0</v>
+        <v>1.284</v>
       </c>
     </row>
     <row r="28" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="B28">
         <v>20</v>
       </c>
       <c r="C28" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D28" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E28" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="F28" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="J28" s="4"/>
       <c r="M28" s="5">
@@ -2190,22 +2246,22 @@
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B29">
         <v>3</v>
       </c>
       <c r="C29" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D29" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E29" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="F29" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="J29" s="4"/>
       <c r="M29" s="5">
@@ -2215,22 +2271,22 @@
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B30">
         <v>3</v>
       </c>
       <c r="C30" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="D30" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E30" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="F30" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="J30" s="4"/>
       <c r="M30" s="5">
@@ -2240,22 +2296,22 @@
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B31">
         <v>1</v>
       </c>
       <c r="C31" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D31" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E31" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="F31" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="J31" s="4"/>
       <c r="M31" s="5">
@@ -2265,22 +2321,22 @@
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B32">
         <v>1</v>
       </c>
       <c r="C32" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D32" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E32" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="F32" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="J32" s="4"/>
       <c r="M32" s="5">
@@ -2290,22 +2346,22 @@
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B33">
         <v>1</v>
       </c>
       <c r="C33" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D33" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E33" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="F33" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="J33" s="4"/>
       <c r="M33" s="5">
@@ -2315,22 +2371,22 @@
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B34">
         <v>1</v>
       </c>
       <c r="C34" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D34" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E34" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="F34" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="J34" s="4"/>
       <c r="M34" s="5">
@@ -2340,22 +2396,22 @@
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B35">
         <v>1</v>
       </c>
       <c r="C35" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="D35" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E35" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="F35" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="J35" s="4"/>
       <c r="M35" s="5">
@@ -2365,22 +2421,22 @@
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B36">
         <v>1</v>
       </c>
       <c r="C36" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D36" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E36" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="F36" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="J36" s="4"/>
       <c r="M36" s="5">
@@ -2390,31 +2446,31 @@
     </row>
     <row r="37" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B37">
         <v>9</v>
       </c>
       <c r="C37" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D37" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="E37" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="F37" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="G37" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="H37" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="I37" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="J37" s="4">
         <v>0.57699999999999996</v>
@@ -2426,28 +2482,28 @@
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B38">
         <v>3</v>
       </c>
       <c r="C38" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D38" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="E38" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="H38" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="I38" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="J38" s="4">
         <v>1.96</v>
@@ -2459,31 +2515,31 @@
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B39">
         <v>1</v>
       </c>
       <c r="C39" t="s">
+        <v>93</v>
+      </c>
+      <c r="D39" t="s">
+        <v>93</v>
+      </c>
+      <c r="E39" t="s">
+        <v>94</v>
+      </c>
+      <c r="F39" t="s">
+        <v>95</v>
+      </c>
+      <c r="G39" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="D39" t="s">
-        <v>96</v>
-      </c>
-      <c r="E39" t="s">
-        <v>97</v>
-      </c>
-      <c r="F39" t="s">
-        <v>98</v>
-      </c>
-      <c r="G39" s="3" t="s">
-        <v>99</v>
-      </c>
       <c r="H39" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="I39" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="J39" s="4">
         <v>0.81</v>
@@ -2495,28 +2551,28 @@
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B40">
         <v>1</v>
       </c>
       <c r="C40" t="s">
+        <v>98</v>
+      </c>
+      <c r="D40" t="s">
+        <v>98</v>
+      </c>
+      <c r="E40" t="s">
+        <v>99</v>
+      </c>
+      <c r="G40" t="s">
+        <v>109</v>
+      </c>
+      <c r="H40" t="s">
+        <v>110</v>
+      </c>
+      <c r="I40" t="s">
         <v>101</v>
-      </c>
-      <c r="D40" t="s">
-        <v>101</v>
-      </c>
-      <c r="E40" t="s">
-        <v>102</v>
-      </c>
-      <c r="G40" t="s">
-        <v>112</v>
-      </c>
-      <c r="H40" t="s">
-        <v>113</v>
-      </c>
-      <c r="I40" t="s">
-        <v>104</v>
       </c>
       <c r="J40" s="4">
         <v>9.61</v>
@@ -2528,31 +2584,31 @@
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="B41">
         <v>4</v>
       </c>
       <c r="C41" t="s">
+        <v>158</v>
+      </c>
+      <c r="D41" t="s">
+        <v>158</v>
+      </c>
+      <c r="E41" t="s">
+        <v>159</v>
+      </c>
+      <c r="F41" t="s">
+        <v>162</v>
+      </c>
+      <c r="G41" t="s">
+        <v>160</v>
+      </c>
+      <c r="H41" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="D41" t="s">
-        <v>161</v>
-      </c>
-      <c r="E41" t="s">
-        <v>162</v>
-      </c>
-      <c r="F41" t="s">
-        <v>165</v>
-      </c>
-      <c r="G41" t="s">
-        <v>163</v>
-      </c>
-      <c r="H41" s="3" t="s">
-        <v>164</v>
-      </c>
       <c r="I41" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="J41" s="4">
         <v>1.71</v>

</xml_diff>

<commit_message>
the RBF relay transistor was redundant, added in another LED and updated diode configuration, resistor sourcing TBD
</commit_message>
<xml_diff>
--- a/RADSAT-SK Timer/RADSAT-SK Timer.xlsx
+++ b/RADSAT-SK Timer/RADSAT-SK Timer.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\USST\power-and-electrical\RADSAT-SK Timer\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\riley\USST\RADSAT-SK\power-and-electrical\RADSAT-SK Timer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7475BC52-36B6-4081-992B-D67B2E143347}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7651C43F-B578-4695-A081-92386930BC72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-3000" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RADSAT-SK Timer" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="188">
   <si>
     <t>Source:</t>
   </si>
@@ -84,12 +84,6 @@
     <t>Battery_Cell</t>
   </si>
   <si>
-    <t>Battery:BatteryHolder_Keystone_1060_1x2032</t>
-  </si>
-  <si>
-    <t>Single-cell battery</t>
-  </si>
-  <si>
     <t xml:space="preserve">C101, C102, C105, C106, C107, C108, </t>
   </si>
   <si>
@@ -138,9 +132,6 @@
     <t>22uF</t>
   </si>
   <si>
-    <t xml:space="preserve">D101, </t>
-  </si>
-  <si>
     <t>LED</t>
   </si>
   <si>
@@ -150,9 +141,6 @@
     <t>D_Zener</t>
   </si>
   <si>
-    <t>Diode_SMD:D_0805_2012Metric</t>
-  </si>
-  <si>
     <t xml:space="preserve">D203, </t>
   </si>
   <si>
@@ -273,9 +261,6 @@
     <t xml:space="preserve">R201, </t>
   </si>
   <si>
-    <t>300k</t>
-  </si>
-  <si>
     <t xml:space="preserve">R205, </t>
   </si>
   <si>
@@ -522,18 +507,6 @@
     <t>Solid State SPST-NC (1 Form B) 4-SOP (0.150", 3.81mm)</t>
   </si>
   <si>
-    <t>R104, R108, R109, R110, R112, R119, R120, R127, R128, R129, R130, R131, R132, R135, R136, R138, R210,R212,R214,R216</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R102, R111, R115, R116, R133, R134, R202, R204, R209, R211, R213, R215, </t>
-  </si>
-  <si>
-    <t>Q101, Q102, Q103, Q104, Q105, Q106, Q107, Q108, Q109, Q201, Q202, Q203, Q204, Q205, Q206</t>
-  </si>
-  <si>
-    <t>5V Zener diode</t>
-  </si>
-  <si>
     <t>https://www.digikey.ca/en/products/detail/stackpole-electronics-inc/RNCP0805FTD100R/2240209</t>
   </si>
   <si>
@@ -559,6 +532,82 @@
   </si>
   <si>
     <t>didkey/mouser</t>
+  </si>
+  <si>
+    <t>BATT HLDR COIN 20MM 1/2 CEL SMD</t>
+  </si>
+  <si>
+    <t>https://www.keyelco.com/userAssets/file/M65p3.pdf</t>
+  </si>
+  <si>
+    <t>SSR_SPST-NC</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/bourns-inc/5-0SMDJ5-0A/9341763</t>
+  </si>
+  <si>
+    <t>https://www.bourns.com/docs/product-datasheets/5-0smdj.pdf</t>
+  </si>
+  <si>
+    <t>5.0SMDJ5.0A</t>
+  </si>
+  <si>
+    <t>9.2V Clamp 543.6A Ipp Tvs Diode Surface Mount DO-214AB (SMC)</t>
+  </si>
+  <si>
+    <t>3M</t>
+  </si>
+  <si>
+    <r>
+      <t>Battery:BatteryHolder_Keystone_1060_1x2032</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>*** NEED TO EDIT***</t>
+    </r>
+  </si>
+  <si>
+    <t>Diode_SMD:D_SMC_Handsoldering</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Buck-Boost Switching Regulator IC Positive Adjustable 2.5V 1 Output 600mA </t>
+  </si>
+  <si>
+    <t>Q101, Q102, Q103, Q104, Q105, Q106, Q107, Q108, Q109, Q201, Q202, Q204, Q205, Q206</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R102, R111, R115, R116, R133, R134, R202, R204, R211, R213, R215, </t>
+  </si>
+  <si>
+    <t>D206</t>
+  </si>
+  <si>
+    <t>D205</t>
+  </si>
+  <si>
+    <t>Orange 605nm LED Indication - Discrete 2V 0603 (1608 Metric)</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/lite-on-inc/LTST-C191KFKT/386833</t>
+  </si>
+  <si>
+    <t>https://optoelectronics.liteon.com/upload/download/DS22-2000-074/LTST-C190KGKT.PDF</t>
+  </si>
+  <si>
+    <t>R104, R108, R109, R110, R112, R119, R120, R127, R128, R129, R130, R131, R132, R135, R136, R209,  R210, R212, R214, R216, R217</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/stackpole-electronics-inc/RMCF0805JT1M00/1757878</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/stackpole-electronics-inc/RMCF0805JT1K00/1757881</t>
   </si>
 </sst>
 </file>
@@ -566,7 +615,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="20" x14ac:knownFonts="1">
     <font>
@@ -1058,7 +1107,7 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="7">
@@ -1068,8 +1117,8 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="43"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="42" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="42" applyFont="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="44">
@@ -1120,7 +1169,7 @@
   </cellStyles>
   <dxfs count="2">
     <dxf>
-      <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1139,8 +1188,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A7:M41" totalsRowShown="0">
-  <autoFilter ref="A7:M41" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A7:M42" totalsRowShown="0">
+  <autoFilter ref="A7:M42" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Ref" dataDxfId="1"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Qnty"/>
@@ -1459,11 +1508,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O41"/>
+  <dimension ref="A1:O42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="H1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="R10" sqref="R10"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="J29" sqref="J29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1496,7 +1545,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -1525,11 +1574,11 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="B6" s="5">
-        <f>SUM(M8:M41)</f>
-        <v>78.73</v>
+        <f>SUM(M8:M42)</f>
+        <v>81.551999999999992</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -1549,13 +1598,13 @@
         <v>12</v>
       </c>
       <c r="F7" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="G7" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="H7" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="I7" t="s">
         <v>13</v>
@@ -1564,13 +1613,13 @@
         <v>14</v>
       </c>
       <c r="K7" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="L7" s="4" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="M7" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
@@ -1587,22 +1636,25 @@
         <v>16</v>
       </c>
       <c r="E8" t="s">
-        <v>17</v>
+        <v>175</v>
       </c>
       <c r="F8" t="s">
-        <v>18</v>
-      </c>
-      <c r="H8" t="s">
-        <v>174</v>
+        <v>167</v>
+      </c>
+      <c r="G8" t="s">
+        <v>168</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>165</v>
       </c>
       <c r="I8" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="J8" s="4">
         <v>4.09</v>
       </c>
-      <c r="K8" t="s">
-        <v>173</v>
+      <c r="K8" s="3" t="s">
+        <v>164</v>
       </c>
       <c r="L8" s="4">
         <v>1.61</v>
@@ -1614,28 +1666,28 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B9">
         <v>6</v>
       </c>
       <c r="C9" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D9" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E9" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="F9" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="H9" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="I9" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="J9" s="4">
         <v>3.36</v>
@@ -1647,22 +1699,22 @@
     </row>
     <row r="10" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B10">
         <v>8</v>
       </c>
       <c r="C10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10" t="s">
         <v>23</v>
       </c>
-      <c r="D10" t="s">
+      <c r="F10" t="s">
         <v>24</v>
-      </c>
-      <c r="E10" t="s">
-        <v>25</v>
-      </c>
-      <c r="F10" t="s">
-        <v>26</v>
       </c>
       <c r="J10" s="4"/>
       <c r="M10" s="5">
@@ -1672,31 +1724,31 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B11">
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D11" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E11" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="G11" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="H11" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="I11" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="J11" s="4">
         <v>0.41</v>
@@ -1708,22 +1760,22 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B12">
         <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D12" t="s">
+        <v>22</v>
+      </c>
+      <c r="E12" t="s">
+        <v>23</v>
+      </c>
+      <c r="F12" t="s">
         <v>24</v>
-      </c>
-      <c r="E12" t="s">
-        <v>25</v>
-      </c>
-      <c r="F12" t="s">
-        <v>26</v>
       </c>
       <c r="J12" s="4"/>
       <c r="M12" s="5">
@@ -1733,22 +1785,22 @@
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B13">
         <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D13" t="s">
+        <v>22</v>
+      </c>
+      <c r="E13" t="s">
+        <v>23</v>
+      </c>
+      <c r="F13" t="s">
         <v>24</v>
-      </c>
-      <c r="E13" t="s">
-        <v>25</v>
-      </c>
-      <c r="F13" t="s">
-        <v>26</v>
       </c>
       <c r="J13" s="4"/>
       <c r="M13" s="5">
@@ -1758,31 +1810,31 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B14">
         <v>1</v>
       </c>
       <c r="C14" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D14" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E14" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="G14" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="H14" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="I14" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="J14" s="4">
         <v>1.0900000000000001</v>
@@ -1794,28 +1846,31 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>35</v>
+        <v>181</v>
       </c>
       <c r="B15">
         <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D15" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E15" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="F15" t="s">
-        <v>171</v>
-      </c>
-      <c r="H15" t="s">
-        <v>172</v>
+        <v>162</v>
+      </c>
+      <c r="G15" t="s">
+        <v>184</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>163</v>
       </c>
       <c r="I15" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="J15" s="4">
         <v>0.33</v>
@@ -1827,466 +1882,501 @@
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>37</v>
+        <v>180</v>
       </c>
       <c r="B16">
         <v>1</v>
       </c>
       <c r="C16" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="D16" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="E16" t="s">
-        <v>39</v>
+        <v>147</v>
       </c>
       <c r="F16" t="s">
-        <v>166</v>
-      </c>
-      <c r="J16" s="4"/>
+        <v>182</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="I16" t="s">
+        <v>96</v>
+      </c>
+      <c r="J16" s="4">
+        <v>0.33</v>
+      </c>
       <c r="M16" s="5">
         <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
-        <v>0</v>
+        <v>0.33</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B17">
         <v>1</v>
       </c>
       <c r="C17" t="s">
-        <v>126</v>
+        <v>172</v>
       </c>
       <c r="D17" t="s">
-        <v>127</v>
+        <v>35</v>
       </c>
       <c r="E17" t="s">
-        <v>128</v>
+        <v>176</v>
       </c>
       <c r="F17" t="s">
-        <v>133</v>
+        <v>173</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>124</v>
+        <v>171</v>
       </c>
       <c r="H17" t="s">
-        <v>125</v>
+        <v>170</v>
       </c>
       <c r="I17" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="J17" s="4">
-        <v>0.76</v>
+        <v>2.33</v>
       </c>
       <c r="M17" s="5">
         <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
-        <v>0.76</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>2.33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>146</v>
+        <v>36</v>
       </c>
       <c r="B18">
         <v>1</v>
       </c>
-      <c r="C18" s="2" t="s">
-        <v>147</v>
+      <c r="C18" t="s">
+        <v>121</v>
       </c>
       <c r="D18" t="s">
-        <v>147</v>
+        <v>122</v>
       </c>
       <c r="E18" t="s">
-        <v>148</v>
+        <v>123</v>
       </c>
       <c r="F18" t="s">
-        <v>149</v>
+        <v>128</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>150</v>
+        <v>119</v>
       </c>
       <c r="H18" t="s">
-        <v>151</v>
+        <v>120</v>
       </c>
       <c r="I18" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="J18" s="4">
+        <v>0.76</v>
+      </c>
+      <c r="M18" s="5">
+        <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
+        <v>0.76</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="D19" t="s">
+        <v>142</v>
+      </c>
+      <c r="E19" t="s">
+        <v>143</v>
+      </c>
+      <c r="F19" t="s">
+        <v>144</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="H19" t="s">
+        <v>146</v>
+      </c>
+      <c r="I19" t="s">
+        <v>96</v>
+      </c>
+      <c r="J19" s="4">
         <v>0.55000000000000004</v>
       </c>
-      <c r="M18" s="5">
+      <c r="M19" s="5">
         <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
         <v>0.55000000000000004</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="B19">
-        <v>2</v>
-      </c>
-      <c r="C19" t="s">
-        <v>42</v>
-      </c>
-      <c r="D19" t="s">
-        <v>42</v>
-      </c>
-      <c r="E19" t="s">
-        <v>43</v>
-      </c>
-      <c r="F19" t="s">
-        <v>136</v>
-      </c>
-      <c r="J19" s="4"/>
-      <c r="M19" s="5">
-        <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
-        <v>0</v>
-      </c>
-      <c r="O19" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="B20">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C20" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="D20" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="E20" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="F20" t="s">
-        <v>116</v>
-      </c>
-      <c r="H20" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="I20" t="s">
-        <v>101</v>
-      </c>
-      <c r="J20" s="4">
-        <v>0.61</v>
-      </c>
-      <c r="K20" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="L20" s="4">
-        <v>0.52</v>
-      </c>
+        <v>131</v>
+      </c>
+      <c r="J20" s="4"/>
       <c r="M20" s="5">
         <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
-        <v>1.1299999999999999</v>
-      </c>
-      <c r="O20" s="3" t="s">
-        <v>117</v>
+        <v>0</v>
+      </c>
+      <c r="O20" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="B21">
         <v>1</v>
       </c>
       <c r="C21" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="D21" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="E21" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="F21" t="s">
-        <v>50</v>
-      </c>
-      <c r="G21" t="s">
-        <v>122</v>
-      </c>
-      <c r="H21" t="s">
-        <v>120</v>
+        <v>111</v>
+      </c>
+      <c r="H21" s="3" t="s">
+        <v>110</v>
       </c>
       <c r="I21" t="s">
-        <v>121</v>
+        <v>96</v>
       </c>
       <c r="J21" s="4">
-        <v>0.59299999999999997</v>
+        <v>0.61</v>
+      </c>
+      <c r="K21" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="L21" s="4">
+        <v>0.52</v>
       </c>
       <c r="M21" s="5">
         <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
-        <v>0.59299999999999997</v>
+        <v>1.1299999999999999</v>
+      </c>
+      <c r="O21" s="3" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="B22">
         <v>1</v>
       </c>
       <c r="C22" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="D22" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="E22" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="F22" t="s">
-        <v>54</v>
-      </c>
-      <c r="J22" s="4"/>
+        <v>46</v>
+      </c>
+      <c r="G22" t="s">
+        <v>117</v>
+      </c>
+      <c r="H22" t="s">
+        <v>115</v>
+      </c>
+      <c r="I22" t="s">
+        <v>116</v>
+      </c>
+      <c r="J22" s="4">
+        <v>0.59299999999999997</v>
+      </c>
       <c r="M22" s="5">
         <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
-        <v>0</v>
-      </c>
-      <c r="O22" t="s">
-        <v>123</v>
+        <v>0.59299999999999997</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="B23">
         <v>1</v>
       </c>
       <c r="C23" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="D23" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="E23" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="F23" t="s">
-        <v>129</v>
-      </c>
-      <c r="H23" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="I23" t="s">
-        <v>101</v>
-      </c>
-      <c r="J23" s="4">
-        <v>1.76</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="J23" s="4"/>
       <c r="M23" s="5">
         <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
-        <v>1.76</v>
+        <v>0</v>
+      </c>
+      <c r="O23" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="B24">
         <v>1</v>
       </c>
       <c r="C24" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="D24" t="s">
-        <v>63</v>
-      </c>
-      <c r="E24" s="6" t="s">
-        <v>155</v>
-      </c>
-      <c r="F24" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="G24" t="s">
-        <v>130</v>
+        <v>54</v>
+      </c>
+      <c r="E24" t="s">
+        <v>55</v>
+      </c>
+      <c r="F24" t="s">
+        <v>124</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>131</v>
+        <v>56</v>
       </c>
       <c r="I24" t="s">
-        <v>132</v>
+        <v>96</v>
       </c>
       <c r="J24" s="4">
+        <v>1.76</v>
+      </c>
+      <c r="M24" s="5">
+        <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
+        <v>1.76</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B25">
+        <v>1</v>
+      </c>
+      <c r="C25" t="s">
+        <v>58</v>
+      </c>
+      <c r="D25" t="s">
+        <v>59</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="G25" t="s">
+        <v>125</v>
+      </c>
+      <c r="H25" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="I25" t="s">
+        <v>127</v>
+      </c>
+      <c r="J25" s="4">
         <v>1.48</v>
       </c>
-      <c r="M24" s="5">
+      <c r="M25" s="5">
         <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
         <v>1.48</v>
-      </c>
-    </row>
-    <row r="25" spans="1:15" ht="45" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="B25">
-        <v>15</v>
-      </c>
-      <c r="C25" t="s">
-        <v>64</v>
-      </c>
-      <c r="D25" t="s">
-        <v>64</v>
-      </c>
-      <c r="E25" t="s">
-        <v>153</v>
-      </c>
-      <c r="F25" t="s">
-        <v>65</v>
-      </c>
-      <c r="G25" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="H25" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="I25" t="s">
-        <v>101</v>
-      </c>
-      <c r="J25" s="4">
-        <v>0.63</v>
-      </c>
-      <c r="M25" s="5">
-        <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
-        <v>9.4499999999999993</v>
       </c>
     </row>
     <row r="26" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>67</v>
+        <v>178</v>
       </c>
       <c r="B26">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C26" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="D26" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="E26" t="s">
-        <v>70</v>
+        <v>148</v>
       </c>
       <c r="F26" t="s">
-        <v>71</v>
-      </c>
-      <c r="J26" s="4"/>
+        <v>61</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="H26" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="I26" t="s">
+        <v>96</v>
+      </c>
+      <c r="J26" s="4">
+        <v>0.63</v>
+      </c>
       <c r="M26" s="5">
         <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
-        <v>0</v>
+        <v>8.82</v>
       </c>
     </row>
     <row r="27" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>164</v>
+        <v>63</v>
       </c>
       <c r="B27">
-        <v>12</v>
-      </c>
-      <c r="C27">
+        <v>10</v>
+      </c>
+      <c r="C27" t="s">
+        <v>64</v>
+      </c>
+      <c r="D27" t="s">
+        <v>65</v>
+      </c>
+      <c r="E27" t="s">
+        <v>66</v>
+      </c>
+      <c r="F27" t="s">
+        <v>67</v>
+      </c>
+      <c r="H27" t="s">
+        <v>186</v>
+      </c>
+      <c r="I27" t="s">
+        <v>96</v>
+      </c>
+      <c r="J27" s="4">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="M27" s="5">
+        <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
+        <v>0.29000000000000004</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="B28">
+        <v>11</v>
+      </c>
+      <c r="C28">
         <v>100</v>
       </c>
-      <c r="D27" t="s">
-        <v>69</v>
-      </c>
-      <c r="E27" t="s">
-        <v>70</v>
-      </c>
-      <c r="F27" t="s">
-        <v>71</v>
-      </c>
-      <c r="H27" t="s">
-        <v>167</v>
-      </c>
-      <c r="I27" t="s">
-        <v>101</v>
-      </c>
-      <c r="J27" s="4">
+      <c r="D28" t="s">
+        <v>65</v>
+      </c>
+      <c r="E28" t="s">
+        <v>66</v>
+      </c>
+      <c r="F28" t="s">
+        <v>67</v>
+      </c>
+      <c r="H28" t="s">
+        <v>158</v>
+      </c>
+      <c r="I28" t="s">
+        <v>96</v>
+      </c>
+      <c r="J28" s="4">
         <v>0.107</v>
       </c>
-      <c r="M27" s="5">
-        <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
-        <v>1.284</v>
-      </c>
-    </row>
-    <row r="28" spans="1:15" ht="45" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="B28">
-        <v>20</v>
-      </c>
-      <c r="C28" t="s">
-        <v>72</v>
-      </c>
-      <c r="D28" t="s">
-        <v>69</v>
-      </c>
-      <c r="E28" t="s">
-        <v>70</v>
-      </c>
-      <c r="F28" t="s">
-        <v>71</v>
-      </c>
-      <c r="J28" s="4"/>
       <c r="M28" s="5">
         <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+        <v>1.177</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>73</v>
+        <v>185</v>
       </c>
       <c r="B29">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="C29" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="D29" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="E29" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="F29" t="s">
-        <v>71</v>
-      </c>
-      <c r="J29" s="4"/>
+        <v>67</v>
+      </c>
+      <c r="H29" t="s">
+        <v>187</v>
+      </c>
+      <c r="I29" t="s">
+        <v>96</v>
+      </c>
+      <c r="J29" s="4">
+        <v>2.9000000000000001E-2</v>
+      </c>
       <c r="M29" s="5">
         <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
-        <v>0</v>
+        <v>0.60899999999999999</v>
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="B30">
         <v>3</v>
       </c>
       <c r="C30" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="D30" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="E30" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="F30" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="J30" s="4"/>
       <c r="M30" s="5">
@@ -2296,22 +2386,22 @@
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="B31">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C31" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="D31" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="E31" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="F31" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="J31" s="4"/>
       <c r="M31" s="5">
@@ -2321,22 +2411,22 @@
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B32">
         <v>1</v>
       </c>
       <c r="C32" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D32" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="E32" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="F32" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="J32" s="4"/>
       <c r="M32" s="5">
@@ -2346,22 +2436,22 @@
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="B33">
         <v>1</v>
       </c>
       <c r="C33" t="s">
-        <v>82</v>
+        <v>174</v>
       </c>
       <c r="D33" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="E33" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="F33" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="J33" s="4"/>
       <c r="M33" s="5">
@@ -2371,22 +2461,22 @@
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="B34">
         <v>1</v>
       </c>
       <c r="C34" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="D34" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="E34" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="F34" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="J34" s="4"/>
       <c r="M34" s="5">
@@ -2396,22 +2486,22 @@
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="B35">
         <v>1</v>
       </c>
       <c r="C35" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="D35" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="E35" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="F35" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="J35" s="4"/>
       <c r="M35" s="5">
@@ -2421,22 +2511,22 @@
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="B36">
         <v>1</v>
       </c>
       <c r="C36" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="D36" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="E36" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="F36" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="J36" s="4"/>
       <c r="M36" s="5">
@@ -2444,176 +2534,204 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>138</v>
+        <v>82</v>
       </c>
       <c r="B37">
+        <v>1</v>
+      </c>
+      <c r="C37" t="s">
+        <v>83</v>
+      </c>
+      <c r="D37" t="s">
+        <v>65</v>
+      </c>
+      <c r="E37" t="s">
+        <v>66</v>
+      </c>
+      <c r="F37" t="s">
+        <v>67</v>
+      </c>
+      <c r="J37" s="4"/>
+      <c r="M37" s="5">
+        <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="B38">
         <v>9</v>
       </c>
-      <c r="C37" t="s">
-        <v>89</v>
-      </c>
-      <c r="D37" t="s">
-        <v>55</v>
-      </c>
-      <c r="E37" t="s">
-        <v>56</v>
-      </c>
-      <c r="F37" t="s">
-        <v>156</v>
-      </c>
-      <c r="G37" t="s">
-        <v>137</v>
-      </c>
-      <c r="H37" t="s">
-        <v>119</v>
-      </c>
-      <c r="I37" t="s">
-        <v>101</v>
-      </c>
-      <c r="J37" s="4">
-        <v>0.57699999999999996</v>
-      </c>
-      <c r="M37" s="5">
-        <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
-        <v>5.1929999999999996</v>
-      </c>
-    </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A38" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="B38">
-        <v>3</v>
-      </c>
       <c r="C38" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="D38" t="s">
-        <v>91</v>
+        <v>51</v>
       </c>
       <c r="E38" t="s">
-        <v>154</v>
-      </c>
-      <c r="G38" s="3" t="s">
-        <v>113</v>
+        <v>52</v>
+      </c>
+      <c r="F38" t="s">
+        <v>151</v>
+      </c>
+      <c r="G38" t="s">
+        <v>132</v>
       </c>
       <c r="H38" t="s">
         <v>114</v>
       </c>
       <c r="I38" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="J38" s="4">
-        <v>1.96</v>
+        <v>0.57699999999999996</v>
       </c>
       <c r="M38" s="5">
         <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
-        <v>5.88</v>
+        <v>5.1929999999999996</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="B39">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C39" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="D39" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="E39" t="s">
-        <v>94</v>
-      </c>
-      <c r="F39" t="s">
-        <v>95</v>
+        <v>149</v>
       </c>
       <c r="G39" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="H39" t="s">
+        <v>109</v>
+      </c>
+      <c r="I39" t="s">
         <v>96</v>
       </c>
-      <c r="H39" t="s">
-        <v>108</v>
-      </c>
-      <c r="I39" t="s">
-        <v>101</v>
-      </c>
       <c r="J39" s="4">
-        <v>0.81</v>
+        <v>1.96</v>
       </c>
       <c r="M39" s="5">
         <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
-        <v>0.81</v>
+        <v>5.88</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="B40">
         <v>1</v>
       </c>
       <c r="C40" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="D40" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="E40" t="s">
-        <v>99</v>
-      </c>
-      <c r="G40" t="s">
-        <v>109</v>
+        <v>89</v>
+      </c>
+      <c r="F40" t="s">
+        <v>90</v>
+      </c>
+      <c r="G40" s="3" t="s">
+        <v>91</v>
       </c>
       <c r="H40" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="I40" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="J40" s="4">
-        <v>9.61</v>
+        <v>0.81</v>
       </c>
       <c r="M40" s="5">
         <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
-        <v>9.61</v>
+        <v>0.81</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B41">
+        <v>1</v>
+      </c>
+      <c r="C41" t="s">
+        <v>93</v>
+      </c>
+      <c r="D41" t="s">
+        <v>93</v>
+      </c>
+      <c r="E41" t="s">
+        <v>94</v>
+      </c>
+      <c r="F41" t="s">
+        <v>177</v>
+      </c>
+      <c r="G41" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="H41" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="I41" t="s">
+        <v>96</v>
+      </c>
+      <c r="J41" s="4">
+        <v>9.61</v>
+      </c>
+      <c r="M41" s="5">
+        <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
+        <v>9.61</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="B42">
+        <v>4</v>
+      </c>
+      <c r="C42" t="s">
+        <v>153</v>
+      </c>
+      <c r="D42" t="s">
+        <v>169</v>
+      </c>
+      <c r="E42" t="s">
+        <v>154</v>
+      </c>
+      <c r="F42" t="s">
         <v>157</v>
       </c>
-      <c r="B41">
-        <v>4</v>
-      </c>
-      <c r="C41" t="s">
-        <v>158</v>
-      </c>
-      <c r="D41" t="s">
-        <v>158</v>
-      </c>
-      <c r="E41" t="s">
-        <v>159</v>
-      </c>
-      <c r="F41" t="s">
-        <v>162</v>
-      </c>
-      <c r="G41" t="s">
-        <v>160</v>
-      </c>
-      <c r="H41" s="3" t="s">
-        <v>161</v>
-      </c>
-      <c r="I41" t="s">
-        <v>101</v>
-      </c>
-      <c r="J41" s="4">
+      <c r="G42" t="s">
+        <v>155</v>
+      </c>
+      <c r="H42" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="I42" t="s">
+        <v>96</v>
+      </c>
+      <c r="J42" s="4">
         <v>1.71</v>
       </c>
-      <c r="M41" s="5">
+      <c r="M42" s="5">
         <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
         <v>6.84</v>
       </c>
@@ -2621,23 +2739,29 @@
   </sheetData>
   <phoneticPr fontId="19" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="H23" r:id="rId1" xr:uid="{DD8AD352-FB06-4715-B587-8B7434FCD99F}"/>
-    <hyperlink ref="G25" r:id="rId2" xr:uid="{5EFE7EEC-7A33-4705-B297-C4BD3E05DA2C}"/>
-    <hyperlink ref="G39" r:id="rId3" xr:uid="{71FE485A-AA2E-4950-BE10-E132C884D307}"/>
-    <hyperlink ref="K20" r:id="rId4" xr:uid="{DB18BABB-D85D-4D81-84B1-06B4803F7A71}"/>
-    <hyperlink ref="G17" r:id="rId5" xr:uid="{6E03D079-3A0C-4BF5-810D-97558264CB66}"/>
-    <hyperlink ref="G18" r:id="rId6" xr:uid="{7C702CAB-8E1E-429C-9A90-1E47838C9BF7}"/>
-    <hyperlink ref="G38" r:id="rId7" xr:uid="{ACFE634D-160F-4B71-8DB2-7FFC85727160}"/>
-    <hyperlink ref="H24" r:id="rId8" xr:uid="{7C8D1661-4DCD-43AD-B870-FF77BABDB784}"/>
-    <hyperlink ref="H20" r:id="rId9" xr:uid="{257864EB-78CF-4B88-864D-5BF4D3EC4937}"/>
-    <hyperlink ref="O20" r:id="rId10" xr:uid="{438620CA-1198-495F-B2D1-DE18D03FD0CF}"/>
-    <hyperlink ref="H25" r:id="rId11" xr:uid="{50608FB6-E114-4108-91A8-FC7B919453D0}"/>
-    <hyperlink ref="H41" r:id="rId12" xr:uid="{8161F553-B981-424E-8CA4-DA1BB9415ECC}"/>
+    <hyperlink ref="H24" r:id="rId1" xr:uid="{DD8AD352-FB06-4715-B587-8B7434FCD99F}"/>
+    <hyperlink ref="G26" r:id="rId2" xr:uid="{5EFE7EEC-7A33-4705-B297-C4BD3E05DA2C}"/>
+    <hyperlink ref="G40" r:id="rId3" xr:uid="{71FE485A-AA2E-4950-BE10-E132C884D307}"/>
+    <hyperlink ref="K21" r:id="rId4" xr:uid="{DB18BABB-D85D-4D81-84B1-06B4803F7A71}"/>
+    <hyperlink ref="G18" r:id="rId5" xr:uid="{6E03D079-3A0C-4BF5-810D-97558264CB66}"/>
+    <hyperlink ref="G19" r:id="rId6" xr:uid="{7C702CAB-8E1E-429C-9A90-1E47838C9BF7}"/>
+    <hyperlink ref="G39" r:id="rId7" xr:uid="{ACFE634D-160F-4B71-8DB2-7FFC85727160}"/>
+    <hyperlink ref="H25" r:id="rId8" xr:uid="{7C8D1661-4DCD-43AD-B870-FF77BABDB784}"/>
+    <hyperlink ref="H21" r:id="rId9" xr:uid="{257864EB-78CF-4B88-864D-5BF4D3EC4937}"/>
+    <hyperlink ref="O21" r:id="rId10" xr:uid="{438620CA-1198-495F-B2D1-DE18D03FD0CF}"/>
+    <hyperlink ref="H26" r:id="rId11" xr:uid="{50608FB6-E114-4108-91A8-FC7B919453D0}"/>
+    <hyperlink ref="H42" r:id="rId12" xr:uid="{8161F553-B981-424E-8CA4-DA1BB9415ECC}"/>
+    <hyperlink ref="H8" r:id="rId13" xr:uid="{9431E3EC-4579-4581-9011-6B05F37CF302}"/>
+    <hyperlink ref="G41" r:id="rId14" xr:uid="{6235F029-DC34-40F5-B3C4-8045E09C4F42}"/>
+    <hyperlink ref="K8" r:id="rId15" xr:uid="{71E59B7F-99D7-40E9-B1FE-1FF9731CAD3F}"/>
+    <hyperlink ref="G17" r:id="rId16" xr:uid="{6C3216AC-996C-4C4E-A7C7-D6FD12DC9E06}"/>
+    <hyperlink ref="H41" r:id="rId17" xr:uid="{89885BDB-09BB-4D47-9D07-262D9AE4373B}"/>
+    <hyperlink ref="H15" r:id="rId18" xr:uid="{81319735-1B12-4848-AD96-716F6B41299B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId13"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId19"/>
   <tableParts count="1">
-    <tablePart r:id="rId14"/>
+    <tablePart r:id="rId20"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
need to go bakc to previos zener diode for overvoltage
</commit_message>
<xml_diff>
--- a/RADSAT-SK Timer/RADSAT-SK Timer.xlsx
+++ b/RADSAT-SK Timer/RADSAT-SK Timer.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\riley\USST\RADSAT-SK\power-and-electrical\RADSAT-SK Timer\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\USST\power-and-electrical\RADSAT-SK Timer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7651C43F-B578-4695-A081-92386930BC72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5A7941E-CD93-451F-988F-CB4F06C61ABB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-3000" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RADSAT-SK Timer" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="193">
   <si>
     <t>Source:</t>
   </si>
@@ -72,9 +72,6 @@
     <t>Footprint</t>
   </si>
   <si>
-    <t>Vendor</t>
-  </si>
-  <si>
     <t>Price</t>
   </si>
   <si>
@@ -93,9 +90,6 @@
     <t>CP</t>
   </si>
   <si>
-    <t xml:space="preserve">C103, C104, C109, C110, C111, C112, C113, C114, </t>
-  </si>
-  <si>
     <t>100n</t>
   </si>
   <si>
@@ -114,12 +108,6 @@
     <t>10uF</t>
   </si>
   <si>
-    <t xml:space="preserve">C205, </t>
-  </si>
-  <si>
-    <t>0.1uF</t>
-  </si>
-  <si>
     <t xml:space="preserve">C207, </t>
   </si>
   <si>
@@ -321,9 +309,6 @@
     <t>10/20/2021  6:26PM</t>
   </si>
   <si>
-    <t>digikey</t>
-  </si>
-  <si>
     <t>Product URL</t>
   </si>
   <si>
@@ -381,9 +366,6 @@
     <t>https://www.mouser.ca/ProductDetail/Hirose-Connector/DF13-5P-125DSA?qs=Ux3WWAnHpjDJWf8XCjmDFw%3D%3D</t>
   </si>
   <si>
-    <t>Mouser</t>
-  </si>
-  <si>
     <t>https://www.mouser.ca/datasheet/2/185/DF13_Catalog_D31687_en-2486995.pdf</t>
   </si>
   <si>
@@ -414,9 +396,6 @@
     <t>https://www.digikey.ca/en/products/detail/sumida-america-components-inc/CDRH4D28NP-100NC/1059478</t>
   </si>
   <si>
-    <t>DIGIKEY</t>
-  </si>
-  <si>
     <t>DIODE SCHOTTKY 20V 1A POWERMITE | from boost circuit</t>
   </si>
   <si>
@@ -529,9 +508,6 @@
   </si>
   <si>
     <t>https://www.digikey.ca/en/products/detail/keystone-electronics/1061/303558</t>
-  </si>
-  <si>
-    <t>didkey/mouser</t>
   </si>
   <si>
     <t>BATT HLDR COIN 20MM 1/2 CEL SMD</t>
@@ -609,13 +585,52 @@
   <si>
     <t>https://www.digikey.ca/en/products/detail/stackpole-electronics-inc/RMCF0805JT1K00/1757881</t>
   </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/vishay-dale/CRCW08053M48FKEA/1176076?s=N4IgjCBcpgbFoDGUBmBDANgZwKYBoQB7KAbRAGYBOcgJkpAF0CAHAFyhAGVWAnASwB2AcxABfAjQAMADgCsCEGw4BVAX1YB5FAFkcaLAFceOEAQMdtGgBYBbLKZA3BHcgDoALNIc20ADxceXuIgALQ0CsiQvAb4RKQg8gyiweGQZMZYfFishDyMBPDQIHwAJhwhYJIQLOyQIA6sAJ7MJnX6yMlAA</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/stackpole-electronics-inc/RMCF0805FT442K/1713153</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/stackpole-electronics-inc/RMCF0805FT5M10/1713191</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/stackpole-electronics-inc/RMCF0805FT60K4/1760362</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/stackpole-electronics-inc/RMCF0805FT15K0/1760487</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/stackpole-electronics-inc/RMCF0805FT619K/1713291</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/stackpole-electronics-inc/RMCF0805JT200K/1757911</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/tdk-corporation/C2012X7R1H104K085AA/2732969</t>
+  </si>
+  <si>
+    <t>C103, C104, C109, C110, C111, C112, C113, C114, C204</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/tdk-corporation/C2012X5R1E155K125AA/2733062</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/hirose-electric-co-ltd/DF13-3P-1-25V-75/9170629</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>Column1</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="20" x14ac:knownFonts="1">
     <font>
@@ -1107,19 +1122,22 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="43"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="42" applyFont="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="42" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="44">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1169,7 +1187,7 @@
   </cellStyles>
   <dxfs count="2">
     <dxf>
-      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+      <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1188,8 +1206,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A7:M42" totalsRowShown="0">
-  <autoFilter ref="A7:M42" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A7:M41" totalsRowShown="0">
+  <autoFilter ref="A7:M41" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Ref" dataDxfId="1"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Qnty"/>
@@ -1199,13 +1217,13 @@
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Description/Notes"/>
     <tableColumn id="12" xr3:uid="{AC2AB4E9-9984-41C3-88C4-EF1E70A1C977}" name="Datasheet"/>
     <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Product URL"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Vendor"/>
     <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Price" dataCellStyle="Currency"/>
     <tableColumn id="10" xr3:uid="{7C21AC37-B81A-4891-A949-B8777B84C389}" name="Related Components"/>
     <tableColumn id="11" xr3:uid="{73FB3C5D-D954-4E05-BC68-91835A2C1577}" name="Price2" dataCellStyle="Currency"/>
     <tableColumn id="13" xr3:uid="{37B8C3F1-4773-42D9-BB38-8CAD10942CF3}" name="Price total" dataDxfId="0">
       <calculatedColumnFormula>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</calculatedColumnFormula>
     </tableColumn>
+    <tableColumn id="8" xr3:uid="{E3F168F5-0327-4120-8A2A-37C19A3AC65B}" name="Column1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1508,11 +1526,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O42"/>
+  <dimension ref="A1:N41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="J29" sqref="J29"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <pane xSplit="8670" topLeftCell="H1" activePane="topRight"/>
+      <selection activeCell="C6" sqref="C6"/>
+      <selection pane="topRight" activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1525,11 +1544,10 @@
     <col min="6" max="6" width="107.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="107.28515625" customWidth="1"/>
     <col min="8" max="8" width="87" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.7109375" customWidth="1"/>
-    <col min="11" max="11" width="25" customWidth="1"/>
-    <col min="12" max="12" width="9.140625" style="4"/>
-    <col min="13" max="13" width="12.42578125" customWidth="1"/>
+    <col min="9" max="9" width="7.7109375" customWidth="1"/>
+    <col min="10" max="10" width="25" customWidth="1"/>
+    <col min="11" max="11" width="9.140625" style="4"/>
+    <col min="12" max="12" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
@@ -1545,7 +1563,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -1574,11 +1592,11 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="B6" s="5">
-        <f>SUM(M8:M42)</f>
-        <v>81.551999999999992</v>
+        <f>SUM(L8:L41)</f>
+        <v>85.551999999999992</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -1598,500 +1616,488 @@
         <v>12</v>
       </c>
       <c r="F7" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="G7" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="H7" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="I7" t="s">
         <v>13</v>
       </c>
       <c r="J7" t="s">
-        <v>14</v>
-      </c>
-      <c r="K7" t="s">
-        <v>100</v>
-      </c>
-      <c r="L7" s="4" t="s">
-        <v>99</v>
+        <v>95</v>
+      </c>
+      <c r="K7" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="L7" t="s">
+        <v>102</v>
       </c>
       <c r="M7" t="s">
-        <v>107</v>
+        <v>192</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B8">
         <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E8" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
       <c r="F8" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="G8" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>165</v>
-      </c>
-      <c r="I8" t="s">
-        <v>166</v>
-      </c>
-      <c r="J8" s="4">
+        <v>158</v>
+      </c>
+      <c r="I8" s="4">
         <v>4.09</v>
       </c>
-      <c r="K8" s="3" t="s">
-        <v>164</v>
-      </c>
-      <c r="L8" s="4">
+      <c r="J8" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="K8" s="4">
         <v>1.61</v>
       </c>
-      <c r="M8" s="5">
+      <c r="L8" s="5">
         <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
         <v>11.4</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B9">
         <v>6</v>
       </c>
       <c r="C9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" t="s">
         <v>18</v>
       </c>
-      <c r="D9" t="s">
-        <v>19</v>
-      </c>
       <c r="E9" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="F9" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="H9" t="s">
-        <v>159</v>
-      </c>
-      <c r="I9" t="s">
-        <v>96</v>
-      </c>
-      <c r="J9" s="4">
+        <v>152</v>
+      </c>
+      <c r="I9" s="4">
         <v>3.36</v>
       </c>
-      <c r="M9" s="5">
+      <c r="L9" s="5">
         <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
         <v>20.16</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="B10">
+        <v>9</v>
+      </c>
+      <c r="C10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" t="s">
         <v>20</v>
       </c>
-      <c r="B10">
-        <v>8</v>
-      </c>
-      <c r="C10" t="s">
+      <c r="E10" t="s">
         <v>21</v>
       </c>
-      <c r="D10" t="s">
+      <c r="F10" t="s">
         <v>22</v>
       </c>
-      <c r="E10" t="s">
-        <v>23</v>
-      </c>
-      <c r="F10" t="s">
-        <v>24</v>
-      </c>
-      <c r="J10" s="4"/>
-      <c r="M10" s="5">
-        <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
-        <v>0</v>
+      <c r="H10" t="s">
+        <v>187</v>
+      </c>
+      <c r="I10" s="4">
+        <v>0.15</v>
+      </c>
+      <c r="L10" s="5">
+        <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
+        <v>1.3499999999999999</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B11">
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D11" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E11" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="G11" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="H11" t="s">
-        <v>139</v>
-      </c>
-      <c r="I11" t="s">
-        <v>96</v>
-      </c>
-      <c r="J11" s="4">
+        <v>132</v>
+      </c>
+      <c r="I11" s="4">
         <v>0.41</v>
       </c>
-      <c r="M11" s="5">
+      <c r="L11" s="5">
         <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
         <v>0.41</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B12">
         <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D12" t="s">
+        <v>20</v>
+      </c>
+      <c r="E12" t="s">
+        <v>21</v>
+      </c>
+      <c r="F12" t="s">
         <v>22</v>
       </c>
-      <c r="E12" t="s">
-        <v>23</v>
-      </c>
-      <c r="F12" t="s">
-        <v>24</v>
-      </c>
-      <c r="J12" s="4"/>
-      <c r="M12" s="5">
-        <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
-        <v>0</v>
+      <c r="H12" t="s">
+        <v>189</v>
+      </c>
+      <c r="I12" s="4">
+        <v>0.41</v>
+      </c>
+      <c r="L12" s="5">
+        <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
+        <v>0.41</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B13">
         <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D13" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E13" t="s">
-        <v>23</v>
-      </c>
-      <c r="F13" t="s">
-        <v>24</v>
-      </c>
-      <c r="J13" s="4"/>
-      <c r="M13" s="5">
-        <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
-        <v>0</v>
+        <v>130</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="G13" t="s">
+        <v>128</v>
+      </c>
+      <c r="H13" t="s">
+        <v>129</v>
+      </c>
+      <c r="I13" s="4">
+        <v>1.0900000000000001</v>
+      </c>
+      <c r="L13" s="5">
+        <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
+        <v>1.0900000000000001</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>31</v>
+        <v>173</v>
       </c>
       <c r="B14">
         <v>1</v>
       </c>
       <c r="C14" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D14" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="E14" t="s">
-        <v>137</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>134</v>
+        <v>140</v>
+      </c>
+      <c r="F14" t="s">
+        <v>155</v>
       </c>
       <c r="G14" t="s">
-        <v>135</v>
-      </c>
-      <c r="H14" t="s">
-        <v>136</v>
-      </c>
-      <c r="I14" t="s">
-        <v>96</v>
-      </c>
-      <c r="J14" s="4">
-        <v>1.0900000000000001</v>
-      </c>
-      <c r="M14" s="5">
-        <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
-        <v>1.0900000000000001</v>
+        <v>176</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="I14" s="4">
+        <v>0.33</v>
+      </c>
+      <c r="L14" s="5">
+        <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
+        <v>0.33</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
       <c r="B15">
         <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D15" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="E15" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="F15" t="s">
-        <v>162</v>
-      </c>
-      <c r="G15" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>163</v>
-      </c>
-      <c r="I15" t="s">
-        <v>96</v>
-      </c>
-      <c r="J15" s="4">
+        <v>175</v>
+      </c>
+      <c r="I15" s="4">
         <v>0.33</v>
       </c>
-      <c r="M15" s="5">
+      <c r="L15" s="5">
         <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
         <v>0.33</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>180</v>
+        <v>30</v>
       </c>
       <c r="B16">
         <v>1</v>
       </c>
       <c r="C16" t="s">
-        <v>33</v>
+        <v>164</v>
       </c>
       <c r="D16" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E16" t="s">
-        <v>147</v>
+        <v>168</v>
       </c>
       <c r="F16" t="s">
-        <v>182</v>
-      </c>
-      <c r="H16" s="3" t="s">
-        <v>183</v>
-      </c>
-      <c r="I16" t="s">
-        <v>96</v>
-      </c>
-      <c r="J16" s="4">
-        <v>0.33</v>
-      </c>
-      <c r="M16" s="5">
-        <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
-        <v>0.33</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+        <v>165</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="H16" t="s">
+        <v>162</v>
+      </c>
+      <c r="I16" s="4">
+        <v>2.33</v>
+      </c>
+      <c r="L16" s="5">
+        <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
+        <v>2.33</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B17">
         <v>1</v>
       </c>
       <c r="C17" t="s">
-        <v>172</v>
+        <v>115</v>
       </c>
       <c r="D17" t="s">
-        <v>35</v>
+        <v>116</v>
       </c>
       <c r="E17" t="s">
-        <v>176</v>
+        <v>117</v>
       </c>
       <c r="F17" t="s">
-        <v>173</v>
+        <v>121</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>171</v>
+        <v>113</v>
       </c>
       <c r="H17" t="s">
-        <v>170</v>
-      </c>
-      <c r="I17" t="s">
-        <v>96</v>
-      </c>
-      <c r="J17" s="4">
-        <v>2.33</v>
-      </c>
-      <c r="M17" s="5">
-        <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
-        <v>2.33</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+        <v>114</v>
+      </c>
+      <c r="I17" s="4">
+        <v>0.76</v>
+      </c>
+      <c r="L17" s="5">
+        <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
+        <v>0.76</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>36</v>
+        <v>134</v>
       </c>
       <c r="B18">
         <v>1</v>
       </c>
-      <c r="C18" t="s">
-        <v>121</v>
+      <c r="C18" s="2" t="s">
+        <v>135</v>
       </c>
       <c r="D18" t="s">
-        <v>122</v>
+        <v>135</v>
       </c>
       <c r="E18" t="s">
-        <v>123</v>
+        <v>136</v>
       </c>
       <c r="F18" t="s">
-        <v>128</v>
+        <v>137</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>119</v>
+        <v>138</v>
       </c>
       <c r="H18" t="s">
-        <v>120</v>
-      </c>
-      <c r="I18" t="s">
-        <v>96</v>
-      </c>
-      <c r="J18" s="4">
-        <v>0.76</v>
-      </c>
-      <c r="M18" s="5">
-        <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
-        <v>0.76</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>139</v>
+      </c>
+      <c r="I18" s="4">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="L18" s="5">
+        <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>141</v>
+        <v>33</v>
       </c>
       <c r="B19">
+        <v>2</v>
+      </c>
+      <c r="C19" t="s">
+        <v>34</v>
+      </c>
+      <c r="D19" t="s">
+        <v>34</v>
+      </c>
+      <c r="E19" t="s">
+        <v>35</v>
+      </c>
+      <c r="F19" t="s">
+        <v>124</v>
+      </c>
+      <c r="I19" s="4"/>
+      <c r="L19" s="5">
+        <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
+        <v>0</v>
+      </c>
+      <c r="N19" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B20">
         <v>1</v>
       </c>
-      <c r="C19" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="D19" t="s">
-        <v>142</v>
-      </c>
-      <c r="E19" t="s">
-        <v>143</v>
-      </c>
-      <c r="F19" t="s">
-        <v>144</v>
-      </c>
-      <c r="G19" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="H19" t="s">
-        <v>146</v>
-      </c>
-      <c r="I19" t="s">
-        <v>96</v>
-      </c>
-      <c r="J19" s="4">
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="M19" s="5">
-        <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
-        <v>0.55000000000000004</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
+      <c r="C20" t="s">
         <v>37</v>
       </c>
-      <c r="B20">
-        <v>2</v>
-      </c>
-      <c r="C20" t="s">
+      <c r="D20" t="s">
+        <v>37</v>
+      </c>
+      <c r="E20" t="s">
         <v>38</v>
       </c>
-      <c r="D20" t="s">
-        <v>38</v>
-      </c>
-      <c r="E20" t="s">
+      <c r="F20" t="s">
+        <v>106</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="I20" s="4">
+        <v>0.61</v>
+      </c>
+      <c r="J20" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="K20" s="4">
+        <v>0.52</v>
+      </c>
+      <c r="L20" s="5">
+        <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
+        <v>1.1299999999999999</v>
+      </c>
+      <c r="N20" s="3" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
         <v>39</v>
-      </c>
-      <c r="F20" t="s">
-        <v>131</v>
-      </c>
-      <c r="J20" s="4"/>
-      <c r="M20" s="5">
-        <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
-        <v>0</v>
-      </c>
-      <c r="O20" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
-        <v>40</v>
       </c>
       <c r="B21">
         <v>1</v>
       </c>
       <c r="C21" t="s">
+        <v>40</v>
+      </c>
+      <c r="D21" t="s">
+        <v>40</v>
+      </c>
+      <c r="E21" t="s">
         <v>41</v>
       </c>
-      <c r="D21" t="s">
-        <v>41</v>
-      </c>
-      <c r="E21" t="s">
+      <c r="F21" t="s">
         <v>42</v>
       </c>
-      <c r="F21" t="s">
+      <c r="G21" t="s">
         <v>111</v>
       </c>
       <c r="H21" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="I21" t="s">
-        <v>96</v>
-      </c>
-      <c r="J21" s="4">
-        <v>0.61</v>
-      </c>
-      <c r="K21" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="L21" s="4">
-        <v>0.52</v>
-      </c>
-      <c r="M21" s="5">
-        <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
-        <v>1.1299999999999999</v>
-      </c>
-      <c r="O21" s="3" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="I21" s="4">
+        <v>0.59299999999999997</v>
+      </c>
+      <c r="L21" s="5">
+        <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
+        <v>0.59299999999999997</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>43</v>
       </c>
@@ -2110,52 +2116,51 @@
       <c r="F22" t="s">
         <v>46</v>
       </c>
-      <c r="G22" t="s">
-        <v>117</v>
-      </c>
-      <c r="H22" t="s">
-        <v>115</v>
-      </c>
-      <c r="I22" t="s">
-        <v>116</v>
-      </c>
-      <c r="J22" s="4">
-        <v>0.59299999999999997</v>
-      </c>
-      <c r="M22" s="5">
-        <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
-        <v>0.59299999999999997</v>
-      </c>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="H22" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="I22" s="4">
+        <v>0.59</v>
+      </c>
+      <c r="L22" s="5">
+        <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
+        <v>0.59</v>
+      </c>
+      <c r="N22" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B23">
         <v>1</v>
       </c>
       <c r="C23" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D23" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="E23" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="F23" t="s">
-        <v>50</v>
-      </c>
-      <c r="J23" s="4"/>
-      <c r="M23" s="5">
-        <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
-        <v>0</v>
-      </c>
-      <c r="O23" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="H23" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="I23" s="4">
+        <v>1.76</v>
+      </c>
+      <c r="L23" s="5">
+        <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
+        <v>1.76</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>53</v>
       </c>
@@ -2166,572 +2171,547 @@
         <v>54</v>
       </c>
       <c r="D24" t="s">
-        <v>54</v>
-      </c>
-      <c r="E24" t="s">
         <v>55</v>
       </c>
-      <c r="F24" t="s">
-        <v>124</v>
+      <c r="E24" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="G24" t="s">
+        <v>119</v>
       </c>
       <c r="H24" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="I24" s="4">
+        <v>1.48</v>
+      </c>
+      <c r="L24" s="5">
+        <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
+        <v>1.48</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="B25">
+        <v>14</v>
+      </c>
+      <c r="C25" t="s">
         <v>56</v>
       </c>
-      <c r="I24" t="s">
-        <v>96</v>
-      </c>
-      <c r="J24" s="4">
-        <v>1.76</v>
-      </c>
-      <c r="M24" s="5">
-        <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
-        <v>1.76</v>
-      </c>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
+      <c r="D25" t="s">
+        <v>56</v>
+      </c>
+      <c r="E25" t="s">
+        <v>141</v>
+      </c>
+      <c r="F25" t="s">
         <v>57</v>
       </c>
-      <c r="B25">
-        <v>1</v>
-      </c>
-      <c r="C25" t="s">
+      <c r="G25" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="D25" t="s">
+      <c r="H25" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="I25" s="4">
+        <v>0.63</v>
+      </c>
+      <c r="L25" s="5">
+        <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
+        <v>8.82</v>
+      </c>
+      <c r="M25" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="E25" s="6" t="s">
-        <v>150</v>
-      </c>
-      <c r="F25" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="G25" t="s">
-        <v>125</v>
-      </c>
-      <c r="H25" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="I25" t="s">
-        <v>127</v>
-      </c>
-      <c r="J25" s="4">
-        <v>1.48</v>
-      </c>
-      <c r="M25" s="5">
-        <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
-        <v>1.48</v>
-      </c>
-    </row>
-    <row r="26" spans="1:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
-        <v>178</v>
-      </c>
       <c r="B26">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C26" t="s">
         <v>60</v>
       </c>
       <c r="D26" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E26" t="s">
-        <v>148</v>
+        <v>62</v>
       </c>
       <c r="F26" t="s">
+        <v>63</v>
+      </c>
+      <c r="H26" t="s">
+        <v>178</v>
+      </c>
+      <c r="I26" s="4">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="L26" s="5">
+        <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
+        <v>0.29000000000000004</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="B27">
+        <v>11</v>
+      </c>
+      <c r="C27" s="7">
+        <v>100</v>
+      </c>
+      <c r="D27" t="s">
         <v>61</v>
       </c>
-      <c r="G26" s="3" t="s">
+      <c r="E27" t="s">
         <v>62</v>
       </c>
-      <c r="H26" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="I26" t="s">
-        <v>96</v>
-      </c>
-      <c r="J26" s="4">
-        <v>0.63</v>
-      </c>
-      <c r="M26" s="5">
-        <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
-        <v>8.82</v>
-      </c>
-    </row>
-    <row r="27" spans="1:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
+      <c r="F27" t="s">
         <v>63</v>
       </c>
-      <c r="B27">
-        <v>10</v>
-      </c>
-      <c r="C27" t="s">
+      <c r="H27" t="s">
+        <v>151</v>
+      </c>
+      <c r="I27" s="4">
+        <v>0.107</v>
+      </c>
+      <c r="L27" s="5">
+        <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
+        <v>1.177</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="B28">
+        <v>21</v>
+      </c>
+      <c r="C28" t="s">
         <v>64</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D28" t="s">
+        <v>61</v>
+      </c>
+      <c r="E28" t="s">
+        <v>62</v>
+      </c>
+      <c r="F28" t="s">
+        <v>63</v>
+      </c>
+      <c r="H28" t="s">
+        <v>179</v>
+      </c>
+      <c r="I28" s="4">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="L28" s="5">
+        <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
+        <v>0.60899999999999999</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="E27" t="s">
+      <c r="B29">
+        <v>3</v>
+      </c>
+      <c r="C29" t="s">
         <v>66</v>
       </c>
-      <c r="F27" t="s">
+      <c r="D29" t="s">
+        <v>61</v>
+      </c>
+      <c r="E29" t="s">
+        <v>62</v>
+      </c>
+      <c r="F29" t="s">
+        <v>63</v>
+      </c>
+      <c r="H29" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="I29" s="4">
+        <v>0.15</v>
+      </c>
+      <c r="L29" s="5">
+        <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
+        <v>0.44999999999999996</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
         <v>67</v>
-      </c>
-      <c r="H27" t="s">
-        <v>186</v>
-      </c>
-      <c r="I27" t="s">
-        <v>96</v>
-      </c>
-      <c r="J27" s="4">
-        <v>2.9000000000000001E-2</v>
-      </c>
-      <c r="M27" s="5">
-        <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
-        <v>0.29000000000000004</v>
-      </c>
-    </row>
-    <row r="28" spans="1:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="B28">
-        <v>11</v>
-      </c>
-      <c r="C28">
-        <v>100</v>
-      </c>
-      <c r="D28" t="s">
-        <v>65</v>
-      </c>
-      <c r="E28" t="s">
-        <v>66</v>
-      </c>
-      <c r="F28" t="s">
-        <v>67</v>
-      </c>
-      <c r="H28" t="s">
-        <v>158</v>
-      </c>
-      <c r="I28" t="s">
-        <v>96</v>
-      </c>
-      <c r="J28" s="4">
-        <v>0.107</v>
-      </c>
-      <c r="M28" s="5">
-        <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
-        <v>1.177</v>
-      </c>
-    </row>
-    <row r="29" spans="1:15" ht="45" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="B29">
-        <v>21</v>
-      </c>
-      <c r="C29" t="s">
-        <v>68</v>
-      </c>
-      <c r="D29" t="s">
-        <v>65</v>
-      </c>
-      <c r="E29" t="s">
-        <v>66</v>
-      </c>
-      <c r="F29" t="s">
-        <v>67</v>
-      </c>
-      <c r="H29" t="s">
-        <v>187</v>
-      </c>
-      <c r="I29" t="s">
-        <v>96</v>
-      </c>
-      <c r="J29" s="4">
-        <v>2.9000000000000001E-2</v>
-      </c>
-      <c r="M29" s="5">
-        <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
-        <v>0.60899999999999999</v>
-      </c>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
-        <v>69</v>
       </c>
       <c r="B30">
         <v>3</v>
       </c>
       <c r="C30" t="s">
+        <v>68</v>
+      </c>
+      <c r="D30" t="s">
+        <v>61</v>
+      </c>
+      <c r="E30" t="s">
+        <v>62</v>
+      </c>
+      <c r="F30" t="s">
+        <v>63</v>
+      </c>
+      <c r="H30" t="s">
+        <v>181</v>
+      </c>
+      <c r="I30" s="4">
+        <v>0.15</v>
+      </c>
+      <c r="L30" s="5">
+        <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
+        <v>0.44999999999999996</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B31">
+        <v>1</v>
+      </c>
+      <c r="C31" t="s">
         <v>70</v>
       </c>
-      <c r="D30" t="s">
-        <v>65</v>
-      </c>
-      <c r="E30" t="s">
-        <v>66</v>
-      </c>
-      <c r="F30" t="s">
-        <v>67</v>
-      </c>
-      <c r="J30" s="4"/>
-      <c r="M30" s="5">
-        <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="s">
+      <c r="D31" t="s">
+        <v>61</v>
+      </c>
+      <c r="E31" t="s">
+        <v>62</v>
+      </c>
+      <c r="F31" t="s">
+        <v>63</v>
+      </c>
+      <c r="H31" t="s">
+        <v>182</v>
+      </c>
+      <c r="I31" s="4">
+        <v>0.15</v>
+      </c>
+      <c r="L31" s="5">
+        <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
         <v>71</v>
-      </c>
-      <c r="B31">
-        <v>3</v>
-      </c>
-      <c r="C31" t="s">
-        <v>72</v>
-      </c>
-      <c r="D31" t="s">
-        <v>65</v>
-      </c>
-      <c r="E31" t="s">
-        <v>66</v>
-      </c>
-      <c r="F31" t="s">
-        <v>67</v>
-      </c>
-      <c r="J31" s="4"/>
-      <c r="M31" s="5">
-        <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
-        <v>73</v>
       </c>
       <c r="B32">
         <v>1</v>
       </c>
       <c r="C32" t="s">
-        <v>74</v>
+        <v>166</v>
       </c>
       <c r="D32" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="E32" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="F32" t="s">
-        <v>67</v>
-      </c>
-      <c r="J32" s="4"/>
-      <c r="M32" s="5">
+        <v>63</v>
+      </c>
+      <c r="I32" s="4"/>
+      <c r="L32" s="5">
         <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B33">
         <v>1</v>
       </c>
       <c r="C33" t="s">
-        <v>174</v>
+        <v>73</v>
       </c>
       <c r="D33" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="E33" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="F33" t="s">
-        <v>67</v>
-      </c>
-      <c r="J33" s="4"/>
-      <c r="M33" s="5">
-        <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+      <c r="H33" t="s">
+        <v>183</v>
+      </c>
+      <c r="I33" s="4">
+        <v>0.15</v>
+      </c>
+      <c r="L33" s="5">
+        <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B34">
         <v>1</v>
       </c>
       <c r="C34" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D34" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="E34" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="F34" t="s">
-        <v>67</v>
-      </c>
-      <c r="J34" s="4"/>
-      <c r="M34" s="5">
-        <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+      <c r="H34" t="s">
+        <v>184</v>
+      </c>
+      <c r="I34" s="4">
+        <v>0.15</v>
+      </c>
+      <c r="L34" s="5">
+        <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B35">
         <v>1</v>
       </c>
       <c r="C35" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D35" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="E35" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="F35" t="s">
-        <v>67</v>
-      </c>
-      <c r="J35" s="4"/>
-      <c r="M35" s="5">
-        <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+      <c r="H35" t="s">
+        <v>185</v>
+      </c>
+      <c r="I35" s="4">
+        <v>0.15</v>
+      </c>
+      <c r="L35" s="5">
+        <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B36">
         <v>1</v>
       </c>
       <c r="C36" t="s">
+        <v>79</v>
+      </c>
+      <c r="D36" t="s">
+        <v>61</v>
+      </c>
+      <c r="E36" t="s">
+        <v>62</v>
+      </c>
+      <c r="F36" t="s">
+        <v>63</v>
+      </c>
+      <c r="H36" t="s">
+        <v>186</v>
+      </c>
+      <c r="I36" s="4">
+        <v>0.15</v>
+      </c>
+      <c r="L36" s="5">
+        <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="B37">
+        <v>9</v>
+      </c>
+      <c r="C37" t="s">
+        <v>80</v>
+      </c>
+      <c r="D37" t="s">
+        <v>47</v>
+      </c>
+      <c r="E37" t="s">
+        <v>48</v>
+      </c>
+      <c r="F37" t="s">
+        <v>144</v>
+      </c>
+      <c r="G37" t="s">
+        <v>125</v>
+      </c>
+      <c r="H37" t="s">
+        <v>109</v>
+      </c>
+      <c r="I37" s="4">
+        <v>0.57699999999999996</v>
+      </c>
+      <c r="L37" s="5">
+        <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
+        <v>5.1929999999999996</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="D36" t="s">
-        <v>65</v>
-      </c>
-      <c r="E36" t="s">
-        <v>66</v>
-      </c>
-      <c r="F36" t="s">
-        <v>67</v>
-      </c>
-      <c r="J36" s="4"/>
-      <c r="M36" s="5">
-        <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A37" s="2" t="s">
+      <c r="B38">
+        <v>3</v>
+      </c>
+      <c r="C38" t="s">
         <v>82</v>
       </c>
-      <c r="B37">
+      <c r="D38" t="s">
+        <v>82</v>
+      </c>
+      <c r="E38" t="s">
+        <v>142</v>
+      </c>
+      <c r="G38" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="H38" t="s">
+        <v>104</v>
+      </c>
+      <c r="I38" s="4">
+        <v>1.96</v>
+      </c>
+      <c r="L38" s="5">
+        <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
+        <v>5.88</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B39">
         <v>1</v>
       </c>
-      <c r="C37" t="s">
-        <v>83</v>
-      </c>
-      <c r="D37" t="s">
-        <v>65</v>
-      </c>
-      <c r="E37" t="s">
-        <v>66</v>
-      </c>
-      <c r="F37" t="s">
-        <v>67</v>
-      </c>
-      <c r="J37" s="4"/>
-      <c r="M37" s="5">
-        <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A38" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="B38">
-        <v>9</v>
-      </c>
-      <c r="C38" t="s">
+      <c r="C39" t="s">
         <v>84</v>
       </c>
-      <c r="D38" t="s">
-        <v>51</v>
-      </c>
-      <c r="E38" t="s">
-        <v>52</v>
-      </c>
-      <c r="F38" t="s">
-        <v>151</v>
-      </c>
-      <c r="G38" t="s">
-        <v>132</v>
-      </c>
-      <c r="H38" t="s">
-        <v>114</v>
-      </c>
-      <c r="I38" t="s">
-        <v>96</v>
-      </c>
-      <c r="J38" s="4">
-        <v>0.57699999999999996</v>
-      </c>
-      <c r="M38" s="5">
-        <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
-        <v>5.1929999999999996</v>
-      </c>
-    </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A39" s="2" t="s">
+      <c r="D39" t="s">
+        <v>84</v>
+      </c>
+      <c r="E39" t="s">
         <v>85</v>
       </c>
-      <c r="B39">
-        <v>3</v>
-      </c>
-      <c r="C39" t="s">
+      <c r="F39" t="s">
         <v>86</v>
       </c>
-      <c r="D39" t="s">
-        <v>86</v>
-      </c>
-      <c r="E39" t="s">
-        <v>149</v>
-      </c>
       <c r="G39" s="3" t="s">
-        <v>108</v>
+        <v>87</v>
       </c>
       <c r="H39" t="s">
-        <v>109</v>
-      </c>
-      <c r="I39" t="s">
-        <v>96</v>
-      </c>
-      <c r="J39" s="4">
-        <v>1.96</v>
-      </c>
-      <c r="M39" s="5">
-        <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
-        <v>5.88</v>
-      </c>
-    </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+      <c r="I39" s="4">
+        <v>0.81</v>
+      </c>
+      <c r="L39" s="5">
+        <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
+        <v>0.81</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B40">
         <v>1</v>
       </c>
       <c r="C40" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D40" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E40" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="F40" t="s">
-        <v>90</v>
+        <v>169</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="H40" t="s">
-        <v>103</v>
-      </c>
-      <c r="I40" t="s">
-        <v>96</v>
-      </c>
-      <c r="J40" s="4">
-        <v>0.81</v>
-      </c>
-      <c r="M40" s="5">
-        <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
-        <v>0.81</v>
-      </c>
-    </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+      <c r="H40" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="I40" s="4">
+        <v>9.61</v>
+      </c>
+      <c r="L40" s="5">
+        <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
+        <v>9.61</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>92</v>
+        <v>145</v>
       </c>
       <c r="B41">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C41" t="s">
-        <v>93</v>
+        <v>146</v>
       </c>
       <c r="D41" t="s">
-        <v>93</v>
+        <v>161</v>
       </c>
       <c r="E41" t="s">
-        <v>94</v>
+        <v>147</v>
       </c>
       <c r="F41" t="s">
-        <v>177</v>
-      </c>
-      <c r="G41" s="3" t="s">
-        <v>104</v>
+        <v>150</v>
+      </c>
+      <c r="G41" t="s">
+        <v>148</v>
       </c>
       <c r="H41" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="I41" t="s">
-        <v>96</v>
-      </c>
-      <c r="J41" s="4">
-        <v>9.61</v>
-      </c>
-      <c r="M41" s="5">
-        <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
-        <v>9.61</v>
-      </c>
-    </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A42" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="B42">
-        <v>4</v>
-      </c>
-      <c r="C42" t="s">
-        <v>153</v>
-      </c>
-      <c r="D42" t="s">
-        <v>169</v>
-      </c>
-      <c r="E42" t="s">
-        <v>154</v>
-      </c>
-      <c r="F42" t="s">
-        <v>157</v>
-      </c>
-      <c r="G42" t="s">
-        <v>155</v>
-      </c>
-      <c r="H42" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="I42" t="s">
-        <v>96</v>
-      </c>
-      <c r="J42" s="4">
+        <v>149</v>
+      </c>
+      <c r="I41" s="4">
         <v>1.71</v>
       </c>
-      <c r="M42" s="5">
+      <c r="L41" s="5">
         <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
         <v>6.84</v>
       </c>
@@ -2739,29 +2719,32 @@
   </sheetData>
   <phoneticPr fontId="19" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="H24" r:id="rId1" xr:uid="{DD8AD352-FB06-4715-B587-8B7434FCD99F}"/>
-    <hyperlink ref="G26" r:id="rId2" xr:uid="{5EFE7EEC-7A33-4705-B297-C4BD3E05DA2C}"/>
-    <hyperlink ref="G40" r:id="rId3" xr:uid="{71FE485A-AA2E-4950-BE10-E132C884D307}"/>
-    <hyperlink ref="K21" r:id="rId4" xr:uid="{DB18BABB-D85D-4D81-84B1-06B4803F7A71}"/>
-    <hyperlink ref="G18" r:id="rId5" xr:uid="{6E03D079-3A0C-4BF5-810D-97558264CB66}"/>
-    <hyperlink ref="G19" r:id="rId6" xr:uid="{7C702CAB-8E1E-429C-9A90-1E47838C9BF7}"/>
-    <hyperlink ref="G39" r:id="rId7" xr:uid="{ACFE634D-160F-4B71-8DB2-7FFC85727160}"/>
-    <hyperlink ref="H25" r:id="rId8" xr:uid="{7C8D1661-4DCD-43AD-B870-FF77BABDB784}"/>
-    <hyperlink ref="H21" r:id="rId9" xr:uid="{257864EB-78CF-4B88-864D-5BF4D3EC4937}"/>
-    <hyperlink ref="O21" r:id="rId10" xr:uid="{438620CA-1198-495F-B2D1-DE18D03FD0CF}"/>
-    <hyperlink ref="H26" r:id="rId11" xr:uid="{50608FB6-E114-4108-91A8-FC7B919453D0}"/>
-    <hyperlink ref="H42" r:id="rId12" xr:uid="{8161F553-B981-424E-8CA4-DA1BB9415ECC}"/>
+    <hyperlink ref="H23" r:id="rId1" xr:uid="{DD8AD352-FB06-4715-B587-8B7434FCD99F}"/>
+    <hyperlink ref="G25" r:id="rId2" xr:uid="{5EFE7EEC-7A33-4705-B297-C4BD3E05DA2C}"/>
+    <hyperlink ref="G39" r:id="rId3" xr:uid="{71FE485A-AA2E-4950-BE10-E132C884D307}"/>
+    <hyperlink ref="J20" r:id="rId4" xr:uid="{DB18BABB-D85D-4D81-84B1-06B4803F7A71}"/>
+    <hyperlink ref="G17" r:id="rId5" xr:uid="{6E03D079-3A0C-4BF5-810D-97558264CB66}"/>
+    <hyperlink ref="G18" r:id="rId6" xr:uid="{7C702CAB-8E1E-429C-9A90-1E47838C9BF7}"/>
+    <hyperlink ref="G38" r:id="rId7" xr:uid="{ACFE634D-160F-4B71-8DB2-7FFC85727160}"/>
+    <hyperlink ref="H24" r:id="rId8" xr:uid="{7C8D1661-4DCD-43AD-B870-FF77BABDB784}"/>
+    <hyperlink ref="H20" r:id="rId9" xr:uid="{257864EB-78CF-4B88-864D-5BF4D3EC4937}"/>
+    <hyperlink ref="N20" r:id="rId10" xr:uid="{438620CA-1198-495F-B2D1-DE18D03FD0CF}"/>
+    <hyperlink ref="H25" r:id="rId11" xr:uid="{50608FB6-E114-4108-91A8-FC7B919453D0}"/>
+    <hyperlink ref="H41" r:id="rId12" xr:uid="{8161F553-B981-424E-8CA4-DA1BB9415ECC}"/>
     <hyperlink ref="H8" r:id="rId13" xr:uid="{9431E3EC-4579-4581-9011-6B05F37CF302}"/>
-    <hyperlink ref="G41" r:id="rId14" xr:uid="{6235F029-DC34-40F5-B3C4-8045E09C4F42}"/>
-    <hyperlink ref="K8" r:id="rId15" xr:uid="{71E59B7F-99D7-40E9-B1FE-1FF9731CAD3F}"/>
-    <hyperlink ref="G17" r:id="rId16" xr:uid="{6C3216AC-996C-4C4E-A7C7-D6FD12DC9E06}"/>
-    <hyperlink ref="H41" r:id="rId17" xr:uid="{89885BDB-09BB-4D47-9D07-262D9AE4373B}"/>
-    <hyperlink ref="H15" r:id="rId18" xr:uid="{81319735-1B12-4848-AD96-716F6B41299B}"/>
+    <hyperlink ref="G40" r:id="rId14" xr:uid="{6235F029-DC34-40F5-B3C4-8045E09C4F42}"/>
+    <hyperlink ref="J8" r:id="rId15" xr:uid="{71E59B7F-99D7-40E9-B1FE-1FF9731CAD3F}"/>
+    <hyperlink ref="G16" r:id="rId16" xr:uid="{6C3216AC-996C-4C4E-A7C7-D6FD12DC9E06}"/>
+    <hyperlink ref="H40" r:id="rId17" xr:uid="{89885BDB-09BB-4D47-9D07-262D9AE4373B}"/>
+    <hyperlink ref="H14" r:id="rId18" xr:uid="{81319735-1B12-4848-AD96-716F6B41299B}"/>
+    <hyperlink ref="H29" r:id="rId19" display="https://www.digikey.ca/en/products/detail/vishay-dale/CRCW08053M48FKEA/1176076?s=N4IgjCBcpgbFoDGUBmBDANgZwKYBoQB7KAbRAGYBOcgJkpAF0CAHAFyhAGVWAnASwB2AcxABfAjQAMADgCsCEGw4BVAX1YB5FAFkcaLAFceOEAQMdtGgBYBbLKZA3BHcgDoALNIc20ADxceXuIgALQ0CsiQvAb4RKQg8gyiweGQZMZYfFishDyMBPDQIHwAJhwhYJIQLOyQIA6sAJ7MJnX6yMlAA" xr:uid="{8E5F6979-FDC7-47E4-9BCE-FC35F6839D40}"/>
+    <hyperlink ref="H21" r:id="rId20" xr:uid="{DCC66DF8-398A-435E-A130-E4BD0B18F19E}"/>
+    <hyperlink ref="H22" r:id="rId21" xr:uid="{9F88BFCE-59FC-4E77-AC2A-F787549E61AD}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId19"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId22"/>
   <tableParts count="1">
-    <tablePart r:id="rId20"/>
+    <tablePart r:id="rId23"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
This contains a completed BOM, Still need to create the Inductor footprint and add sponsor names/logo, then can get into retracing this sucker
</commit_message>
<xml_diff>
--- a/RADSAT-SK Timer/RADSAT-SK Timer.xlsx
+++ b/RADSAT-SK Timer/RADSAT-SK Timer.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\USST\power-and-electrical\RADSAT-SK Timer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5A7941E-CD93-451F-988F-CB4F06C61ABB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14E0510D-FA89-4151-A389-422153548DC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-3000" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RADSAT-SK Timer" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="194">
   <si>
     <t>Source:</t>
   </si>
@@ -507,9 +507,6 @@
     <t>https://www.mouser.ca/ProductDetail/Panasonic-Industrial-Devices/CR-2025-F2N?qs=FNor9lU6pf%2F%2FKr9xpq%252B%252BCQ%3D%3D</t>
   </si>
   <si>
-    <t>https://www.digikey.ca/en/products/detail/keystone-electronics/1061/303558</t>
-  </si>
-  <si>
     <t>BATT HLDR COIN 20MM 1/2 CEL SMD</t>
   </si>
   <si>
@@ -534,22 +531,6 @@
     <t>3M</t>
   </si>
   <si>
-    <r>
-      <t>Battery:BatteryHolder_Keystone_1060_1x2032</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>*** NEED TO EDIT***</t>
-    </r>
-  </si>
-  <si>
     <t>Diode_SMD:D_SMC_Handsoldering</t>
   </si>
   <si>
@@ -619,10 +600,19 @@
     <t>https://www.digikey.ca/en/products/detail/hirose-electric-co-ltd/DF13-3P-1-25V-75/9170629</t>
   </si>
   <si>
-    <t>m</t>
-  </si>
-  <si>
     <t>Column1</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/vishay-general-semiconductor-diodes-division/BZX884B5V6L-G3-08/14312759</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/keystone-electronics/1060TR/303557</t>
+  </si>
+  <si>
+    <t>Battery:BatteryHolder_Keystone_1060_1x2032</t>
   </si>
 </sst>
 </file>
@@ -1206,8 +1196,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A7:M41" totalsRowShown="0">
-  <autoFilter ref="A7:M41" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A7:M42" totalsRowShown="0">
+  <autoFilter ref="A7:M42" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Ref" dataDxfId="1"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Qnty"/>
@@ -1526,12 +1516,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N41"/>
+  <dimension ref="A1:N42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <pane xSplit="8670" topLeftCell="H1" activePane="topRight"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <pane xSplit="8670" topLeftCell="G1" activePane="topRight"/>
       <selection activeCell="C6" sqref="C6"/>
-      <selection pane="topRight" activeCell="H19" sqref="H19"/>
+      <selection pane="topRight" activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1595,8 +1585,8 @@
         <v>101</v>
       </c>
       <c r="B6" s="5">
-        <f>SUM(L8:L41)</f>
-        <v>85.551999999999992</v>
+        <f>SUM(L8:L42)</f>
+        <v>81.611999999999995</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -1637,7 +1627,7 @@
         <v>102</v>
       </c>
       <c r="M7" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
@@ -1654,19 +1644,19 @@
         <v>15</v>
       </c>
       <c r="E8" t="s">
-        <v>167</v>
+        <v>193</v>
       </c>
       <c r="F8" t="s">
+        <v>158</v>
+      </c>
+      <c r="G8" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="G8" t="s">
-        <v>160</v>
-      </c>
       <c r="H8" s="3" t="s">
-        <v>158</v>
+        <v>192</v>
       </c>
       <c r="I8" s="4">
-        <v>4.09</v>
+        <v>2.12</v>
       </c>
       <c r="J8" s="3" t="s">
         <v>157</v>
@@ -1676,7 +1666,7 @@
       </c>
       <c r="L8" s="5">
         <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
-        <v>11.4</v>
+        <v>7.4600000000000009</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
@@ -1711,7 +1701,7 @@
     </row>
     <row r="10" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B10">
         <v>9</v>
@@ -1729,7 +1719,7 @@
         <v>22</v>
       </c>
       <c r="H10" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="I10" s="4">
         <v>0.15</v>
@@ -1792,7 +1782,7 @@
         <v>22</v>
       </c>
       <c r="H12" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="I12" s="4">
         <v>0.41</v>
@@ -1837,7 +1827,7 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -1855,7 +1845,7 @@
         <v>155</v>
       </c>
       <c r="G14" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="H14" s="3" t="s">
         <v>156</v>
@@ -1870,7 +1860,7 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -1885,10 +1875,10 @@
         <v>140</v>
       </c>
       <c r="F15" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="I15" s="4">
         <v>0.33</v>
@@ -1906,25 +1896,28 @@
         <v>1</v>
       </c>
       <c r="C16" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D16" t="s">
         <v>31</v>
       </c>
       <c r="E16" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="F16" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H16" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="I16" s="4">
         <v>2.33</v>
+      </c>
+      <c r="J16" t="s">
+        <v>191</v>
       </c>
       <c r="L16" s="5">
         <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
@@ -2117,7 +2110,7 @@
         <v>46</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="I22" s="4">
         <v>0.59</v>
@@ -2179,7 +2172,7 @@
       <c r="F24" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="G24" t="s">
+      <c r="G24" s="3" t="s">
         <v>119</v>
       </c>
       <c r="H24" s="3" t="s">
@@ -2195,7 +2188,7 @@
     </row>
     <row r="25" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B25">
         <v>14</v>
@@ -2224,9 +2217,6 @@
       <c r="L25" s="5">
         <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
         <v>8.82</v>
-      </c>
-      <c r="M25" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="26" spans="1:14" ht="30" x14ac:dyDescent="0.25">
@@ -2249,7 +2239,7 @@
         <v>63</v>
       </c>
       <c r="H26" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="I26" s="4">
         <v>2.9000000000000001E-2</v>
@@ -2261,7 +2251,7 @@
     </row>
     <row r="27" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B27">
         <v>11</v>
@@ -2291,7 +2281,7 @@
     </row>
     <row r="28" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B28">
         <v>21</v>
@@ -2309,7 +2299,7 @@
         <v>63</v>
       </c>
       <c r="H28" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="I28" s="4">
         <v>2.9000000000000001E-2</v>
@@ -2339,7 +2329,7 @@
         <v>63</v>
       </c>
       <c r="H29" s="3" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="I29" s="4">
         <v>0.15</v>
@@ -2369,7 +2359,7 @@
         <v>63</v>
       </c>
       <c r="H30" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="I30" s="4">
         <v>0.15</v>
@@ -2399,7 +2389,7 @@
         <v>63</v>
       </c>
       <c r="H31" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="I31" s="4">
         <v>0.15</v>
@@ -2417,7 +2407,7 @@
         <v>1</v>
       </c>
       <c r="C32" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D32" t="s">
         <v>61</v>
@@ -2454,7 +2444,7 @@
         <v>63</v>
       </c>
       <c r="H33" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="I33" s="4">
         <v>0.15</v>
@@ -2484,7 +2474,7 @@
         <v>63</v>
       </c>
       <c r="H34" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="I34" s="4">
         <v>0.15</v>
@@ -2514,7 +2504,7 @@
         <v>63</v>
       </c>
       <c r="H35" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="I35" s="4">
         <v>0.15</v>
@@ -2544,7 +2534,7 @@
         <v>63</v>
       </c>
       <c r="H36" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="I36" s="4">
         <v>0.15</v>
@@ -2667,7 +2657,7 @@
         <v>90</v>
       </c>
       <c r="F40" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="G40" s="3" t="s">
         <v>99</v>
@@ -2694,7 +2684,7 @@
         <v>146</v>
       </c>
       <c r="D41" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E41" t="s">
         <v>147</v>
@@ -2714,6 +2704,19 @@
       <c r="L41" s="5">
         <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
         <v>6.84</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D42" t="s">
+        <v>190</v>
+      </c>
+      <c r="E42" t="s">
+        <v>190</v>
+      </c>
+      <c r="I42" s="4"/>
+      <c r="L42" s="5">
+        <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2740,11 +2743,13 @@
     <hyperlink ref="H29" r:id="rId19" display="https://www.digikey.ca/en/products/detail/vishay-dale/CRCW08053M48FKEA/1176076?s=N4IgjCBcpgbFoDGUBmBDANgZwKYBoQB7KAbRAGYBOcgJkpAF0CAHAFyhAGVWAnASwB2AcxABfAjQAMADgCsCEGw4BVAX1YB5FAFkcaLAFceOEAQMdtGgBYBbLKZA3BHcgDoALNIc20ADxceXuIgALQ0CsiQvAb4RKQg8gyiweGQZMZYfFishDyMBPDQIHwAJhwhYJIQLOyQIA6sAJ7MJnX6yMlAA" xr:uid="{8E5F6979-FDC7-47E4-9BCE-FC35F6839D40}"/>
     <hyperlink ref="H21" r:id="rId20" xr:uid="{DCC66DF8-398A-435E-A130-E4BD0B18F19E}"/>
     <hyperlink ref="H22" r:id="rId21" xr:uid="{9F88BFCE-59FC-4E77-AC2A-F787549E61AD}"/>
+    <hyperlink ref="G8" r:id="rId22" xr:uid="{7EF7B759-262D-46EA-A639-06793509DE1D}"/>
+    <hyperlink ref="G24" r:id="rId23" xr:uid="{3168245F-C5D1-4FC5-9A41-850D03AE3A38}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId22"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId24"/>
   <tableParts count="1">
-    <tablePart r:id="rId23"/>
+    <tablePart r:id="rId25"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Made changes to accomadate the RBF alternate charge plug
</commit_message>
<xml_diff>
--- a/RADSAT-SK Timer/RADSAT-SK Timer.xlsx
+++ b/RADSAT-SK Timer/RADSAT-SK Timer.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\USST\power-and-electrical\RADSAT-SK Timer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14E0510D-FA89-4151-A389-422153548DC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB5C3CC6-5F83-4610-A985-3F07C4E6EF84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -180,9 +180,6 @@
     <t>Connector_Hirose:Hirose_DF13-02P-1.25DSA_1x02_P1.25mm_Vertical</t>
   </si>
   <si>
-    <t xml:space="preserve">J210, </t>
-  </si>
-  <si>
     <t>ZX62WRD-B-5PC</t>
   </si>
   <si>
@@ -613,6 +610,9 @@
   </si>
   <si>
     <t>Battery:BatteryHolder_Keystone_1060_1x2032</t>
+  </si>
+  <si>
+    <t>J210, (REMOVED WITH RBF CHARGING PIN)</t>
   </si>
 </sst>
 </file>
@@ -1518,10 +1518,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <pane xSplit="8670" topLeftCell="G1" activePane="topRight"/>
-      <selection activeCell="C6" sqref="C6"/>
-      <selection pane="topRight" activeCell="G28" sqref="G28"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <pane xSplit="8670" topLeftCell="B1"/>
+      <selection activeCell="A23" sqref="A23"/>
+      <selection pane="topRight" activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1553,7 +1553,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -1582,11 +1582,11 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B6" s="5">
         <f>SUM(L8:L42)</f>
-        <v>81.611999999999995</v>
+        <v>79.852000000000004</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -1606,28 +1606,28 @@
         <v>12</v>
       </c>
       <c r="F7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="I7" t="s">
         <v>13</v>
       </c>
       <c r="J7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="K7" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="L7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="M7" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
@@ -1644,22 +1644,22 @@
         <v>15</v>
       </c>
       <c r="E8" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="F8" t="s">
+        <v>157</v>
+      </c>
+      <c r="G8" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="G8" s="3" t="s">
-        <v>159</v>
-      </c>
       <c r="H8" s="3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I8" s="4">
         <v>2.12</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="K8" s="4">
         <v>1.61</v>
@@ -1683,13 +1683,13 @@
         <v>18</v>
       </c>
       <c r="E9" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H9" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="I9" s="4">
         <v>3.36</v>
@@ -1701,7 +1701,7 @@
     </row>
     <row r="10" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B10">
         <v>9</v>
@@ -1719,7 +1719,7 @@
         <v>22</v>
       </c>
       <c r="H10" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="I10" s="4">
         <v>0.15</v>
@@ -1746,13 +1746,13 @@
         <v>21</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G11" t="s">
+        <v>130</v>
+      </c>
+      <c r="H11" t="s">
         <v>131</v>
-      </c>
-      <c r="H11" t="s">
-        <v>132</v>
       </c>
       <c r="I11" s="4">
         <v>0.41</v>
@@ -1782,7 +1782,7 @@
         <v>22</v>
       </c>
       <c r="H12" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="I12" s="4">
         <v>0.41</v>
@@ -1806,16 +1806,16 @@
         <v>20</v>
       </c>
       <c r="E13" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F13" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="G13" t="s">
         <v>127</v>
       </c>
-      <c r="G13" t="s">
+      <c r="H13" t="s">
         <v>128</v>
-      </c>
-      <c r="H13" t="s">
-        <v>129</v>
       </c>
       <c r="I13" s="4">
         <v>1.0900000000000001</v>
@@ -1827,7 +1827,7 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -1839,16 +1839,16 @@
         <v>29</v>
       </c>
       <c r="E14" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F14" t="s">
+        <v>154</v>
+      </c>
+      <c r="G14" t="s">
+        <v>173</v>
+      </c>
+      <c r="H14" s="3" t="s">
         <v>155</v>
-      </c>
-      <c r="G14" t="s">
-        <v>174</v>
-      </c>
-      <c r="H14" s="3" t="s">
-        <v>156</v>
       </c>
       <c r="I14" s="4">
         <v>0.33</v>
@@ -1860,7 +1860,7 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -1872,13 +1872,13 @@
         <v>29</v>
       </c>
       <c r="E15" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F15" t="s">
+        <v>171</v>
+      </c>
+      <c r="H15" s="3" t="s">
         <v>172</v>
-      </c>
-      <c r="H15" s="3" t="s">
-        <v>173</v>
       </c>
       <c r="I15" s="4">
         <v>0.33</v>
@@ -1896,28 +1896,28 @@
         <v>1</v>
       </c>
       <c r="C16" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D16" t="s">
         <v>31</v>
       </c>
       <c r="E16" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F16" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="H16" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="I16" s="4">
         <v>2.33</v>
       </c>
       <c r="J16" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="L16" s="5">
         <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
@@ -1932,22 +1932,22 @@
         <v>1</v>
       </c>
       <c r="C17" t="s">
+        <v>114</v>
+      </c>
+      <c r="D17" t="s">
         <v>115</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
         <v>116</v>
       </c>
-      <c r="E17" t="s">
-        <v>117</v>
-      </c>
       <c r="F17" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G17" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="H17" t="s">
         <v>113</v>
-      </c>
-      <c r="H17" t="s">
-        <v>114</v>
       </c>
       <c r="I17" s="4">
         <v>0.76</v>
@@ -1959,28 +1959,28 @@
     </row>
     <row r="18" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B18">
         <v>1</v>
       </c>
       <c r="C18" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="D18" t="s">
+        <v>134</v>
+      </c>
+      <c r="E18" t="s">
         <v>135</v>
       </c>
-      <c r="D18" t="s">
-        <v>135</v>
-      </c>
-      <c r="E18" t="s">
+      <c r="F18" t="s">
         <v>136</v>
       </c>
-      <c r="F18" t="s">
+      <c r="G18" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="G18" s="3" t="s">
+      <c r="H18" t="s">
         <v>138</v>
-      </c>
-      <c r="H18" t="s">
-        <v>139</v>
       </c>
       <c r="I18" s="4">
         <v>0.55000000000000004</v>
@@ -2007,7 +2007,7 @@
         <v>35</v>
       </c>
       <c r="F19" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="I19" s="4"/>
       <c r="L19" s="5">
@@ -2015,7 +2015,7 @@
         <v>0</v>
       </c>
       <c r="N19" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
@@ -2035,16 +2035,16 @@
         <v>38</v>
       </c>
       <c r="F20" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I20" s="4">
         <v>0.61</v>
       </c>
       <c r="J20" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="K20" s="4">
         <v>0.52</v>
@@ -2054,7 +2054,7 @@
         <v>1.1299999999999999</v>
       </c>
       <c r="N20" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
@@ -2077,10 +2077,10 @@
         <v>42</v>
       </c>
       <c r="G21" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I21" s="4">
         <v>0.59299999999999997</v>
@@ -2110,7 +2110,7 @@
         <v>46</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="I22" s="4">
         <v>0.59</v>
@@ -2120,63 +2120,63 @@
         <v>0.59</v>
       </c>
       <c r="N22" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="B23">
+        <v>0</v>
+      </c>
+      <c r="C23" t="s">
         <v>49</v>
       </c>
-      <c r="B23">
-        <v>1</v>
-      </c>
-      <c r="C23" t="s">
+      <c r="D23" t="s">
+        <v>49</v>
+      </c>
+      <c r="E23" t="s">
         <v>50</v>
       </c>
-      <c r="D23" t="s">
-        <v>50</v>
-      </c>
-      <c r="E23" t="s">
+      <c r="F23" t="s">
+        <v>117</v>
+      </c>
+      <c r="H23" s="3" t="s">
         <v>51</v>
-      </c>
-      <c r="F23" t="s">
-        <v>118</v>
-      </c>
-      <c r="H23" s="3" t="s">
-        <v>52</v>
       </c>
       <c r="I23" s="4">
         <v>1.76</v>
       </c>
       <c r="L23" s="5">
         <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
-        <v>1.76</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B24">
         <v>1</v>
       </c>
       <c r="C24" t="s">
+        <v>53</v>
+      </c>
+      <c r="D24" t="s">
         <v>54</v>
       </c>
-      <c r="D24" t="s">
-        <v>55</v>
-      </c>
       <c r="E24" s="6" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G24" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="H24" s="3" t="s">
         <v>119</v>
-      </c>
-      <c r="H24" s="3" t="s">
-        <v>120</v>
       </c>
       <c r="I24" s="4">
         <v>1.48</v>
@@ -2188,28 +2188,28 @@
     </row>
     <row r="25" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B25">
         <v>14</v>
       </c>
       <c r="C25" t="s">
+        <v>55</v>
+      </c>
+      <c r="D25" t="s">
+        <v>55</v>
+      </c>
+      <c r="E25" t="s">
+        <v>140</v>
+      </c>
+      <c r="F25" t="s">
         <v>56</v>
       </c>
-      <c r="D25" t="s">
-        <v>56</v>
-      </c>
-      <c r="E25" t="s">
-        <v>141</v>
-      </c>
-      <c r="F25" t="s">
+      <c r="G25" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="G25" s="3" t="s">
-        <v>58</v>
-      </c>
       <c r="H25" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I25" s="4">
         <v>0.63</v>
@@ -2221,25 +2221,25 @@
     </row>
     <row r="26" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B26">
         <v>10</v>
       </c>
       <c r="C26" t="s">
+        <v>59</v>
+      </c>
+      <c r="D26" t="s">
         <v>60</v>
       </c>
-      <c r="D26" t="s">
+      <c r="E26" t="s">
         <v>61</v>
       </c>
-      <c r="E26" t="s">
+      <c r="F26" t="s">
         <v>62</v>
       </c>
-      <c r="F26" t="s">
-        <v>63</v>
-      </c>
       <c r="H26" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="I26" s="4">
         <v>2.9000000000000001E-2</v>
@@ -2251,7 +2251,7 @@
     </row>
     <row r="27" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B27">
         <v>11</v>
@@ -2260,16 +2260,16 @@
         <v>100</v>
       </c>
       <c r="D27" t="s">
+        <v>60</v>
+      </c>
+      <c r="E27" t="s">
         <v>61</v>
       </c>
-      <c r="E27" t="s">
+      <c r="F27" t="s">
         <v>62</v>
       </c>
-      <c r="F27" t="s">
-        <v>63</v>
-      </c>
       <c r="H27" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="I27" s="4">
         <v>0.107</v>
@@ -2281,25 +2281,25 @@
     </row>
     <row r="28" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B28">
         <v>21</v>
       </c>
       <c r="C28" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D28" t="s">
+        <v>60</v>
+      </c>
+      <c r="E28" t="s">
         <v>61</v>
       </c>
-      <c r="E28" t="s">
+      <c r="F28" t="s">
         <v>62</v>
       </c>
-      <c r="F28" t="s">
-        <v>63</v>
-      </c>
       <c r="H28" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I28" s="4">
         <v>2.9000000000000001E-2</v>
@@ -2311,25 +2311,25 @@
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B29">
         <v>3</v>
       </c>
       <c r="C29" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D29" t="s">
+        <v>60</v>
+      </c>
+      <c r="E29" t="s">
         <v>61</v>
       </c>
-      <c r="E29" t="s">
+      <c r="F29" t="s">
         <v>62</v>
       </c>
-      <c r="F29" t="s">
-        <v>63</v>
-      </c>
       <c r="H29" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I29" s="4">
         <v>0.15</v>
@@ -2341,25 +2341,25 @@
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B30">
         <v>3</v>
       </c>
       <c r="C30" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D30" t="s">
+        <v>60</v>
+      </c>
+      <c r="E30" t="s">
         <v>61</v>
       </c>
-      <c r="E30" t="s">
+      <c r="F30" t="s">
         <v>62</v>
       </c>
-      <c r="F30" t="s">
-        <v>63</v>
-      </c>
       <c r="H30" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I30" s="4">
         <v>0.15</v>
@@ -2371,25 +2371,25 @@
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B31">
         <v>1</v>
       </c>
       <c r="C31" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D31" t="s">
+        <v>60</v>
+      </c>
+      <c r="E31" t="s">
         <v>61</v>
       </c>
-      <c r="E31" t="s">
+      <c r="F31" t="s">
         <v>62</v>
       </c>
-      <c r="F31" t="s">
-        <v>63</v>
-      </c>
       <c r="H31" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I31" s="4">
         <v>0.15</v>
@@ -2401,22 +2401,22 @@
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B32">
         <v>1</v>
       </c>
       <c r="C32" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D32" t="s">
+        <v>60</v>
+      </c>
+      <c r="E32" t="s">
         <v>61</v>
       </c>
-      <c r="E32" t="s">
+      <c r="F32" t="s">
         <v>62</v>
-      </c>
-      <c r="F32" t="s">
-        <v>63</v>
       </c>
       <c r="I32" s="4"/>
       <c r="L32" s="5">
@@ -2426,25 +2426,25 @@
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B33">
         <v>1</v>
       </c>
       <c r="C33" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D33" t="s">
+        <v>60</v>
+      </c>
+      <c r="E33" t="s">
         <v>61</v>
       </c>
-      <c r="E33" t="s">
+      <c r="F33" t="s">
         <v>62</v>
       </c>
-      <c r="F33" t="s">
-        <v>63</v>
-      </c>
       <c r="H33" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="I33" s="4">
         <v>0.15</v>
@@ -2456,25 +2456,25 @@
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B34">
         <v>1</v>
       </c>
       <c r="C34" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D34" t="s">
+        <v>60</v>
+      </c>
+      <c r="E34" t="s">
         <v>61</v>
       </c>
-      <c r="E34" t="s">
+      <c r="F34" t="s">
         <v>62</v>
       </c>
-      <c r="F34" t="s">
-        <v>63</v>
-      </c>
       <c r="H34" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="I34" s="4">
         <v>0.15</v>
@@ -2486,25 +2486,25 @@
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B35">
         <v>1</v>
       </c>
       <c r="C35" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D35" t="s">
+        <v>60</v>
+      </c>
+      <c r="E35" t="s">
         <v>61</v>
       </c>
-      <c r="E35" t="s">
+      <c r="F35" t="s">
         <v>62</v>
       </c>
-      <c r="F35" t="s">
-        <v>63</v>
-      </c>
       <c r="H35" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="I35" s="4">
         <v>0.15</v>
@@ -2516,25 +2516,25 @@
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B36">
         <v>1</v>
       </c>
       <c r="C36" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D36" t="s">
+        <v>60</v>
+      </c>
+      <c r="E36" t="s">
         <v>61</v>
       </c>
-      <c r="E36" t="s">
+      <c r="F36" t="s">
         <v>62</v>
       </c>
-      <c r="F36" t="s">
-        <v>63</v>
-      </c>
       <c r="H36" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I36" s="4">
         <v>0.15</v>
@@ -2546,13 +2546,13 @@
     </row>
     <row r="37" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B37">
         <v>9</v>
       </c>
       <c r="C37" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D37" t="s">
         <v>47</v>
@@ -2561,13 +2561,13 @@
         <v>48</v>
       </c>
       <c r="F37" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G37" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="H37" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I37" s="4">
         <v>0.57699999999999996</v>
@@ -2579,25 +2579,25 @@
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B38">
         <v>3</v>
       </c>
       <c r="C38" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D38" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E38" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G38" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="H38" t="s">
         <v>103</v>
-      </c>
-      <c r="H38" t="s">
-        <v>104</v>
       </c>
       <c r="I38" s="4">
         <v>1.96</v>
@@ -2609,28 +2609,28 @@
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B39">
         <v>1</v>
       </c>
       <c r="C39" t="s">
+        <v>83</v>
+      </c>
+      <c r="D39" t="s">
+        <v>83</v>
+      </c>
+      <c r="E39" t="s">
         <v>84</v>
       </c>
-      <c r="D39" t="s">
-        <v>84</v>
-      </c>
-      <c r="E39" t="s">
+      <c r="F39" t="s">
         <v>85</v>
       </c>
-      <c r="F39" t="s">
+      <c r="G39" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="G39" s="3" t="s">
-        <v>87</v>
-      </c>
       <c r="H39" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I39" s="4">
         <v>0.81</v>
@@ -2642,28 +2642,28 @@
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B40">
         <v>1</v>
       </c>
       <c r="C40" t="s">
+        <v>88</v>
+      </c>
+      <c r="D40" t="s">
+        <v>88</v>
+      </c>
+      <c r="E40" t="s">
         <v>89</v>
       </c>
-      <c r="D40" t="s">
-        <v>89</v>
-      </c>
-      <c r="E40" t="s">
-        <v>90</v>
-      </c>
       <c r="F40" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="G40" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="H40" s="3" t="s">
         <v>99</v>
-      </c>
-      <c r="H40" s="3" t="s">
-        <v>100</v>
       </c>
       <c r="I40" s="4">
         <v>9.61</v>
@@ -2675,28 +2675,28 @@
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B41">
         <v>4</v>
       </c>
       <c r="C41" t="s">
+        <v>145</v>
+      </c>
+      <c r="D41" t="s">
+        <v>159</v>
+      </c>
+      <c r="E41" t="s">
         <v>146</v>
       </c>
-      <c r="D41" t="s">
-        <v>160</v>
-      </c>
-      <c r="E41" t="s">
+      <c r="F41" t="s">
+        <v>149</v>
+      </c>
+      <c r="G41" t="s">
         <v>147</v>
       </c>
-      <c r="F41" t="s">
-        <v>150</v>
-      </c>
-      <c r="G41" t="s">
+      <c r="H41" s="3" t="s">
         <v>148</v>
-      </c>
-      <c r="H41" s="3" t="s">
-        <v>149</v>
       </c>
       <c r="I41" s="4">
         <v>1.71</v>
@@ -2708,10 +2708,10 @@
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D42" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E42" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="I42" s="4"/>
       <c r="L42" s="5">

</xml_diff>

<commit_message>
RBF Circuit was modified and new components added to BOM
</commit_message>
<xml_diff>
--- a/RADSAT-SK Timer/RADSAT-SK Timer.xlsx
+++ b/RADSAT-SK Timer/RADSAT-SK Timer.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\USST\power-and-electrical\RADSAT-SK Timer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB5C3CC6-5F83-4610-A985-3F07C4E6EF84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC13FC79-4541-460B-BB97-034F9A7F0CD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-3000" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RADSAT-SK Timer" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="195">
   <si>
     <t>Source:</t>
   </si>
@@ -207,9 +207,6 @@
     <t>https://www.infineon.com/dgdl/irlml2060pbf.pdf?fileId=5546d462533600a401535664b7fb25ee</t>
   </si>
   <si>
-    <t xml:space="preserve">R101, R103, R107, R113, R114, R117, R118, R124, R126, R203, </t>
-  </si>
-  <si>
     <t>1M</t>
   </si>
   <si>
@@ -366,9 +363,6 @@
     <t>https://www.mouser.ca/datasheet/2/185/DF13_Catalog_D31687_en-2486995.pdf</t>
   </si>
   <si>
-    <t>no vertical through hole?</t>
-  </si>
-  <si>
     <t>https://www.onsemi.com/pdf/datasheet/mbrm120l-d.pdf</t>
   </si>
   <si>
@@ -534,12 +528,6 @@
     <t xml:space="preserve">Buck-Boost Switching Regulator IC Positive Adjustable 2.5V 1 Output 600mA </t>
   </si>
   <si>
-    <t>Q101, Q102, Q103, Q104, Q105, Q106, Q107, Q108, Q109, Q201, Q202, Q204, Q205, Q206</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R102, R111, R115, R116, R133, R134, R202, R204, R211, R213, R215, </t>
-  </si>
-  <si>
     <t>D206</t>
   </si>
   <si>
@@ -613,6 +601,21 @@
   </si>
   <si>
     <t>J210, (REMOVED WITH RBF CHARGING PIN)</t>
+  </si>
+  <si>
+    <t>Q101, Q102, Q103, Q104, Q105, Q106, Q107, Q108, Q109, Q201, Q202, Q204, Q205, Q206 ,Q207</t>
+  </si>
+  <si>
+    <t>R101, R103, R107, R113, R114, R117, R118, R124, R126, R203, R221</t>
+  </si>
+  <si>
+    <t>R102, R111, R115, R116, R133, R134, R202, R204, R211, R213, R215, R220</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>no vertical through hole  :(</t>
   </si>
 </sst>
 </file>
@@ -1518,10 +1521,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <pane xSplit="8670" topLeftCell="B1"/>
-      <selection activeCell="A23" sqref="A23"/>
-      <selection pane="topRight" activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="8670" activePane="topRight"/>
+      <selection activeCell="C45" sqref="C45"/>
+      <selection pane="topRight" activeCell="O26" sqref="O26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1553,7 +1556,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -1582,11 +1585,11 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B6" s="5">
         <f>SUM(L8:L42)</f>
-        <v>79.852000000000004</v>
+        <v>80.617999999999995</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -1606,28 +1609,28 @@
         <v>12</v>
       </c>
       <c r="F7" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="G7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="I7" t="s">
         <v>13</v>
       </c>
       <c r="J7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="K7" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="L7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="M7" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
@@ -1644,22 +1647,22 @@
         <v>15</v>
       </c>
       <c r="E8" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="F8" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="I8" s="4">
         <v>2.12</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="K8" s="4">
         <v>1.61</v>
@@ -1683,13 +1686,13 @@
         <v>18</v>
       </c>
       <c r="E9" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="F9" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="H9" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="I9" s="4">
         <v>3.36</v>
@@ -1701,7 +1704,7 @@
     </row>
     <row r="10" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="B10">
         <v>9</v>
@@ -1719,7 +1722,7 @@
         <v>22</v>
       </c>
       <c r="H10" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="I10" s="4">
         <v>0.15</v>
@@ -1746,13 +1749,13 @@
         <v>21</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="G11" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="H11" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="I11" s="4">
         <v>0.41</v>
@@ -1782,7 +1785,7 @@
         <v>22</v>
       </c>
       <c r="H12" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="I12" s="4">
         <v>0.41</v>
@@ -1806,16 +1809,16 @@
         <v>20</v>
       </c>
       <c r="E13" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="F13" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="G13" t="s">
+        <v>125</v>
+      </c>
+      <c r="H13" t="s">
         <v>126</v>
-      </c>
-      <c r="G13" t="s">
-        <v>127</v>
-      </c>
-      <c r="H13" t="s">
-        <v>128</v>
       </c>
       <c r="I13" s="4">
         <v>1.0900000000000001</v>
@@ -1827,7 +1830,7 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -1839,16 +1842,16 @@
         <v>29</v>
       </c>
       <c r="E14" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="F14" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="G14" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="I14" s="4">
         <v>0.33</v>
@@ -1860,7 +1863,7 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -1872,13 +1875,13 @@
         <v>29</v>
       </c>
       <c r="E15" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="F15" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="I15" s="4">
         <v>0.33</v>
@@ -1896,28 +1899,28 @@
         <v>1</v>
       </c>
       <c r="C16" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D16" t="s">
         <v>31</v>
       </c>
       <c r="E16" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="F16" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="H16" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="I16" s="4">
         <v>2.33</v>
       </c>
       <c r="J16" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="L16" s="5">
         <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
@@ -1932,22 +1935,22 @@
         <v>1</v>
       </c>
       <c r="C17" t="s">
+        <v>112</v>
+      </c>
+      <c r="D17" t="s">
+        <v>113</v>
+      </c>
+      <c r="E17" t="s">
         <v>114</v>
       </c>
-      <c r="D17" t="s">
-        <v>115</v>
-      </c>
-      <c r="E17" t="s">
-        <v>116</v>
-      </c>
       <c r="F17" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="H17" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="I17" s="4">
         <v>0.76</v>
@@ -1959,28 +1962,28 @@
     </row>
     <row r="18" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B18">
         <v>1</v>
       </c>
       <c r="C18" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="D18" t="s">
+        <v>132</v>
+      </c>
+      <c r="E18" t="s">
+        <v>133</v>
+      </c>
+      <c r="F18" t="s">
         <v>134</v>
       </c>
-      <c r="D18" t="s">
-        <v>134</v>
-      </c>
-      <c r="E18" t="s">
+      <c r="G18" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="F18" t="s">
+      <c r="H18" t="s">
         <v>136</v>
-      </c>
-      <c r="G18" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="H18" t="s">
-        <v>138</v>
       </c>
       <c r="I18" s="4">
         <v>0.55000000000000004</v>
@@ -2007,7 +2010,7 @@
         <v>35</v>
       </c>
       <c r="F19" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="I19" s="4"/>
       <c r="L19" s="5">
@@ -2015,7 +2018,7 @@
         <v>0</v>
       </c>
       <c r="N19" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
@@ -2035,16 +2038,16 @@
         <v>38</v>
       </c>
       <c r="F20" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="I20" s="4">
         <v>0.61</v>
       </c>
       <c r="J20" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="K20" s="4">
         <v>0.52</v>
@@ -2054,7 +2057,7 @@
         <v>1.1299999999999999</v>
       </c>
       <c r="N20" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
@@ -2077,10 +2080,10 @@
         <v>42</v>
       </c>
       <c r="G21" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I21" s="4">
         <v>0.59299999999999997</v>
@@ -2110,7 +2113,7 @@
         <v>46</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="I22" s="4">
         <v>0.59</v>
@@ -2120,12 +2123,12 @@
         <v>0.59</v>
       </c>
       <c r="N22" t="s">
-        <v>111</v>
+        <v>194</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B23">
         <v>0</v>
@@ -2140,7 +2143,7 @@
         <v>50</v>
       </c>
       <c r="F23" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="H23" s="3" t="s">
         <v>51</v>
@@ -2167,16 +2170,16 @@
         <v>54</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="I24" s="4">
         <v>1.48</v>
@@ -2186,12 +2189,12 @@
         <v>1.48</v>
       </c>
     </row>
-    <row r="25" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>167</v>
+        <v>190</v>
       </c>
       <c r="B25">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C25" t="s">
         <v>55</v>
@@ -2200,7 +2203,7 @@
         <v>55</v>
       </c>
       <c r="E25" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F25" t="s">
         <v>56</v>
@@ -2209,97 +2212,97 @@
         <v>57</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I25" s="4">
         <v>0.63</v>
       </c>
       <c r="L25" s="5">
         <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
-        <v>8.82</v>
+        <v>9.4499999999999993</v>
       </c>
     </row>
     <row r="26" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="B26">
+        <v>11</v>
+      </c>
+      <c r="C26" t="s">
         <v>58</v>
       </c>
-      <c r="B26">
-        <v>10</v>
-      </c>
-      <c r="C26" t="s">
+      <c r="D26" t="s">
         <v>59</v>
       </c>
-      <c r="D26" t="s">
+      <c r="E26" t="s">
         <v>60</v>
       </c>
-      <c r="E26" t="s">
+      <c r="F26" t="s">
         <v>61</v>
       </c>
-      <c r="F26" t="s">
-        <v>62</v>
-      </c>
       <c r="H26" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="I26" s="4">
         <v>2.9000000000000001E-2</v>
       </c>
       <c r="L26" s="5">
         <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
-        <v>0.29000000000000004</v>
+        <v>0.31900000000000001</v>
       </c>
     </row>
     <row r="27" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>168</v>
+        <v>192</v>
       </c>
       <c r="B27">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C27" s="7">
         <v>100</v>
       </c>
       <c r="D27" t="s">
+        <v>59</v>
+      </c>
+      <c r="E27" t="s">
         <v>60</v>
       </c>
-      <c r="E27" t="s">
+      <c r="F27" t="s">
         <v>61</v>
       </c>
-      <c r="F27" t="s">
-        <v>62</v>
-      </c>
       <c r="H27" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="I27" s="4">
         <v>0.107</v>
       </c>
       <c r="L27" s="5">
         <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
-        <v>1.177</v>
+        <v>1.284</v>
       </c>
     </row>
     <row r="28" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="B28">
         <v>21</v>
       </c>
       <c r="C28" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D28" t="s">
+        <v>59</v>
+      </c>
+      <c r="E28" t="s">
         <v>60</v>
       </c>
-      <c r="E28" t="s">
+      <c r="F28" t="s">
         <v>61</v>
       </c>
-      <c r="F28" t="s">
-        <v>62</v>
-      </c>
       <c r="H28" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="I28" s="4">
         <v>2.9000000000000001E-2</v>
@@ -2311,25 +2314,25 @@
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B29">
         <v>3</v>
       </c>
       <c r="C29" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D29" t="s">
+        <v>59</v>
+      </c>
+      <c r="E29" t="s">
         <v>60</v>
       </c>
-      <c r="E29" t="s">
+      <c r="F29" t="s">
         <v>61</v>
       </c>
-      <c r="F29" t="s">
-        <v>62</v>
-      </c>
       <c r="H29" s="3" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="I29" s="4">
         <v>0.15</v>
@@ -2341,25 +2344,25 @@
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B30">
         <v>3</v>
       </c>
       <c r="C30" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D30" t="s">
+        <v>59</v>
+      </c>
+      <c r="E30" t="s">
         <v>60</v>
       </c>
-      <c r="E30" t="s">
+      <c r="F30" t="s">
         <v>61</v>
       </c>
-      <c r="F30" t="s">
-        <v>62</v>
-      </c>
       <c r="H30" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="I30" s="4">
         <v>0.15</v>
@@ -2371,25 +2374,25 @@
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B31">
         <v>1</v>
       </c>
       <c r="C31" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D31" t="s">
+        <v>59</v>
+      </c>
+      <c r="E31" t="s">
         <v>60</v>
       </c>
-      <c r="E31" t="s">
+      <c r="F31" t="s">
         <v>61</v>
       </c>
-      <c r="F31" t="s">
-        <v>62</v>
-      </c>
       <c r="H31" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="I31" s="4">
         <v>0.15</v>
@@ -2401,22 +2404,22 @@
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B32">
         <v>1</v>
       </c>
       <c r="C32" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D32" t="s">
+        <v>59</v>
+      </c>
+      <c r="E32" t="s">
         <v>60</v>
       </c>
-      <c r="E32" t="s">
+      <c r="F32" t="s">
         <v>61</v>
-      </c>
-      <c r="F32" t="s">
-        <v>62</v>
       </c>
       <c r="I32" s="4"/>
       <c r="L32" s="5">
@@ -2424,27 +2427,27 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B33">
         <v>1</v>
       </c>
       <c r="C33" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D33" t="s">
+        <v>59</v>
+      </c>
+      <c r="E33" t="s">
         <v>60</v>
       </c>
-      <c r="E33" t="s">
+      <c r="F33" t="s">
         <v>61</v>
       </c>
-      <c r="F33" t="s">
-        <v>62</v>
-      </c>
       <c r="H33" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="I33" s="4">
         <v>0.15</v>
@@ -2454,27 +2457,27 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B34">
         <v>1</v>
       </c>
       <c r="C34" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D34" t="s">
+        <v>59</v>
+      </c>
+      <c r="E34" t="s">
         <v>60</v>
       </c>
-      <c r="E34" t="s">
+      <c r="F34" t="s">
         <v>61</v>
       </c>
-      <c r="F34" t="s">
-        <v>62</v>
-      </c>
       <c r="H34" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="I34" s="4">
         <v>0.15</v>
@@ -2484,27 +2487,27 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B35">
         <v>1</v>
       </c>
       <c r="C35" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D35" t="s">
+        <v>59</v>
+      </c>
+      <c r="E35" t="s">
         <v>60</v>
       </c>
-      <c r="E35" t="s">
+      <c r="F35" t="s">
         <v>61</v>
       </c>
-      <c r="F35" t="s">
-        <v>62</v>
-      </c>
       <c r="H35" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="I35" s="4">
         <v>0.15</v>
@@ -2514,27 +2517,27 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B36">
         <v>1</v>
       </c>
       <c r="C36" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D36" t="s">
+        <v>59</v>
+      </c>
+      <c r="E36" t="s">
         <v>60</v>
       </c>
-      <c r="E36" t="s">
+      <c r="F36" t="s">
         <v>61</v>
       </c>
-      <c r="F36" t="s">
-        <v>62</v>
-      </c>
       <c r="H36" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="I36" s="4">
         <v>0.15</v>
@@ -2544,15 +2547,15 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="37" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B37">
         <v>9</v>
       </c>
       <c r="C37" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D37" t="s">
         <v>47</v>
@@ -2561,13 +2564,13 @@
         <v>48</v>
       </c>
       <c r="F37" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="G37" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="H37" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I37" s="4">
         <v>0.57699999999999996</v>
@@ -2577,27 +2580,27 @@
         <v>5.1929999999999996</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B38">
         <v>3</v>
       </c>
       <c r="C38" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D38" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E38" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="G38" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="H38" t="s">
         <v>102</v>
-      </c>
-      <c r="H38" t="s">
-        <v>103</v>
       </c>
       <c r="I38" s="4">
         <v>1.96</v>
@@ -2607,30 +2610,30 @@
         <v>5.88</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B39">
         <v>1</v>
       </c>
       <c r="C39" t="s">
+        <v>82</v>
+      </c>
+      <c r="D39" t="s">
+        <v>82</v>
+      </c>
+      <c r="E39" t="s">
         <v>83</v>
       </c>
-      <c r="D39" t="s">
-        <v>83</v>
-      </c>
-      <c r="E39" t="s">
+      <c r="F39" t="s">
         <v>84</v>
       </c>
-      <c r="F39" t="s">
+      <c r="G39" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="G39" s="3" t="s">
-        <v>86</v>
-      </c>
       <c r="H39" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I39" s="4">
         <v>0.81</v>
@@ -2640,30 +2643,30 @@
         <v>0.81</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B40">
         <v>1</v>
       </c>
       <c r="C40" t="s">
+        <v>87</v>
+      </c>
+      <c r="D40" t="s">
+        <v>87</v>
+      </c>
+      <c r="E40" t="s">
         <v>88</v>
       </c>
-      <c r="D40" t="s">
-        <v>88</v>
-      </c>
-      <c r="E40" t="s">
-        <v>89</v>
-      </c>
       <c r="F40" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="G40" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="H40" s="3" t="s">
         <v>98</v>
-      </c>
-      <c r="H40" s="3" t="s">
-        <v>99</v>
       </c>
       <c r="I40" s="4">
         <v>9.61</v>
@@ -2673,30 +2676,30 @@
         <v>9.61</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B41">
         <v>4</v>
       </c>
       <c r="C41" t="s">
+        <v>143</v>
+      </c>
+      <c r="D41" t="s">
+        <v>157</v>
+      </c>
+      <c r="E41" t="s">
+        <v>144</v>
+      </c>
+      <c r="F41" t="s">
+        <v>147</v>
+      </c>
+      <c r="G41" t="s">
         <v>145</v>
       </c>
-      <c r="D41" t="s">
-        <v>159</v>
-      </c>
-      <c r="E41" t="s">
+      <c r="H41" s="3" t="s">
         <v>146</v>
-      </c>
-      <c r="F41" t="s">
-        <v>149</v>
-      </c>
-      <c r="G41" t="s">
-        <v>147</v>
-      </c>
-      <c r="H41" s="3" t="s">
-        <v>148</v>
       </c>
       <c r="I41" s="4">
         <v>1.71</v>
@@ -2706,17 +2709,45 @@
         <v>6.84</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="B42" t="s">
+        <v>185</v>
+      </c>
+      <c r="C42" t="s">
+        <v>185</v>
+      </c>
       <c r="D42" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="E42" t="s">
-        <v>189</v>
-      </c>
-      <c r="I42" s="4"/>
-      <c r="L42" s="5">
-        <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
-        <v>0</v>
+        <v>185</v>
+      </c>
+      <c r="F42" t="s">
+        <v>185</v>
+      </c>
+      <c r="G42" t="s">
+        <v>185</v>
+      </c>
+      <c r="H42" t="s">
+        <v>185</v>
+      </c>
+      <c r="I42" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="J42" t="s">
+        <v>185</v>
+      </c>
+      <c r="K42" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="L42" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="M42" t="s">
+        <v>185</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modified Inductor Footprint, fixed 3d Model orientation, generated gerbers and drill files. Still unsure about ESD Protection, but can simply remove components from board later.
</commit_message>
<xml_diff>
--- a/RADSAT-SK Timer/RADSAT-SK Timer.xlsx
+++ b/RADSAT-SK Timer/RADSAT-SK Timer.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\USST\power-and-electrical\RADSAT-SK Timer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC13FC79-4541-460B-BB97-034F9A7F0CD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EF66A48-DB20-4B03-A890-70269C741DCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-3000" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RADSAT-SK Timer" sheetId="1" r:id="rId1"/>
@@ -1521,10 +1521,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="8670" activePane="topRight"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <pane xSplit="8670" topLeftCell="H1" activePane="topRight"/>
       <selection activeCell="C45" sqref="C45"/>
-      <selection pane="topRight" activeCell="O26" sqref="O26"/>
+      <selection pane="topRight" activeCell="P14" sqref="P14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
added link for CSKB and created zip folder for gerbers
</commit_message>
<xml_diff>
--- a/RADSAT-SK Timer/RADSAT-SK Timer.xlsx
+++ b/RADSAT-SK Timer/RADSAT-SK Timer.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\USST\power-and-electrical\RADSAT-SK Timer\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chris\Dropbox\PC\Desktop\RADSAT-SK\power-and-electrical\RADSAT-SK Timer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EF66A48-DB20-4B03-A890-70269C741DCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7398E06-786D-40AA-8C9D-5E0E5848FFF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="5280" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RADSAT-SK Timer" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="197">
   <si>
     <t>Source:</t>
   </si>
@@ -616,6 +616,12 @@
   </si>
   <si>
     <t>no vertical through hole  :(</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/samtec-inc/ESQ-126-39-G-D/3601055</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/stackpole-electronics-inc/RMCF0402JT3M00/1712450</t>
   </si>
 </sst>
 </file>
@@ -623,7 +629,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="20" x14ac:knownFonts="1">
     <font>
@@ -1115,7 +1121,7 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="8">
@@ -1125,8 +1131,8 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="43"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="42" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="42" applyFont="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1180,7 +1186,7 @@
   </cellStyles>
   <dxfs count="2">
     <dxf>
-      <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1521,10 +1527,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
       <pane xSplit="8670" topLeftCell="H1" activePane="topRight"/>
-      <selection activeCell="C45" sqref="C45"/>
-      <selection pane="topRight" activeCell="P14" sqref="P14"/>
+      <selection activeCell="C30" sqref="C30"/>
+      <selection pane="topRight" activeCell="H41" sqref="H41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1691,7 +1697,7 @@
       <c r="F9" t="s">
         <v>150</v>
       </c>
-      <c r="H9" t="s">
+      <c r="H9" s="3" t="s">
         <v>149</v>
       </c>
       <c r="I9" s="4">
@@ -1721,7 +1727,7 @@
       <c r="F10" t="s">
         <v>22</v>
       </c>
-      <c r="H10" t="s">
+      <c r="H10" s="3" t="s">
         <v>180</v>
       </c>
       <c r="I10" s="4">
@@ -1754,7 +1760,7 @@
       <c r="G11" t="s">
         <v>128</v>
       </c>
-      <c r="H11" t="s">
+      <c r="H11" s="3" t="s">
         <v>129</v>
       </c>
       <c r="I11" s="4">
@@ -1784,7 +1790,7 @@
       <c r="F12" t="s">
         <v>22</v>
       </c>
-      <c r="H12" t="s">
+      <c r="H12" s="3" t="s">
         <v>182</v>
       </c>
       <c r="I12" s="4">
@@ -1817,7 +1823,7 @@
       <c r="G13" t="s">
         <v>125</v>
       </c>
-      <c r="H13" t="s">
+      <c r="H13" s="3" t="s">
         <v>126</v>
       </c>
       <c r="I13" s="4">
@@ -1913,7 +1919,7 @@
       <c r="G16" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="H16" t="s">
+      <c r="H16" s="3" t="s">
         <v>158</v>
       </c>
       <c r="I16" s="4">
@@ -1949,7 +1955,7 @@
       <c r="G17" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="H17" t="s">
+      <c r="H17" s="3" t="s">
         <v>111</v>
       </c>
       <c r="I17" s="4">
@@ -1982,7 +1988,7 @@
       <c r="G18" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="H18" t="s">
+      <c r="H18" s="3" t="s">
         <v>136</v>
       </c>
       <c r="I18" s="4">
@@ -2012,6 +2018,9 @@
       <c r="F19" t="s">
         <v>121</v>
       </c>
+      <c r="H19" s="3" t="s">
+        <v>195</v>
+      </c>
       <c r="I19" s="4"/>
       <c r="L19" s="5">
         <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
@@ -2241,7 +2250,7 @@
       <c r="F26" t="s">
         <v>61</v>
       </c>
-      <c r="H26" t="s">
+      <c r="H26" s="3" t="s">
         <v>171</v>
       </c>
       <c r="I26" s="4">
@@ -2271,7 +2280,7 @@
       <c r="F27" t="s">
         <v>61</v>
       </c>
-      <c r="H27" t="s">
+      <c r="H27" s="3" t="s">
         <v>148</v>
       </c>
       <c r="I27" s="4">
@@ -2301,7 +2310,7 @@
       <c r="F28" t="s">
         <v>61</v>
       </c>
-      <c r="H28" t="s">
+      <c r="H28" s="3" t="s">
         <v>172</v>
       </c>
       <c r="I28" s="4">
@@ -2361,7 +2370,7 @@
       <c r="F30" t="s">
         <v>61</v>
       </c>
-      <c r="H30" t="s">
+      <c r="H30" s="3" t="s">
         <v>174</v>
       </c>
       <c r="I30" s="4">
@@ -2391,7 +2400,7 @@
       <c r="F31" t="s">
         <v>61</v>
       </c>
-      <c r="H31" t="s">
+      <c r="H31" s="3" t="s">
         <v>175</v>
       </c>
       <c r="I31" s="4">
@@ -2421,6 +2430,9 @@
       <c r="F32" t="s">
         <v>61</v>
       </c>
+      <c r="H32" s="3" t="s">
+        <v>196</v>
+      </c>
       <c r="I32" s="4"/>
       <c r="L32" s="5">
         <f>Table1[[#This Row],[Qnty]]*(Table1[[#This Row],[Price]]+Table1[[#This Row],[Price2]])</f>
@@ -2446,7 +2458,7 @@
       <c r="F33" t="s">
         <v>61</v>
       </c>
-      <c r="H33" t="s">
+      <c r="H33" s="3" t="s">
         <v>176</v>
       </c>
       <c r="I33" s="4">
@@ -2476,7 +2488,7 @@
       <c r="F34" t="s">
         <v>61</v>
       </c>
-      <c r="H34" t="s">
+      <c r="H34" s="3" t="s">
         <v>177</v>
       </c>
       <c r="I34" s="4">
@@ -2506,7 +2518,7 @@
       <c r="F35" t="s">
         <v>61</v>
       </c>
-      <c r="H35" t="s">
+      <c r="H35" s="3" t="s">
         <v>178</v>
       </c>
       <c r="I35" s="4">
@@ -2536,7 +2548,7 @@
       <c r="F36" t="s">
         <v>61</v>
       </c>
-      <c r="H36" t="s">
+      <c r="H36" s="3" t="s">
         <v>179</v>
       </c>
       <c r="I36" s="4">
@@ -2569,7 +2581,7 @@
       <c r="G37" t="s">
         <v>122</v>
       </c>
-      <c r="H37" t="s">
+      <c r="H37" s="3" t="s">
         <v>107</v>
       </c>
       <c r="I37" s="4">
@@ -2599,7 +2611,7 @@
       <c r="G38" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="H38" t="s">
+      <c r="H38" s="3" t="s">
         <v>102</v>
       </c>
       <c r="I38" s="4">
@@ -2632,7 +2644,7 @@
       <c r="G39" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="H39" t="s">
+      <c r="H39" s="3" t="s">
         <v>96</v>
       </c>
       <c r="I39" s="4">
@@ -2776,11 +2788,34 @@
     <hyperlink ref="H22" r:id="rId21" xr:uid="{9F88BFCE-59FC-4E77-AC2A-F787549E61AD}"/>
     <hyperlink ref="G8" r:id="rId22" xr:uid="{7EF7B759-262D-46EA-A639-06793509DE1D}"/>
     <hyperlink ref="G24" r:id="rId23" xr:uid="{3168245F-C5D1-4FC5-9A41-850D03AE3A38}"/>
+    <hyperlink ref="H9" r:id="rId24" xr:uid="{D2F18E9A-4EEF-4DFB-9464-467E3CB87545}"/>
+    <hyperlink ref="H10" r:id="rId25" xr:uid="{6EA5851C-4DE0-4AE1-A93F-F4E1891A6E56}"/>
+    <hyperlink ref="H11" r:id="rId26" xr:uid="{A4A63C80-D81B-41A8-9D17-DA13860AFF0C}"/>
+    <hyperlink ref="H12" r:id="rId27" xr:uid="{FB0FE70B-C364-42F0-8334-909BE9F3530F}"/>
+    <hyperlink ref="H13" r:id="rId28" xr:uid="{D8045C79-7C94-4B9A-90C5-443A97D6307C}"/>
+    <hyperlink ref="H15" r:id="rId29" xr:uid="{25BC693A-4556-4C54-8097-4D4EFEDECC74}"/>
+    <hyperlink ref="H16" r:id="rId30" xr:uid="{63C6E5A8-312F-4989-BC3C-F2753D4D48C8}"/>
+    <hyperlink ref="H17" r:id="rId31" xr:uid="{917DFABC-0BF9-4FC1-989A-934C0798D878}"/>
+    <hyperlink ref="H18" r:id="rId32" xr:uid="{F51D08AD-41BF-47DB-9432-2F2763766474}"/>
+    <hyperlink ref="H19" r:id="rId33" xr:uid="{BFEED53D-A401-4A64-84DC-C09AB9B842FF}"/>
+    <hyperlink ref="H26" r:id="rId34" xr:uid="{C36989B8-8047-46E4-B870-2A6E2082FDA8}"/>
+    <hyperlink ref="H27" r:id="rId35" xr:uid="{044807EF-B53D-4CED-93D1-2FBE103B7C58}"/>
+    <hyperlink ref="H28" r:id="rId36" xr:uid="{D22B22B1-6A44-488D-89C1-D001EA25276F}"/>
+    <hyperlink ref="H30" r:id="rId37" xr:uid="{2F1579BD-1D8B-4C7A-8556-26CE21030C51}"/>
+    <hyperlink ref="H31" r:id="rId38" xr:uid="{DF8FD442-6FA3-475E-8930-519F6D005F5E}"/>
+    <hyperlink ref="H32" r:id="rId39" xr:uid="{D9323780-D784-4B4B-981C-035E032EF20F}"/>
+    <hyperlink ref="H33" r:id="rId40" xr:uid="{201456CA-D616-43EA-BEFF-7EEB89783A1A}"/>
+    <hyperlink ref="H34" r:id="rId41" xr:uid="{8B11D193-0761-48AF-881B-2B79A34A4EDB}"/>
+    <hyperlink ref="H35" r:id="rId42" xr:uid="{78EDA067-310F-488C-B69E-C9A92416FAF1}"/>
+    <hyperlink ref="H36" r:id="rId43" xr:uid="{B7C92DF1-AEBE-4DCF-A509-B8CC5DB3418F}"/>
+    <hyperlink ref="H37" r:id="rId44" xr:uid="{85C9D92F-E9D2-47A6-B9CD-593D3E36F6F5}"/>
+    <hyperlink ref="H38" r:id="rId45" xr:uid="{33B47597-B885-47A6-A7D1-DB4E5CF526D6}"/>
+    <hyperlink ref="H39" r:id="rId46" xr:uid="{BE4E7E51-528E-47D3-ACD5-6F5D5522A500}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId24"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId47"/>
   <tableParts count="1">
-    <tablePart r:id="rId25"/>
+    <tablePart r:id="rId48"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>